<commit_message>
Atualizado por script em 06-11-2023 14:45
</commit_message>
<xml_diff>
--- a/2023/greece_super-league-2_2023-2024.xlsx
+++ b/2023/greece_super-league-2_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V66"/>
+  <dimension ref="A1:V67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6277,71 +6277,71 @@
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>Ionikos</t>
+          <t>Kozani FC</t>
         </is>
       </c>
       <c r="G64" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Kalamata</t>
+          <t>AEL Larissa</t>
         </is>
       </c>
       <c r="I64" t="n">
         <v>2</v>
       </c>
       <c r="J64" t="n">
-        <v>2.56</v>
+        <v>3.62</v>
       </c>
       <c r="K64" t="inlineStr">
         <is>
-          <t>05/11/2023 03:13</t>
+          <t>04/11/2023 02:12</t>
         </is>
       </c>
       <c r="L64" t="n">
-        <v>2.88</v>
+        <v>4.52</v>
       </c>
       <c r="M64" t="inlineStr">
         <is>
-          <t>05/11/2023 13:59</t>
+          <t>05/11/2023 13:40</t>
         </is>
       </c>
       <c r="N64" t="n">
-        <v>3</v>
+        <v>2.95</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>05/11/2023 03:13</t>
+          <t>04/11/2023 02:12</t>
         </is>
       </c>
       <c r="P64" t="n">
-        <v>3.15</v>
+        <v>3.12</v>
       </c>
       <c r="Q64" t="inlineStr">
         <is>
-          <t>05/11/2023 13:59</t>
+          <t>05/11/2023 13:40</t>
         </is>
       </c>
       <c r="R64" t="n">
-        <v>2.82</v>
+        <v>2</v>
       </c>
       <c r="S64" t="inlineStr">
         <is>
-          <t>05/11/2023 03:13</t>
+          <t>04/11/2023 02:12</t>
         </is>
       </c>
       <c r="T64" t="n">
-        <v>2.46</v>
+        <v>1.88</v>
       </c>
       <c r="U64" t="inlineStr">
         <is>
-          <t>05/11/2023 13:59</t>
+          <t>05/11/2023 13:40</t>
         </is>
       </c>
       <c r="V64" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/ionikos-kalamata/2JXbBSs2/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/kozani-fc-ael-larissa/U5776LC6/</t>
         </is>
       </c>
     </row>
@@ -6369,71 +6369,71 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>Panathinaikos B</t>
+          <t>Ionikos</t>
         </is>
       </c>
       <c r="G65" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>PAE Egaleo</t>
+          <t>Kalamata</t>
         </is>
       </c>
       <c r="I65" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J65" t="n">
-        <v>2.48</v>
+        <v>2.56</v>
       </c>
       <c r="K65" t="inlineStr">
         <is>
-          <t>04/11/2023 02:12</t>
+          <t>05/11/2023 03:13</t>
         </is>
       </c>
       <c r="L65" t="n">
-        <v>2.59</v>
+        <v>2.88</v>
       </c>
       <c r="M65" t="inlineStr">
         <is>
-          <t>05/11/2023 13:55</t>
+          <t>05/11/2023 13:59</t>
         </is>
       </c>
       <c r="N65" t="n">
-        <v>2.88</v>
+        <v>3</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>04/11/2023 02:12</t>
+          <t>05/11/2023 03:13</t>
         </is>
       </c>
       <c r="P65" t="n">
-        <v>3.01</v>
+        <v>3.15</v>
       </c>
       <c r="Q65" t="inlineStr">
         <is>
-          <t>05/11/2023 13:55</t>
+          <t>05/11/2023 13:59</t>
         </is>
       </c>
       <c r="R65" t="n">
-        <v>2.75</v>
+        <v>2.82</v>
       </c>
       <c r="S65" t="inlineStr">
         <is>
-          <t>04/11/2023 02:12</t>
+          <t>05/11/2023 03:13</t>
         </is>
       </c>
       <c r="T65" t="n">
-        <v>2.83</v>
+        <v>2.46</v>
       </c>
       <c r="U65" t="inlineStr">
         <is>
-          <t>05/11/2023 03:41</t>
+          <t>05/11/2023 13:59</t>
         </is>
       </c>
       <c r="V65" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/panathinaikos-pae-egaleo/OSYfC8Se/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/ionikos-kalamata/2JXbBSs2/</t>
         </is>
       </c>
     </row>
@@ -6461,22 +6461,22 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>Kozani FC</t>
+          <t>Panathinaikos B</t>
         </is>
       </c>
       <c r="G66" t="n">
+        <v>1</v>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>PAE Egaleo</t>
+        </is>
+      </c>
+      <c r="I66" t="n">
         <v>0</v>
       </c>
-      <c r="H66" t="inlineStr">
-        <is>
-          <t>AEL Larissa</t>
-        </is>
-      </c>
-      <c r="I66" t="n">
-        <v>2</v>
-      </c>
       <c r="J66" t="n">
-        <v>3.62</v>
+        <v>2.48</v>
       </c>
       <c r="K66" t="inlineStr">
         <is>
@@ -6484,15 +6484,15 @@
         </is>
       </c>
       <c r="L66" t="n">
-        <v>4.52</v>
+        <v>2.59</v>
       </c>
       <c r="M66" t="inlineStr">
         <is>
-          <t>05/11/2023 13:40</t>
+          <t>05/11/2023 13:55</t>
         </is>
       </c>
       <c r="N66" t="n">
-        <v>2.95</v>
+        <v>2.88</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
@@ -6500,15 +6500,15 @@
         </is>
       </c>
       <c r="P66" t="n">
-        <v>3.12</v>
+        <v>3.01</v>
       </c>
       <c r="Q66" t="inlineStr">
         <is>
-          <t>05/11/2023 13:40</t>
+          <t>05/11/2023 13:55</t>
         </is>
       </c>
       <c r="R66" t="n">
-        <v>2</v>
+        <v>2.75</v>
       </c>
       <c r="S66" t="inlineStr">
         <is>
@@ -6516,16 +6516,108 @@
         </is>
       </c>
       <c r="T66" t="n">
-        <v>1.88</v>
+        <v>2.83</v>
       </c>
       <c r="U66" t="inlineStr">
         <is>
-          <t>05/11/2023 13:40</t>
+          <t>05/11/2023 03:41</t>
         </is>
       </c>
       <c r="V66" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/kozani-fc-ael-larissa/U5776LC6/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/panathinaikos-pae-egaleo/OSYfC8Se/</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>greece</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>super-league-2</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E67" s="2" t="n">
+        <v>45236.5625</v>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>Athens Kallithea</t>
+        </is>
+      </c>
+      <c r="G67" t="n">
+        <v>0</v>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>PAE Chania</t>
+        </is>
+      </c>
+      <c r="I67" t="n">
+        <v>1</v>
+      </c>
+      <c r="J67" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>05/11/2023 01:42</t>
+        </is>
+      </c>
+      <c r="L67" t="n">
+        <v>1.98</v>
+      </c>
+      <c r="M67" t="inlineStr">
+        <is>
+          <t>06/11/2023 12:24</t>
+        </is>
+      </c>
+      <c r="N67" t="n">
+        <v>3.51</v>
+      </c>
+      <c r="O67" t="inlineStr">
+        <is>
+          <t>05/11/2023 01:42</t>
+        </is>
+      </c>
+      <c r="P67" t="n">
+        <v>3.03</v>
+      </c>
+      <c r="Q67" t="inlineStr">
+        <is>
+          <t>06/11/2023 12:24</t>
+        </is>
+      </c>
+      <c r="R67" t="n">
+        <v>5.44</v>
+      </c>
+      <c r="S67" t="inlineStr">
+        <is>
+          <t>05/11/2023 01:42</t>
+        </is>
+      </c>
+      <c r="T67" t="n">
+        <v>4.22</v>
+      </c>
+      <c r="U67" t="inlineStr">
+        <is>
+          <t>06/11/2023 12:24</t>
+        </is>
+      </c>
+      <c r="V67" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/athens-kallithea-pae-chania/4OBszCK2/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 20-11-2023 14:45
</commit_message>
<xml_diff>
--- a/2023/greece_super-league-2_2023-2024.xlsx
+++ b/2023/greece_super-league-2_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V89"/>
+  <dimension ref="A1:V90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1585,71 +1585,71 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Panachaiki</t>
+          <t>PAOK B</t>
         </is>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Panathinaikos B</t>
+          <t>Kampaniakos</t>
         </is>
       </c>
       <c r="I13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J13" t="n">
-        <v>2.03</v>
+        <v>1.46</v>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>29/09/2023 02:12</t>
+          <t>30/09/2023 03:12</t>
         </is>
       </c>
       <c r="L13" t="n">
-        <v>2.78</v>
+        <v>1.52</v>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>30/09/2023 14:56</t>
+          <t>30/09/2023 13:01</t>
         </is>
       </c>
       <c r="N13" t="n">
-        <v>3.16</v>
+        <v>4.27</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>29/09/2023 02:12</t>
+          <t>30/09/2023 03:12</t>
         </is>
       </c>
       <c r="P13" t="n">
-        <v>2.92</v>
+        <v>4.05</v>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>30/09/2023 13:25</t>
+          <t>30/09/2023 13:17</t>
         </is>
       </c>
       <c r="R13" t="n">
-        <v>3.27</v>
+        <v>5.93</v>
       </c>
       <c r="S13" t="inlineStr">
         <is>
-          <t>29/09/2023 02:12</t>
+          <t>30/09/2023 03:12</t>
         </is>
       </c>
       <c r="T13" t="n">
-        <v>2.72</v>
+        <v>6.09</v>
       </c>
       <c r="U13" t="inlineStr">
         <is>
-          <t>30/09/2023 14:56</t>
+          <t>30/09/2023 13:17</t>
         </is>
       </c>
       <c r="V13" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/panachaiki-panathinaikos/xh8LWHQB/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/paok-kampaniakos/S6W0xkkj/</t>
         </is>
       </c>
     </row>
@@ -1677,71 +1677,71 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>PAOK B</t>
+          <t>Panachaiki</t>
         </is>
       </c>
       <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Panathinaikos B</t>
+        </is>
+      </c>
+      <c r="I14" t="n">
         <v>2</v>
       </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>Kampaniakos</t>
-        </is>
-      </c>
-      <c r="I14" t="n">
-        <v>3</v>
-      </c>
       <c r="J14" t="n">
-        <v>1.46</v>
+        <v>2.03</v>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>30/09/2023 03:12</t>
+          <t>29/09/2023 02:12</t>
         </is>
       </c>
       <c r="L14" t="n">
-        <v>1.52</v>
+        <v>2.78</v>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>30/09/2023 13:01</t>
+          <t>30/09/2023 14:56</t>
         </is>
       </c>
       <c r="N14" t="n">
-        <v>4.27</v>
+        <v>3.16</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>30/09/2023 03:12</t>
+          <t>29/09/2023 02:12</t>
         </is>
       </c>
       <c r="P14" t="n">
-        <v>4.05</v>
+        <v>2.92</v>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>30/09/2023 13:17</t>
+          <t>30/09/2023 13:25</t>
         </is>
       </c>
       <c r="R14" t="n">
-        <v>5.93</v>
+        <v>3.27</v>
       </c>
       <c r="S14" t="inlineStr">
         <is>
-          <t>30/09/2023 03:12</t>
+          <t>29/09/2023 02:12</t>
         </is>
       </c>
       <c r="T14" t="n">
-        <v>6.09</v>
+        <v>2.72</v>
       </c>
       <c r="U14" t="inlineStr">
         <is>
-          <t>30/09/2023 13:17</t>
+          <t>30/09/2023 14:56</t>
         </is>
       </c>
       <c r="V14" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/paok-kampaniakos/S6W0xkkj/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/panachaiki-panathinaikos/xh8LWHQB/</t>
         </is>
       </c>
     </row>
@@ -2505,71 +2505,71 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Kozani FC</t>
+          <t>AEL Larissa</t>
         </is>
       </c>
       <c r="G23" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Makedonikos</t>
+          <t>Iraklis 1908</t>
         </is>
       </c>
       <c r="I23" t="n">
         <v>0</v>
       </c>
       <c r="J23" t="n">
-        <v>2.36</v>
+        <v>1.95</v>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>10/10/2023 11:12</t>
+          <t>10/10/2023 02:12</t>
         </is>
       </c>
       <c r="L23" t="n">
-        <v>2.63</v>
+        <v>1.96</v>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>11/10/2023 14:58</t>
+          <t>11/10/2023 14:52</t>
         </is>
       </c>
       <c r="N23" t="n">
-        <v>2.79</v>
+        <v>3.06</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>10/10/2023 11:12</t>
+          <t>10/10/2023 02:12</t>
         </is>
       </c>
       <c r="P23" t="n">
-        <v>2.86</v>
+        <v>3.04</v>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>11/10/2023 14:58</t>
+          <t>11/10/2023 14:52</t>
         </is>
       </c>
       <c r="R23" t="n">
-        <v>3.1</v>
+        <v>3.62</v>
       </c>
       <c r="S23" t="inlineStr">
         <is>
-          <t>10/10/2023 11:12</t>
+          <t>10/10/2023 02:12</t>
         </is>
       </c>
       <c r="T23" t="n">
-        <v>2.93</v>
+        <v>4.31</v>
       </c>
       <c r="U23" t="inlineStr">
         <is>
-          <t>11/10/2023 14:16</t>
+          <t>11/10/2023 14:52</t>
         </is>
       </c>
       <c r="V23" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/kozani-fc-makedonikos-neapolis/t4a21ZU9/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/ael-larissa-iraklis-fc/WhhFbXES/</t>
         </is>
       </c>
     </row>
@@ -2597,71 +2597,71 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>AEL Larissa</t>
+          <t>Karditsa</t>
         </is>
       </c>
       <c r="G24" t="n">
+        <v>3</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Aiolikos</t>
+        </is>
+      </c>
+      <c r="I24" t="n">
         <v>1</v>
       </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>Iraklis 1908</t>
-        </is>
-      </c>
-      <c r="I24" t="n">
-        <v>0</v>
-      </c>
       <c r="J24" t="n">
-        <v>1.95</v>
+        <v>1.96</v>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>10/10/2023 02:12</t>
+          <t>10/10/2023 11:12</t>
         </is>
       </c>
       <c r="L24" t="n">
-        <v>1.96</v>
+        <v>1.86</v>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>11/10/2023 14:52</t>
+          <t>11/10/2023 14:54</t>
         </is>
       </c>
       <c r="N24" t="n">
-        <v>3.06</v>
+        <v>2.97</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>10/10/2023 02:12</t>
+          <t>10/10/2023 11:12</t>
         </is>
       </c>
       <c r="P24" t="n">
-        <v>3.04</v>
+        <v>3.27</v>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>11/10/2023 14:52</t>
+          <t>11/10/2023 14:54</t>
         </is>
       </c>
       <c r="R24" t="n">
-        <v>3.62</v>
+        <v>3.86</v>
       </c>
       <c r="S24" t="inlineStr">
         <is>
-          <t>10/10/2023 02:12</t>
+          <t>10/10/2023 11:12</t>
         </is>
       </c>
       <c r="T24" t="n">
-        <v>4.31</v>
+        <v>4.4</v>
       </c>
       <c r="U24" t="inlineStr">
         <is>
-          <t>11/10/2023 14:52</t>
+          <t>11/10/2023 14:54</t>
         </is>
       </c>
       <c r="V24" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/ael-larissa-iraklis-fc/WhhFbXES/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/karditsa-aiolikos-fc/2JmBaDaM/</t>
         </is>
       </c>
     </row>
@@ -2689,22 +2689,22 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Karditsa</t>
+          <t>Kozani FC</t>
         </is>
       </c>
       <c r="G25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Aiolikos</t>
+          <t>Makedonikos</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25" t="n">
-        <v>1.96</v>
+        <v>2.36</v>
       </c>
       <c r="K25" t="inlineStr">
         <is>
@@ -2712,15 +2712,15 @@
         </is>
       </c>
       <c r="L25" t="n">
-        <v>1.86</v>
+        <v>2.63</v>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>11/10/2023 14:54</t>
+          <t>11/10/2023 14:58</t>
         </is>
       </c>
       <c r="N25" t="n">
-        <v>2.97</v>
+        <v>2.79</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
@@ -2728,15 +2728,15 @@
         </is>
       </c>
       <c r="P25" t="n">
-        <v>3.27</v>
+        <v>2.86</v>
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>11/10/2023 14:54</t>
+          <t>11/10/2023 14:58</t>
         </is>
       </c>
       <c r="R25" t="n">
-        <v>3.86</v>
+        <v>3.1</v>
       </c>
       <c r="S25" t="inlineStr">
         <is>
@@ -2744,16 +2744,16 @@
         </is>
       </c>
       <c r="T25" t="n">
-        <v>4.4</v>
+        <v>2.93</v>
       </c>
       <c r="U25" t="inlineStr">
         <is>
-          <t>11/10/2023 14:54</t>
+          <t>11/10/2023 14:16</t>
         </is>
       </c>
       <c r="V25" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/karditsa-aiolikos-fc/2JmBaDaM/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/kozani-fc-makedonikos-neapolis/t4a21ZU9/</t>
         </is>
       </c>
     </row>
@@ -3977,7 +3977,7 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Apollon Pontou</t>
+          <t>Kozani FC</t>
         </is>
       </c>
       <c r="G39" t="n">
@@ -3985,63 +3985,63 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Niki Volos</t>
+          <t>Karditsa</t>
         </is>
       </c>
       <c r="I39" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J39" t="n">
-        <v>4.17</v>
+        <v>2.75</v>
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>21/10/2023 02:13</t>
+          <t>22/10/2023 12:12</t>
         </is>
       </c>
       <c r="L39" t="n">
-        <v>9.99</v>
+        <v>2.58</v>
       </c>
       <c r="M39" t="inlineStr">
         <is>
-          <t>22/10/2023 14:56</t>
+          <t>22/10/2023 14:49</t>
         </is>
       </c>
       <c r="N39" t="n">
-        <v>3.18</v>
+        <v>2.74</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>21/10/2023 02:13</t>
+          <t>22/10/2023 12:12</t>
         </is>
       </c>
       <c r="P39" t="n">
-        <v>4.44</v>
+        <v>2.74</v>
       </c>
       <c r="Q39" t="inlineStr">
         <is>
-          <t>22/10/2023 14:56</t>
+          <t>22/10/2023 13:54</t>
         </is>
       </c>
       <c r="R39" t="n">
-        <v>1.78</v>
+        <v>2.92</v>
       </c>
       <c r="S39" t="inlineStr">
         <is>
-          <t>21/10/2023 02:13</t>
+          <t>22/10/2023 12:12</t>
         </is>
       </c>
       <c r="T39" t="n">
-        <v>1.34</v>
+        <v>3.14</v>
       </c>
       <c r="U39" t="inlineStr">
         <is>
-          <t>22/10/2023 14:56</t>
+          <t>22/10/2023 14:49</t>
         </is>
       </c>
       <c r="V39" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/apollon-pontou-niki-volos/UTgL7Aiq/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/kozani-fc-karditsa/OnHhCjqS/</t>
         </is>
       </c>
     </row>
@@ -4161,7 +4161,7 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Kozani FC</t>
+          <t>Apollon Pontou</t>
         </is>
       </c>
       <c r="G41" t="n">
@@ -4169,63 +4169,63 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Karditsa</t>
+          <t>Niki Volos</t>
         </is>
       </c>
       <c r="I41" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J41" t="n">
-        <v>2.75</v>
+        <v>4.17</v>
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>22/10/2023 12:12</t>
+          <t>21/10/2023 02:13</t>
         </is>
       </c>
       <c r="L41" t="n">
-        <v>2.58</v>
+        <v>9.99</v>
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>22/10/2023 14:49</t>
+          <t>22/10/2023 14:56</t>
         </is>
       </c>
       <c r="N41" t="n">
-        <v>2.74</v>
+        <v>3.18</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>22/10/2023 12:12</t>
+          <t>21/10/2023 02:13</t>
         </is>
       </c>
       <c r="P41" t="n">
-        <v>2.74</v>
+        <v>4.44</v>
       </c>
       <c r="Q41" t="inlineStr">
         <is>
-          <t>22/10/2023 13:54</t>
+          <t>22/10/2023 14:56</t>
         </is>
       </c>
       <c r="R41" t="n">
-        <v>2.92</v>
+        <v>1.78</v>
       </c>
       <c r="S41" t="inlineStr">
         <is>
-          <t>22/10/2023 12:12</t>
+          <t>21/10/2023 02:13</t>
         </is>
       </c>
       <c r="T41" t="n">
-        <v>3.14</v>
+        <v>1.34</v>
       </c>
       <c r="U41" t="inlineStr">
         <is>
-          <t>22/10/2023 14:49</t>
+          <t>22/10/2023 14:56</t>
         </is>
       </c>
       <c r="V41" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/kozani-fc-karditsa/OnHhCjqS/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/apollon-pontou-niki-volos/UTgL7Aiq/</t>
         </is>
       </c>
     </row>
@@ -4621,71 +4621,71 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Levadiakos</t>
+          <t>PAE Chania</t>
         </is>
       </c>
       <c r="G46" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>AEK Athens FC B</t>
+          <t>Panachaiki</t>
         </is>
       </c>
       <c r="I46" t="n">
         <v>1</v>
       </c>
       <c r="J46" t="n">
-        <v>1.3</v>
+        <v>1.42</v>
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>28/10/2023 01:12</t>
+          <t>27/10/2023 02:13</t>
         </is>
       </c>
       <c r="L46" t="n">
-        <v>1.36</v>
+        <v>1.22</v>
       </c>
       <c r="M46" t="inlineStr">
         <is>
-          <t>28/10/2023 13:55</t>
+          <t>28/10/2023 13:34</t>
         </is>
       </c>
       <c r="N46" t="n">
-        <v>4.78</v>
+        <v>4.07</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>28/10/2023 01:12</t>
+          <t>27/10/2023 02:13</t>
         </is>
       </c>
       <c r="P46" t="n">
-        <v>4.28</v>
+        <v>5.62</v>
       </c>
       <c r="Q46" t="inlineStr">
         <is>
-          <t>28/10/2023 13:55</t>
+          <t>28/10/2023 13:58</t>
         </is>
       </c>
       <c r="R46" t="n">
-        <v>9.51</v>
+        <v>6.07</v>
       </c>
       <c r="S46" t="inlineStr">
         <is>
-          <t>28/10/2023 01:12</t>
+          <t>27/10/2023 02:13</t>
         </is>
       </c>
       <c r="T46" t="n">
-        <v>9.83</v>
+        <v>14.35</v>
       </c>
       <c r="U46" t="inlineStr">
         <is>
-          <t>28/10/2023 13:55</t>
+          <t>28/10/2023 13:58</t>
         </is>
       </c>
       <c r="V46" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/levadiakos-aek/xbk08srf/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/pae-chania-panachaiki/xYNDv6Ok/</t>
         </is>
       </c>
     </row>
@@ -4713,7 +4713,7 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Giouchtas</t>
+          <t>Levadiakos</t>
         </is>
       </c>
       <c r="G47" t="n">
@@ -4721,14 +4721,14 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Panathinaikos B</t>
+          <t>AEK Athens FC B</t>
         </is>
       </c>
       <c r="I47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J47" t="n">
-        <v>1.83</v>
+        <v>1.3</v>
       </c>
       <c r="K47" t="inlineStr">
         <is>
@@ -4736,7 +4736,7 @@
         </is>
       </c>
       <c r="L47" t="n">
-        <v>1.91</v>
+        <v>1.36</v>
       </c>
       <c r="M47" t="inlineStr">
         <is>
@@ -4744,7 +4744,7 @@
         </is>
       </c>
       <c r="N47" t="n">
-        <v>3.35</v>
+        <v>4.78</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
@@ -4752,7 +4752,7 @@
         </is>
       </c>
       <c r="P47" t="n">
-        <v>3.24</v>
+        <v>4.28</v>
       </c>
       <c r="Q47" t="inlineStr">
         <is>
@@ -4760,7 +4760,7 @@
         </is>
       </c>
       <c r="R47" t="n">
-        <v>4.09</v>
+        <v>9.51</v>
       </c>
       <c r="S47" t="inlineStr">
         <is>
@@ -4768,7 +4768,7 @@
         </is>
       </c>
       <c r="T47" t="n">
-        <v>4.19</v>
+        <v>9.83</v>
       </c>
       <c r="U47" t="inlineStr">
         <is>
@@ -4777,7 +4777,7 @@
       </c>
       <c r="V47" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/giouchtas-panathinaikos/AJ7XbzA4/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/levadiakos-aek/xbk08srf/</t>
         </is>
       </c>
     </row>
@@ -4805,7 +4805,7 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Kalamata</t>
+          <t>Giouchtas</t>
         </is>
       </c>
       <c r="G48" t="n">
@@ -4813,63 +4813,63 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Ilioupoli</t>
+          <t>Panathinaikos B</t>
         </is>
       </c>
       <c r="I48" t="n">
         <v>0</v>
       </c>
       <c r="J48" t="n">
-        <v>1.44</v>
+        <v>1.83</v>
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>27/10/2023 02:13</t>
+          <t>28/10/2023 01:12</t>
         </is>
       </c>
       <c r="L48" t="n">
-        <v>1.38</v>
+        <v>1.91</v>
       </c>
       <c r="M48" t="inlineStr">
         <is>
-          <t>28/10/2023 13:43</t>
+          <t>28/10/2023 13:55</t>
         </is>
       </c>
       <c r="N48" t="n">
-        <v>3.96</v>
+        <v>3.35</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>27/10/2023 02:13</t>
+          <t>28/10/2023 01:12</t>
         </is>
       </c>
       <c r="P48" t="n">
-        <v>4.35</v>
+        <v>3.24</v>
       </c>
       <c r="Q48" t="inlineStr">
         <is>
-          <t>28/10/2023 13:43</t>
+          <t>28/10/2023 13:55</t>
         </is>
       </c>
       <c r="R48" t="n">
-        <v>5.97</v>
+        <v>4.09</v>
       </c>
       <c r="S48" t="inlineStr">
         <is>
-          <t>27/10/2023 02:13</t>
+          <t>28/10/2023 01:12</t>
         </is>
       </c>
       <c r="T48" t="n">
-        <v>8.56</v>
+        <v>4.19</v>
       </c>
       <c r="U48" t="inlineStr">
         <is>
-          <t>28/10/2023 13:43</t>
+          <t>28/10/2023 13:55</t>
         </is>
       </c>
       <c r="V48" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/kalamata-ilioupoli/bsP9un9q/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/giouchtas-panathinaikos/AJ7XbzA4/</t>
         </is>
       </c>
     </row>
@@ -4897,22 +4897,22 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>PAE Chania</t>
+          <t>Kalamata</t>
         </is>
       </c>
       <c r="G49" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Panachaiki</t>
+          <t>Ilioupoli</t>
         </is>
       </c>
       <c r="I49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J49" t="n">
-        <v>1.42</v>
+        <v>1.44</v>
       </c>
       <c r="K49" t="inlineStr">
         <is>
@@ -4920,15 +4920,15 @@
         </is>
       </c>
       <c r="L49" t="n">
-        <v>1.22</v>
+        <v>1.38</v>
       </c>
       <c r="M49" t="inlineStr">
         <is>
-          <t>28/10/2023 13:34</t>
+          <t>28/10/2023 13:43</t>
         </is>
       </c>
       <c r="N49" t="n">
-        <v>4.07</v>
+        <v>3.96</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
@@ -4936,15 +4936,15 @@
         </is>
       </c>
       <c r="P49" t="n">
-        <v>5.62</v>
+        <v>4.35</v>
       </c>
       <c r="Q49" t="inlineStr">
         <is>
-          <t>28/10/2023 13:58</t>
+          <t>28/10/2023 13:43</t>
         </is>
       </c>
       <c r="R49" t="n">
-        <v>6.07</v>
+        <v>5.97</v>
       </c>
       <c r="S49" t="inlineStr">
         <is>
@@ -4952,16 +4952,16 @@
         </is>
       </c>
       <c r="T49" t="n">
-        <v>14.35</v>
+        <v>8.56</v>
       </c>
       <c r="U49" t="inlineStr">
         <is>
-          <t>28/10/2023 13:58</t>
+          <t>28/10/2023 13:43</t>
         </is>
       </c>
       <c r="V49" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/pae-chania-panachaiki/xYNDv6Ok/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/kalamata-ilioupoli/bsP9un9q/</t>
         </is>
       </c>
     </row>
@@ -6093,22 +6093,22 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>Ionikos</t>
+          <t>Kampaniakos</t>
         </is>
       </c>
       <c r="G62" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Kalamata</t>
+          <t>Apollon Pontou</t>
         </is>
       </c>
       <c r="I62" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J62" t="n">
-        <v>2.56</v>
+        <v>2.17</v>
       </c>
       <c r="K62" t="inlineStr">
         <is>
@@ -6116,15 +6116,15 @@
         </is>
       </c>
       <c r="L62" t="n">
-        <v>2.88</v>
+        <v>1.97</v>
       </c>
       <c r="M62" t="inlineStr">
         <is>
-          <t>05/11/2023 13:59</t>
+          <t>05/11/2023 12:16</t>
         </is>
       </c>
       <c r="N62" t="n">
-        <v>3</v>
+        <v>2.99</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
@@ -6132,15 +6132,15 @@
         </is>
       </c>
       <c r="P62" t="n">
-        <v>3.15</v>
+        <v>3.11</v>
       </c>
       <c r="Q62" t="inlineStr">
         <is>
-          <t>05/11/2023 13:59</t>
+          <t>05/11/2023 12:16</t>
         </is>
       </c>
       <c r="R62" t="n">
-        <v>2.82</v>
+        <v>3.42</v>
       </c>
       <c r="S62" t="inlineStr">
         <is>
@@ -6148,16 +6148,16 @@
         </is>
       </c>
       <c r="T62" t="n">
-        <v>2.46</v>
+        <v>4.12</v>
       </c>
       <c r="U62" t="inlineStr">
         <is>
-          <t>05/11/2023 13:59</t>
+          <t>05/11/2023 12:16</t>
         </is>
       </c>
       <c r="V62" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/ionikos-kalamata/2JXbBSs2/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/kampaniakos-apollon-pontou/CUdC5uSC/</t>
         </is>
       </c>
     </row>
@@ -6185,22 +6185,22 @@
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>Panathinaikos B</t>
+          <t>AEK Athens FC B</t>
         </is>
       </c>
       <c r="G63" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>PAE Egaleo</t>
+          <t>Niki Volos</t>
         </is>
       </c>
       <c r="I63" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J63" t="n">
-        <v>2.48</v>
+        <v>4.16</v>
       </c>
       <c r="K63" t="inlineStr">
         <is>
@@ -6208,15 +6208,15 @@
         </is>
       </c>
       <c r="L63" t="n">
-        <v>2.59</v>
+        <v>4.09</v>
       </c>
       <c r="M63" t="inlineStr">
         <is>
-          <t>05/11/2023 13:55</t>
+          <t>05/11/2023 13:57</t>
         </is>
       </c>
       <c r="N63" t="n">
-        <v>2.88</v>
+        <v>3.15</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
@@ -6228,11 +6228,11 @@
       </c>
       <c r="Q63" t="inlineStr">
         <is>
-          <t>05/11/2023 13:55</t>
+          <t>05/11/2023 13:57</t>
         </is>
       </c>
       <c r="R63" t="n">
-        <v>2.75</v>
+        <v>1.79</v>
       </c>
       <c r="S63" t="inlineStr">
         <is>
@@ -6240,16 +6240,16 @@
         </is>
       </c>
       <c r="T63" t="n">
-        <v>2.83</v>
+        <v>2.02</v>
       </c>
       <c r="U63" t="inlineStr">
         <is>
-          <t>05/11/2023 03:41</t>
+          <t>05/11/2023 13:57</t>
         </is>
       </c>
       <c r="V63" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/panathinaikos-pae-egaleo/OSYfC8Se/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/aek-niki-volos/vykbTrKJ/</t>
         </is>
       </c>
     </row>
@@ -6277,7 +6277,7 @@
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>AEK Athens FC B</t>
+          <t>Kozani FC</t>
         </is>
       </c>
       <c r="G64" t="n">
@@ -6285,14 +6285,14 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Niki Volos</t>
+          <t>AEL Larissa</t>
         </is>
       </c>
       <c r="I64" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J64" t="n">
-        <v>4.16</v>
+        <v>3.62</v>
       </c>
       <c r="K64" t="inlineStr">
         <is>
@@ -6300,15 +6300,15 @@
         </is>
       </c>
       <c r="L64" t="n">
-        <v>4.09</v>
+        <v>4.52</v>
       </c>
       <c r="M64" t="inlineStr">
         <is>
-          <t>05/11/2023 13:57</t>
+          <t>05/11/2023 13:40</t>
         </is>
       </c>
       <c r="N64" t="n">
-        <v>3.15</v>
+        <v>2.95</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
@@ -6316,15 +6316,15 @@
         </is>
       </c>
       <c r="P64" t="n">
-        <v>3.01</v>
+        <v>3.12</v>
       </c>
       <c r="Q64" t="inlineStr">
         <is>
-          <t>05/11/2023 13:57</t>
+          <t>05/11/2023 13:40</t>
         </is>
       </c>
       <c r="R64" t="n">
-        <v>1.79</v>
+        <v>2</v>
       </c>
       <c r="S64" t="inlineStr">
         <is>
@@ -6332,16 +6332,16 @@
         </is>
       </c>
       <c r="T64" t="n">
-        <v>2.02</v>
+        <v>1.88</v>
       </c>
       <c r="U64" t="inlineStr">
         <is>
-          <t>05/11/2023 13:57</t>
+          <t>05/11/2023 13:40</t>
         </is>
       </c>
       <c r="V64" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/aek-niki-volos/vykbTrKJ/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/kozani-fc-ael-larissa/U5776LC6/</t>
         </is>
       </c>
     </row>
@@ -6369,22 +6369,22 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>Kampaniakos</t>
+          <t>Ionikos</t>
         </is>
       </c>
       <c r="G65" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Apollon Pontou</t>
+          <t>Kalamata</t>
         </is>
       </c>
       <c r="I65" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J65" t="n">
-        <v>2.17</v>
+        <v>2.56</v>
       </c>
       <c r="K65" t="inlineStr">
         <is>
@@ -6392,15 +6392,15 @@
         </is>
       </c>
       <c r="L65" t="n">
-        <v>1.97</v>
+        <v>2.88</v>
       </c>
       <c r="M65" t="inlineStr">
         <is>
-          <t>05/11/2023 12:16</t>
+          <t>05/11/2023 13:59</t>
         </is>
       </c>
       <c r="N65" t="n">
-        <v>2.99</v>
+        <v>3</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
@@ -6408,15 +6408,15 @@
         </is>
       </c>
       <c r="P65" t="n">
-        <v>3.11</v>
+        <v>3.15</v>
       </c>
       <c r="Q65" t="inlineStr">
         <is>
-          <t>05/11/2023 12:16</t>
+          <t>05/11/2023 13:59</t>
         </is>
       </c>
       <c r="R65" t="n">
-        <v>3.42</v>
+        <v>2.82</v>
       </c>
       <c r="S65" t="inlineStr">
         <is>
@@ -6424,16 +6424,16 @@
         </is>
       </c>
       <c r="T65" t="n">
-        <v>4.12</v>
+        <v>2.46</v>
       </c>
       <c r="U65" t="inlineStr">
         <is>
-          <t>05/11/2023 12:16</t>
+          <t>05/11/2023 13:59</t>
         </is>
       </c>
       <c r="V65" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/kampaniakos-apollon-pontou/CUdC5uSC/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/ionikos-kalamata/2JXbBSs2/</t>
         </is>
       </c>
     </row>
@@ -6461,22 +6461,22 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>Kozani FC</t>
+          <t>Panathinaikos B</t>
         </is>
       </c>
       <c r="G66" t="n">
+        <v>1</v>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>PAE Egaleo</t>
+        </is>
+      </c>
+      <c r="I66" t="n">
         <v>0</v>
       </c>
-      <c r="H66" t="inlineStr">
-        <is>
-          <t>AEL Larissa</t>
-        </is>
-      </c>
-      <c r="I66" t="n">
-        <v>2</v>
-      </c>
       <c r="J66" t="n">
-        <v>3.62</v>
+        <v>2.48</v>
       </c>
       <c r="K66" t="inlineStr">
         <is>
@@ -6484,15 +6484,15 @@
         </is>
       </c>
       <c r="L66" t="n">
-        <v>4.52</v>
+        <v>2.59</v>
       </c>
       <c r="M66" t="inlineStr">
         <is>
-          <t>05/11/2023 13:40</t>
+          <t>05/11/2023 13:55</t>
         </is>
       </c>
       <c r="N66" t="n">
-        <v>2.95</v>
+        <v>2.88</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
@@ -6500,15 +6500,15 @@
         </is>
       </c>
       <c r="P66" t="n">
-        <v>3.12</v>
+        <v>3.01</v>
       </c>
       <c r="Q66" t="inlineStr">
         <is>
-          <t>05/11/2023 13:40</t>
+          <t>05/11/2023 13:55</t>
         </is>
       </c>
       <c r="R66" t="n">
-        <v>2</v>
+        <v>2.75</v>
       </c>
       <c r="S66" t="inlineStr">
         <is>
@@ -6516,16 +6516,16 @@
         </is>
       </c>
       <c r="T66" t="n">
-        <v>1.88</v>
+        <v>2.83</v>
       </c>
       <c r="U66" t="inlineStr">
         <is>
-          <t>05/11/2023 13:40</t>
+          <t>05/11/2023 03:41</t>
         </is>
       </c>
       <c r="V66" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/kozani-fc-ael-larissa/U5776LC6/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/panathinaikos-pae-egaleo/OSYfC8Se/</t>
         </is>
       </c>
     </row>
@@ -7289,22 +7289,22 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>Panachaiki</t>
+          <t>Niki Volos</t>
         </is>
       </c>
       <c r="G75" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Ionikos</t>
+          <t>Iraklis 1908</t>
         </is>
       </c>
       <c r="I75" t="n">
         <v>1</v>
       </c>
       <c r="J75" t="n">
-        <v>4.2</v>
+        <v>1.87</v>
       </c>
       <c r="K75" t="inlineStr">
         <is>
@@ -7312,15 +7312,15 @@
         </is>
       </c>
       <c r="L75" t="n">
-        <v>6.83</v>
+        <v>2.02</v>
       </c>
       <c r="M75" t="inlineStr">
         <is>
-          <t>12/11/2023 13:58</t>
+          <t>12/11/2023 12:05</t>
         </is>
       </c>
       <c r="N75" t="n">
-        <v>3.26</v>
+        <v>3.03</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
@@ -7328,15 +7328,15 @@
         </is>
       </c>
       <c r="P75" t="n">
-        <v>3.77</v>
+        <v>3</v>
       </c>
       <c r="Q75" t="inlineStr">
         <is>
-          <t>12/11/2023 13:58</t>
+          <t>12/11/2023 12:12</t>
         </is>
       </c>
       <c r="R75" t="n">
-        <v>1.75</v>
+        <v>3.98</v>
       </c>
       <c r="S75" t="inlineStr">
         <is>
@@ -7344,16 +7344,16 @@
         </is>
       </c>
       <c r="T75" t="n">
-        <v>1.52</v>
+        <v>4.13</v>
       </c>
       <c r="U75" t="inlineStr">
         <is>
-          <t>12/11/2023 13:58</t>
+          <t>12/11/2023 12:05</t>
         </is>
       </c>
       <c r="V75" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/panachaiki-ionikos/2JgUQ7sk/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/niki-volos-iraklis-fc/jypvKvs6/</t>
         </is>
       </c>
     </row>
@@ -7381,22 +7381,22 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>Niki Volos</t>
+          <t>Ilioupoli</t>
         </is>
       </c>
       <c r="G76" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Iraklis 1908</t>
+          <t>Athens Kallithea</t>
         </is>
       </c>
       <c r="I76" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J76" t="n">
-        <v>1.87</v>
+        <v>4.68</v>
       </c>
       <c r="K76" t="inlineStr">
         <is>
@@ -7404,15 +7404,15 @@
         </is>
       </c>
       <c r="L76" t="n">
-        <v>2.02</v>
+        <v>4.56</v>
       </c>
       <c r="M76" t="inlineStr">
         <is>
-          <t>12/11/2023 12:05</t>
+          <t>12/11/2023 13:55</t>
         </is>
       </c>
       <c r="N76" t="n">
-        <v>3.03</v>
+        <v>3.36</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
@@ -7420,15 +7420,15 @@
         </is>
       </c>
       <c r="P76" t="n">
-        <v>3</v>
+        <v>3.13</v>
       </c>
       <c r="Q76" t="inlineStr">
         <is>
-          <t>12/11/2023 12:12</t>
+          <t>12/11/2023 13:55</t>
         </is>
       </c>
       <c r="R76" t="n">
-        <v>3.98</v>
+        <v>1.65</v>
       </c>
       <c r="S76" t="inlineStr">
         <is>
@@ -7436,16 +7436,16 @@
         </is>
       </c>
       <c r="T76" t="n">
-        <v>4.13</v>
+        <v>1.88</v>
       </c>
       <c r="U76" t="inlineStr">
         <is>
-          <t>12/11/2023 12:05</t>
+          <t>12/11/2023 13:55</t>
         </is>
       </c>
       <c r="V76" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/niki-volos-iraklis-fc/jypvKvs6/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/ilioupoli-athens-kallithea/GMcYPRde/</t>
         </is>
       </c>
     </row>
@@ -7473,22 +7473,22 @@
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>Ilioupoli</t>
+          <t>PAE Chania</t>
         </is>
       </c>
       <c r="G77" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Athens Kallithea</t>
+          <t>Panathinaikos B</t>
         </is>
       </c>
       <c r="I77" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J77" t="n">
-        <v>4.68</v>
+        <v>1.37</v>
       </c>
       <c r="K77" t="inlineStr">
         <is>
@@ -7496,15 +7496,15 @@
         </is>
       </c>
       <c r="L77" t="n">
-        <v>4.56</v>
+        <v>1.32</v>
       </c>
       <c r="M77" t="inlineStr">
         <is>
-          <t>12/11/2023 13:55</t>
+          <t>12/11/2023 12:05</t>
         </is>
       </c>
       <c r="N77" t="n">
-        <v>3.36</v>
+        <v>4.28</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
@@ -7512,15 +7512,15 @@
         </is>
       </c>
       <c r="P77" t="n">
-        <v>3.13</v>
+        <v>4.79</v>
       </c>
       <c r="Q77" t="inlineStr">
         <is>
-          <t>12/11/2023 13:55</t>
+          <t>12/11/2023 12:07</t>
         </is>
       </c>
       <c r="R77" t="n">
-        <v>1.65</v>
+        <v>6.55</v>
       </c>
       <c r="S77" t="inlineStr">
         <is>
@@ -7528,16 +7528,16 @@
         </is>
       </c>
       <c r="T77" t="n">
-        <v>1.88</v>
+        <v>9.890000000000001</v>
       </c>
       <c r="U77" t="inlineStr">
         <is>
-          <t>12/11/2023 13:55</t>
+          <t>12/11/2023 12:07</t>
         </is>
       </c>
       <c r="V77" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/ilioupoli-athens-kallithea/GMcYPRde/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/pae-chania-panathinaikos/8dfQRmSr/</t>
         </is>
       </c>
     </row>
@@ -7565,22 +7565,22 @@
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>PAE Chania</t>
+          <t>Panachaiki</t>
         </is>
       </c>
       <c r="G78" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Panathinaikos B</t>
+          <t>Ionikos</t>
         </is>
       </c>
       <c r="I78" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J78" t="n">
-        <v>1.37</v>
+        <v>4.2</v>
       </c>
       <c r="K78" t="inlineStr">
         <is>
@@ -7588,15 +7588,15 @@
         </is>
       </c>
       <c r="L78" t="n">
-        <v>1.32</v>
+        <v>6.83</v>
       </c>
       <c r="M78" t="inlineStr">
         <is>
-          <t>12/11/2023 12:05</t>
+          <t>12/11/2023 13:58</t>
         </is>
       </c>
       <c r="N78" t="n">
-        <v>4.28</v>
+        <v>3.26</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
@@ -7604,15 +7604,15 @@
         </is>
       </c>
       <c r="P78" t="n">
-        <v>4.79</v>
+        <v>3.77</v>
       </c>
       <c r="Q78" t="inlineStr">
         <is>
-          <t>12/11/2023 12:07</t>
+          <t>12/11/2023 13:58</t>
         </is>
       </c>
       <c r="R78" t="n">
-        <v>6.55</v>
+        <v>1.75</v>
       </c>
       <c r="S78" t="inlineStr">
         <is>
@@ -7620,16 +7620,16 @@
         </is>
       </c>
       <c r="T78" t="n">
-        <v>9.890000000000001</v>
+        <v>1.52</v>
       </c>
       <c r="U78" t="inlineStr">
         <is>
-          <t>12/11/2023 12:07</t>
+          <t>12/11/2023 13:58</t>
         </is>
       </c>
       <c r="V78" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/pae-chania-panathinaikos/8dfQRmSr/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/panachaiki-ionikos/2JgUQ7sk/</t>
         </is>
       </c>
     </row>
@@ -8025,22 +8025,22 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>Kampaniakos</t>
+          <t>Karditsa</t>
         </is>
       </c>
       <c r="G83" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Iraklis 1908</t>
+          <t>Levadiakos</t>
         </is>
       </c>
       <c r="I83" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J83" t="n">
-        <v>3.87</v>
+        <v>4.29</v>
       </c>
       <c r="K83" t="inlineStr">
         <is>
@@ -8048,15 +8048,15 @@
         </is>
       </c>
       <c r="L83" t="n">
-        <v>4.12</v>
+        <v>5.74</v>
       </c>
       <c r="M83" t="inlineStr">
         <is>
-          <t>19/11/2023 12:04</t>
+          <t>19/11/2023 13:50</t>
         </is>
       </c>
       <c r="N83" t="n">
-        <v>3.15</v>
+        <v>3.08</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
@@ -8064,15 +8064,15 @@
         </is>
       </c>
       <c r="P83" t="n">
-        <v>3.11</v>
+        <v>3.31</v>
       </c>
       <c r="Q83" t="inlineStr">
         <is>
-          <t>19/11/2023 12:52</t>
+          <t>19/11/2023 13:50</t>
         </is>
       </c>
       <c r="R83" t="n">
-        <v>1.85</v>
+        <v>1.79</v>
       </c>
       <c r="S83" t="inlineStr">
         <is>
@@ -8080,16 +8080,16 @@
         </is>
       </c>
       <c r="T83" t="n">
-        <v>1.97</v>
+        <v>1.68</v>
       </c>
       <c r="U83" t="inlineStr">
         <is>
-          <t>19/11/2023 12:52</t>
+          <t>19/11/2023 13:50</t>
         </is>
       </c>
       <c r="V83" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/kampaniakos-iraklis-fc/6R0RGyBJ/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/karditsa-levadiakos/2cncBFYt/</t>
         </is>
       </c>
     </row>
@@ -8577,71 +8577,163 @@
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>Karditsa</t>
+          <t>Kampaniakos</t>
         </is>
       </c>
       <c r="G89" t="n">
+        <v>1</v>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>Iraklis 1908</t>
+        </is>
+      </c>
+      <c r="I89" t="n">
+        <v>3</v>
+      </c>
+      <c r="J89" t="n">
+        <v>3.87</v>
+      </c>
+      <c r="K89" t="inlineStr">
+        <is>
+          <t>18/11/2023 02:12</t>
+        </is>
+      </c>
+      <c r="L89" t="n">
+        <v>4.12</v>
+      </c>
+      <c r="M89" t="inlineStr">
+        <is>
+          <t>19/11/2023 12:04</t>
+        </is>
+      </c>
+      <c r="N89" t="n">
+        <v>3.15</v>
+      </c>
+      <c r="O89" t="inlineStr">
+        <is>
+          <t>18/11/2023 02:12</t>
+        </is>
+      </c>
+      <c r="P89" t="n">
+        <v>3.11</v>
+      </c>
+      <c r="Q89" t="inlineStr">
+        <is>
+          <t>19/11/2023 12:52</t>
+        </is>
+      </c>
+      <c r="R89" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="S89" t="inlineStr">
+        <is>
+          <t>18/11/2023 02:12</t>
+        </is>
+      </c>
+      <c r="T89" t="n">
+        <v>1.97</v>
+      </c>
+      <c r="U89" t="inlineStr">
+        <is>
+          <t>19/11/2023 12:52</t>
+        </is>
+      </c>
+      <c r="V89" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/kampaniakos-iraklis-fc/6R0RGyBJ/</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>greece</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>super-league-2</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E90" s="2" t="n">
+        <v>45250.58333333334</v>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>Niki Volos</t>
+        </is>
+      </c>
+      <c r="G90" t="n">
+        <v>1</v>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>Makedonikos</t>
+        </is>
+      </c>
+      <c r="I90" t="n">
         <v>2</v>
       </c>
-      <c r="H89" t="inlineStr">
-        <is>
-          <t>Levadiakos</t>
-        </is>
-      </c>
-      <c r="I89" t="n">
-        <v>0</v>
-      </c>
-      <c r="J89" t="n">
-        <v>4.29</v>
-      </c>
-      <c r="K89" t="inlineStr">
-        <is>
-          <t>18/11/2023 02:12</t>
-        </is>
-      </c>
-      <c r="L89" t="n">
-        <v>5.74</v>
-      </c>
-      <c r="M89" t="inlineStr">
-        <is>
-          <t>19/11/2023 13:50</t>
-        </is>
-      </c>
-      <c r="N89" t="n">
-        <v>3.08</v>
-      </c>
-      <c r="O89" t="inlineStr">
-        <is>
-          <t>18/11/2023 02:12</t>
-        </is>
-      </c>
-      <c r="P89" t="n">
-        <v>3.31</v>
-      </c>
-      <c r="Q89" t="inlineStr">
-        <is>
-          <t>19/11/2023 13:50</t>
-        </is>
-      </c>
-      <c r="R89" t="n">
-        <v>1.79</v>
-      </c>
-      <c r="S89" t="inlineStr">
-        <is>
-          <t>18/11/2023 02:12</t>
-        </is>
-      </c>
-      <c r="T89" t="n">
-        <v>1.68</v>
-      </c>
-      <c r="U89" t="inlineStr">
-        <is>
-          <t>19/11/2023 13:50</t>
-        </is>
-      </c>
-      <c r="V89" t="inlineStr">
-        <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/karditsa-levadiakos/2cncBFYt/</t>
+      <c r="J90" t="n">
+        <v>1.57</v>
+      </c>
+      <c r="K90" t="inlineStr">
+        <is>
+          <t>19/11/2023 02:12</t>
+        </is>
+      </c>
+      <c r="L90" t="n">
+        <v>1.53</v>
+      </c>
+      <c r="M90" t="inlineStr">
+        <is>
+          <t>20/11/2023 13:53</t>
+        </is>
+      </c>
+      <c r="N90" t="n">
+        <v>3.39</v>
+      </c>
+      <c r="O90" t="inlineStr">
+        <is>
+          <t>19/11/2023 02:12</t>
+        </is>
+      </c>
+      <c r="P90" t="n">
+        <v>3.68</v>
+      </c>
+      <c r="Q90" t="inlineStr">
+        <is>
+          <t>20/11/2023 13:58</t>
+        </is>
+      </c>
+      <c r="R90" t="n">
+        <v>5.47</v>
+      </c>
+      <c r="S90" t="inlineStr">
+        <is>
+          <t>19/11/2023 02:12</t>
+        </is>
+      </c>
+      <c r="T90" t="n">
+        <v>6.91</v>
+      </c>
+      <c r="U90" t="inlineStr">
+        <is>
+          <t>20/11/2023 13:58</t>
+        </is>
+      </c>
+      <c r="V90" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/niki-volos-makedonikos-neapolis/EXk1AZmm/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 03-01-2024 14:45
</commit_message>
<xml_diff>
--- a/2023/greece_super-league-2_2023-2024.xlsx
+++ b/2023/greece_super-league-2_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V138"/>
+  <dimension ref="A1:V141"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3517,22 +3517,22 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Ionikos</t>
+          <t>PAOK B</t>
         </is>
       </c>
       <c r="G34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Tilikratis L.</t>
+          <t>Aiolikos</t>
         </is>
       </c>
       <c r="I34" t="n">
         <v>0</v>
       </c>
       <c r="J34" t="n">
-        <v>1.3</v>
+        <v>1.57</v>
       </c>
       <c r="K34" t="inlineStr">
         <is>
@@ -3540,15 +3540,15 @@
         </is>
       </c>
       <c r="L34" t="n">
-        <v>1.22</v>
+        <v>1.75</v>
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>21/10/2023 12:52</t>
+          <t>21/10/2023 14:43</t>
         </is>
       </c>
       <c r="N34" t="n">
-        <v>4.55</v>
+        <v>3.91</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
@@ -3556,15 +3556,15 @@
         </is>
       </c>
       <c r="P34" t="n">
-        <v>5.42</v>
+        <v>3.66</v>
       </c>
       <c r="Q34" t="inlineStr">
         <is>
-          <t>21/10/2023 13:02</t>
+          <t>21/10/2023 14:43</t>
         </is>
       </c>
       <c r="R34" t="n">
-        <v>10.53</v>
+        <v>5.06</v>
       </c>
       <c r="S34" t="inlineStr">
         <is>
@@ -3572,16 +3572,16 @@
         </is>
       </c>
       <c r="T34" t="n">
-        <v>14.23</v>
+        <v>4.44</v>
       </c>
       <c r="U34" t="inlineStr">
         <is>
-          <t>21/10/2023 12:52</t>
+          <t>21/10/2023 14:43</t>
         </is>
       </c>
       <c r="V34" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/ionikos-tilikratis-lefkada/hry7rFPN/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/paok-aiolikos-fc/fyiX48y2/</t>
         </is>
       </c>
     </row>
@@ -3609,22 +3609,22 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>PAOK B</t>
+          <t>Ionikos</t>
         </is>
       </c>
       <c r="G35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Aiolikos</t>
+          <t>Tilikratis L.</t>
         </is>
       </c>
       <c r="I35" t="n">
         <v>0</v>
       </c>
       <c r="J35" t="n">
-        <v>1.57</v>
+        <v>1.3</v>
       </c>
       <c r="K35" t="inlineStr">
         <is>
@@ -3632,15 +3632,15 @@
         </is>
       </c>
       <c r="L35" t="n">
-        <v>1.75</v>
+        <v>1.22</v>
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>21/10/2023 14:43</t>
+          <t>21/10/2023 12:52</t>
         </is>
       </c>
       <c r="N35" t="n">
-        <v>3.91</v>
+        <v>4.55</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
@@ -3648,15 +3648,15 @@
         </is>
       </c>
       <c r="P35" t="n">
-        <v>3.66</v>
+        <v>5.42</v>
       </c>
       <c r="Q35" t="inlineStr">
         <is>
-          <t>21/10/2023 14:43</t>
+          <t>21/10/2023 13:02</t>
         </is>
       </c>
       <c r="R35" t="n">
-        <v>5.06</v>
+        <v>10.53</v>
       </c>
       <c r="S35" t="inlineStr">
         <is>
@@ -3664,16 +3664,16 @@
         </is>
       </c>
       <c r="T35" t="n">
-        <v>4.44</v>
+        <v>14.23</v>
       </c>
       <c r="U35" t="inlineStr">
         <is>
-          <t>21/10/2023 14:43</t>
+          <t>21/10/2023 12:52</t>
         </is>
       </c>
       <c r="V35" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/paok-aiolikos-fc/fyiX48y2/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/ionikos-tilikratis-lefkada/hry7rFPN/</t>
         </is>
       </c>
     </row>
@@ -4621,7 +4621,7 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Giouchtas</t>
+          <t>Levadiakos</t>
         </is>
       </c>
       <c r="G46" t="n">
@@ -4629,14 +4629,14 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Panathinaikos B</t>
+          <t>AEK Athens FC B</t>
         </is>
       </c>
       <c r="I46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J46" t="n">
-        <v>1.83</v>
+        <v>1.3</v>
       </c>
       <c r="K46" t="inlineStr">
         <is>
@@ -4644,7 +4644,7 @@
         </is>
       </c>
       <c r="L46" t="n">
-        <v>1.91</v>
+        <v>1.36</v>
       </c>
       <c r="M46" t="inlineStr">
         <is>
@@ -4652,7 +4652,7 @@
         </is>
       </c>
       <c r="N46" t="n">
-        <v>3.35</v>
+        <v>4.78</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
@@ -4660,7 +4660,7 @@
         </is>
       </c>
       <c r="P46" t="n">
-        <v>3.24</v>
+        <v>4.28</v>
       </c>
       <c r="Q46" t="inlineStr">
         <is>
@@ -4668,7 +4668,7 @@
         </is>
       </c>
       <c r="R46" t="n">
-        <v>4.09</v>
+        <v>9.51</v>
       </c>
       <c r="S46" t="inlineStr">
         <is>
@@ -4676,7 +4676,7 @@
         </is>
       </c>
       <c r="T46" t="n">
-        <v>4.19</v>
+        <v>9.83</v>
       </c>
       <c r="U46" t="inlineStr">
         <is>
@@ -4685,7 +4685,7 @@
       </c>
       <c r="V46" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/giouchtas-panathinaikos/AJ7XbzA4/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/levadiakos-aek/xbk08srf/</t>
         </is>
       </c>
     </row>
@@ -4713,71 +4713,71 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Levadiakos</t>
+          <t>PAE Egaleo</t>
         </is>
       </c>
       <c r="G47" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>AEK Athens FC B</t>
+          <t>Athens Kallithea</t>
         </is>
       </c>
       <c r="I47" t="n">
         <v>1</v>
       </c>
       <c r="J47" t="n">
-        <v>1.3</v>
+        <v>4.46</v>
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>28/10/2023 01:12</t>
+          <t>27/10/2023 02:13</t>
         </is>
       </c>
       <c r="L47" t="n">
-        <v>1.36</v>
+        <v>7.03</v>
       </c>
       <c r="M47" t="inlineStr">
         <is>
-          <t>28/10/2023 13:55</t>
+          <t>28/10/2023 12:23</t>
         </is>
       </c>
       <c r="N47" t="n">
-        <v>4.78</v>
+        <v>3.12</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>28/10/2023 01:12</t>
+          <t>27/10/2023 02:13</t>
         </is>
       </c>
       <c r="P47" t="n">
-        <v>4.28</v>
+        <v>3.72</v>
       </c>
       <c r="Q47" t="inlineStr">
         <is>
-          <t>28/10/2023 13:55</t>
+          <t>28/10/2023 12:23</t>
         </is>
       </c>
       <c r="R47" t="n">
-        <v>9.51</v>
+        <v>1.75</v>
       </c>
       <c r="S47" t="inlineStr">
         <is>
-          <t>28/10/2023 01:12</t>
+          <t>27/10/2023 02:13</t>
         </is>
       </c>
       <c r="T47" t="n">
-        <v>9.83</v>
+        <v>1.52</v>
       </c>
       <c r="U47" t="inlineStr">
         <is>
-          <t>28/10/2023 13:55</t>
+          <t>28/10/2023 12:23</t>
         </is>
       </c>
       <c r="V47" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/levadiakos-aek/xbk08srf/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/pae-egaleo-athens-kallithea/WYetcEvH/</t>
         </is>
       </c>
     </row>
@@ -4805,22 +4805,22 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>PAE Egaleo</t>
+          <t>PAE Chania</t>
         </is>
       </c>
       <c r="G48" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Athens Kallithea</t>
+          <t>Panachaiki</t>
         </is>
       </c>
       <c r="I48" t="n">
         <v>1</v>
       </c>
       <c r="J48" t="n">
-        <v>4.46</v>
+        <v>1.42</v>
       </c>
       <c r="K48" t="inlineStr">
         <is>
@@ -4828,15 +4828,15 @@
         </is>
       </c>
       <c r="L48" t="n">
-        <v>7.03</v>
+        <v>1.22</v>
       </c>
       <c r="M48" t="inlineStr">
         <is>
-          <t>28/10/2023 12:23</t>
+          <t>28/10/2023 13:34</t>
         </is>
       </c>
       <c r="N48" t="n">
-        <v>3.12</v>
+        <v>4.07</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
@@ -4844,15 +4844,15 @@
         </is>
       </c>
       <c r="P48" t="n">
-        <v>3.72</v>
+        <v>5.62</v>
       </c>
       <c r="Q48" t="inlineStr">
         <is>
-          <t>28/10/2023 12:23</t>
+          <t>28/10/2023 13:58</t>
         </is>
       </c>
       <c r="R48" t="n">
-        <v>1.75</v>
+        <v>6.07</v>
       </c>
       <c r="S48" t="inlineStr">
         <is>
@@ -4860,16 +4860,16 @@
         </is>
       </c>
       <c r="T48" t="n">
-        <v>1.52</v>
+        <v>14.35</v>
       </c>
       <c r="U48" t="inlineStr">
         <is>
-          <t>28/10/2023 12:23</t>
+          <t>28/10/2023 13:58</t>
         </is>
       </c>
       <c r="V48" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/pae-egaleo-athens-kallithea/WYetcEvH/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/pae-chania-panachaiki/xYNDv6Ok/</t>
         </is>
       </c>
     </row>
@@ -4897,71 +4897,71 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>PAE Chania</t>
+          <t>Giouchtas</t>
         </is>
       </c>
       <c r="G49" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Panachaiki</t>
+          <t>Panathinaikos B</t>
         </is>
       </c>
       <c r="I49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J49" t="n">
-        <v>1.42</v>
+        <v>1.83</v>
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>27/10/2023 02:13</t>
+          <t>28/10/2023 01:12</t>
         </is>
       </c>
       <c r="L49" t="n">
-        <v>1.22</v>
+        <v>1.91</v>
       </c>
       <c r="M49" t="inlineStr">
         <is>
-          <t>28/10/2023 13:34</t>
+          <t>28/10/2023 13:55</t>
         </is>
       </c>
       <c r="N49" t="n">
-        <v>4.07</v>
+        <v>3.35</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>27/10/2023 02:13</t>
+          <t>28/10/2023 01:12</t>
         </is>
       </c>
       <c r="P49" t="n">
-        <v>5.62</v>
+        <v>3.24</v>
       </c>
       <c r="Q49" t="inlineStr">
         <is>
-          <t>28/10/2023 13:58</t>
+          <t>28/10/2023 13:55</t>
         </is>
       </c>
       <c r="R49" t="n">
-        <v>6.07</v>
+        <v>4.09</v>
       </c>
       <c r="S49" t="inlineStr">
         <is>
-          <t>27/10/2023 02:13</t>
+          <t>28/10/2023 01:12</t>
         </is>
       </c>
       <c r="T49" t="n">
-        <v>14.35</v>
+        <v>4.19</v>
       </c>
       <c r="U49" t="inlineStr">
         <is>
-          <t>28/10/2023 13:58</t>
+          <t>28/10/2023 13:55</t>
         </is>
       </c>
       <c r="V49" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/pae-chania-panachaiki/xYNDv6Ok/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/giouchtas-panathinaikos/AJ7XbzA4/</t>
         </is>
       </c>
     </row>
@@ -5173,22 +5173,22 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Makedonikos</t>
+          <t>Karditsa</t>
         </is>
       </c>
       <c r="G52" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>PAOK B</t>
+          <t>AEL Larissa</t>
         </is>
       </c>
       <c r="I52" t="n">
         <v>2</v>
       </c>
       <c r="J52" t="n">
-        <v>1.95</v>
+        <v>3.52</v>
       </c>
       <c r="K52" t="inlineStr">
         <is>
@@ -5196,15 +5196,15 @@
         </is>
       </c>
       <c r="L52" t="n">
-        <v>1.94</v>
+        <v>3.94</v>
       </c>
       <c r="M52" t="inlineStr">
         <is>
-          <t>29/10/2023 13:59</t>
+          <t>29/10/2023 13:57</t>
         </is>
       </c>
       <c r="N52" t="n">
-        <v>3.06</v>
+        <v>2.91</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
@@ -5212,15 +5212,15 @@
         </is>
       </c>
       <c r="P52" t="n">
-        <v>3.16</v>
+        <v>3.08</v>
       </c>
       <c r="Q52" t="inlineStr">
         <is>
-          <t>29/10/2023 13:59</t>
+          <t>29/10/2023 13:57</t>
         </is>
       </c>
       <c r="R52" t="n">
-        <v>3.62</v>
+        <v>2.05</v>
       </c>
       <c r="S52" t="inlineStr">
         <is>
@@ -5228,16 +5228,16 @@
         </is>
       </c>
       <c r="T52" t="n">
-        <v>4.14</v>
+        <v>2.03</v>
       </c>
       <c r="U52" t="inlineStr">
         <is>
-          <t>29/10/2023 13:59</t>
+          <t>29/10/2023 13:57</t>
         </is>
       </c>
       <c r="V52" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/makedonikos-neapolis-paok/b7jd9NSm/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/karditsa-ael-larissa/46YNRVrF/</t>
         </is>
       </c>
     </row>
@@ -5265,22 +5265,22 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Karditsa</t>
+          <t>Makedonikos</t>
         </is>
       </c>
       <c r="G53" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>AEL Larissa</t>
+          <t>PAOK B</t>
         </is>
       </c>
       <c r="I53" t="n">
         <v>2</v>
       </c>
       <c r="J53" t="n">
-        <v>3.52</v>
+        <v>1.95</v>
       </c>
       <c r="K53" t="inlineStr">
         <is>
@@ -5288,15 +5288,15 @@
         </is>
       </c>
       <c r="L53" t="n">
-        <v>3.94</v>
+        <v>1.94</v>
       </c>
       <c r="M53" t="inlineStr">
         <is>
-          <t>29/10/2023 13:57</t>
+          <t>29/10/2023 13:59</t>
         </is>
       </c>
       <c r="N53" t="n">
-        <v>2.91</v>
+        <v>3.06</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
@@ -5304,15 +5304,15 @@
         </is>
       </c>
       <c r="P53" t="n">
-        <v>3.08</v>
+        <v>3.16</v>
       </c>
       <c r="Q53" t="inlineStr">
         <is>
-          <t>29/10/2023 13:57</t>
+          <t>29/10/2023 13:59</t>
         </is>
       </c>
       <c r="R53" t="n">
-        <v>2.05</v>
+        <v>3.62</v>
       </c>
       <c r="S53" t="inlineStr">
         <is>
@@ -5320,16 +5320,16 @@
         </is>
       </c>
       <c r="T53" t="n">
-        <v>2.03</v>
+        <v>4.14</v>
       </c>
       <c r="U53" t="inlineStr">
         <is>
-          <t>29/10/2023 13:57</t>
+          <t>29/10/2023 13:59</t>
         </is>
       </c>
       <c r="V53" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/karditsa-ael-larissa/46YNRVrF/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/makedonikos-neapolis-paok/b7jd9NSm/</t>
         </is>
       </c>
     </row>
@@ -5725,71 +5725,71 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>Ilioupoli</t>
+          <t>Iraklis 1908</t>
         </is>
       </c>
       <c r="G58" t="n">
+        <v>0</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>Levadiakos</t>
+        </is>
+      </c>
+      <c r="I58" t="n">
         <v>1</v>
       </c>
-      <c r="H58" t="inlineStr">
-        <is>
-          <t>Panachaiki</t>
-        </is>
-      </c>
-      <c r="I58" t="n">
-        <v>0</v>
-      </c>
       <c r="J58" t="n">
-        <v>1.66</v>
+        <v>3.01</v>
       </c>
       <c r="K58" t="inlineStr">
         <is>
-          <t>03/11/2023 02:13</t>
+          <t>04/11/2023 05:12</t>
         </is>
       </c>
       <c r="L58" t="n">
-        <v>1.38</v>
+        <v>3.53</v>
       </c>
       <c r="M58" t="inlineStr">
         <is>
-          <t>04/11/2023 13:44</t>
+          <t>04/11/2023 13:55</t>
         </is>
       </c>
       <c r="N58" t="n">
-        <v>3.48</v>
+        <v>2.91</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>03/11/2023 02:13</t>
+          <t>04/11/2023 05:12</t>
         </is>
       </c>
       <c r="P58" t="n">
-        <v>4.36</v>
+        <v>3</v>
       </c>
       <c r="Q58" t="inlineStr">
         <is>
-          <t>04/11/2023 13:48</t>
+          <t>04/11/2023 13:55</t>
         </is>
       </c>
       <c r="R58" t="n">
-        <v>4.41</v>
+        <v>2.42</v>
       </c>
       <c r="S58" t="inlineStr">
         <is>
-          <t>03/11/2023 02:13</t>
+          <t>04/11/2023 05:12</t>
         </is>
       </c>
       <c r="T58" t="n">
-        <v>8.41</v>
+        <v>2.2</v>
       </c>
       <c r="U58" t="inlineStr">
         <is>
-          <t>04/11/2023 13:44</t>
+          <t>04/11/2023 13:55</t>
         </is>
       </c>
       <c r="V58" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/ilioupoli-panachaiki/GbFoZVZ8/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/iraklis-fc-levadiakos/IRm2S2ZP/</t>
         </is>
       </c>
     </row>
@@ -5817,71 +5817,71 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>Iraklis 1908</t>
+          <t>PAOK B</t>
         </is>
       </c>
       <c r="G59" t="n">
+        <v>2</v>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>Karditsa</t>
+        </is>
+      </c>
+      <c r="I59" t="n">
         <v>0</v>
       </c>
-      <c r="H59" t="inlineStr">
-        <is>
-          <t>Levadiakos</t>
-        </is>
-      </c>
-      <c r="I59" t="n">
-        <v>1</v>
-      </c>
       <c r="J59" t="n">
-        <v>3.01</v>
+        <v>1.99</v>
       </c>
       <c r="K59" t="inlineStr">
         <is>
-          <t>04/11/2023 05:12</t>
+          <t>03/11/2023 02:13</t>
         </is>
       </c>
       <c r="L59" t="n">
-        <v>3.53</v>
+        <v>2.38</v>
       </c>
       <c r="M59" t="inlineStr">
         <is>
-          <t>04/11/2023 13:55</t>
+          <t>04/11/2023 12:04</t>
         </is>
       </c>
       <c r="N59" t="n">
-        <v>2.91</v>
+        <v>3.12</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>04/11/2023 05:12</t>
+          <t>03/11/2023 02:13</t>
         </is>
       </c>
       <c r="P59" t="n">
-        <v>3</v>
+        <v>2.89</v>
       </c>
       <c r="Q59" t="inlineStr">
         <is>
-          <t>04/11/2023 13:55</t>
+          <t>04/11/2023 12:04</t>
         </is>
       </c>
       <c r="R59" t="n">
-        <v>2.42</v>
+        <v>3.44</v>
       </c>
       <c r="S59" t="inlineStr">
         <is>
-          <t>04/11/2023 05:12</t>
+          <t>03/11/2023 02:13</t>
         </is>
       </c>
       <c r="T59" t="n">
-        <v>2.2</v>
+        <v>3.27</v>
       </c>
       <c r="U59" t="inlineStr">
         <is>
-          <t>04/11/2023 13:55</t>
+          <t>04/11/2023 12:04</t>
         </is>
       </c>
       <c r="V59" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/iraklis-fc-levadiakos/IRm2S2ZP/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/paok-karditsa/jLeG4asJ/</t>
         </is>
       </c>
     </row>
@@ -5909,22 +5909,22 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>PAOK B</t>
+          <t>Ilioupoli</t>
         </is>
       </c>
       <c r="G60" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Karditsa</t>
+          <t>Panachaiki</t>
         </is>
       </c>
       <c r="I60" t="n">
         <v>0</v>
       </c>
       <c r="J60" t="n">
-        <v>1.99</v>
+        <v>1.66</v>
       </c>
       <c r="K60" t="inlineStr">
         <is>
@@ -5932,15 +5932,15 @@
         </is>
       </c>
       <c r="L60" t="n">
-        <v>2.38</v>
+        <v>1.38</v>
       </c>
       <c r="M60" t="inlineStr">
         <is>
-          <t>04/11/2023 12:04</t>
+          <t>04/11/2023 13:44</t>
         </is>
       </c>
       <c r="N60" t="n">
-        <v>3.12</v>
+        <v>3.48</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
@@ -5948,15 +5948,15 @@
         </is>
       </c>
       <c r="P60" t="n">
-        <v>2.89</v>
+        <v>4.36</v>
       </c>
       <c r="Q60" t="inlineStr">
         <is>
-          <t>04/11/2023 12:04</t>
+          <t>04/11/2023 13:48</t>
         </is>
       </c>
       <c r="R60" t="n">
-        <v>3.44</v>
+        <v>4.41</v>
       </c>
       <c r="S60" t="inlineStr">
         <is>
@@ -5964,16 +5964,16 @@
         </is>
       </c>
       <c r="T60" t="n">
-        <v>3.27</v>
+        <v>8.41</v>
       </c>
       <c r="U60" t="inlineStr">
         <is>
-          <t>04/11/2023 12:04</t>
+          <t>04/11/2023 13:44</t>
         </is>
       </c>
       <c r="V60" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/paok-karditsa/jLeG4asJ/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/ilioupoli-panachaiki/GbFoZVZ8/</t>
         </is>
       </c>
     </row>
@@ -6921,71 +6921,71 @@
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>AEL Larissa</t>
+          <t>Kalamata</t>
         </is>
       </c>
       <c r="G71" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>PAOK B</t>
+          <t>Tilikratis L.</t>
         </is>
       </c>
       <c r="I71" t="n">
         <v>0</v>
       </c>
       <c r="J71" t="n">
-        <v>1.43</v>
+        <v>1.13</v>
       </c>
       <c r="K71" t="inlineStr">
         <is>
-          <t>10/11/2023 02:13</t>
+          <t>11/11/2023 12:01</t>
         </is>
       </c>
       <c r="L71" t="n">
-        <v>1.33</v>
+        <v>1.13</v>
       </c>
       <c r="M71" t="inlineStr">
         <is>
-          <t>11/11/2023 13:40</t>
+          <t>11/11/2023 12:01</t>
         </is>
       </c>
       <c r="N71" t="n">
-        <v>3.99</v>
+        <v>7.63</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>10/11/2023 02:13</t>
+          <t>11/11/2023 12:01</t>
         </is>
       </c>
       <c r="P71" t="n">
-        <v>4.69</v>
+        <v>7.63</v>
       </c>
       <c r="Q71" t="inlineStr">
         <is>
-          <t>11/11/2023 13:40</t>
+          <t>11/11/2023 12:01</t>
         </is>
       </c>
       <c r="R71" t="n">
-        <v>6.04</v>
+        <v>18.11</v>
       </c>
       <c r="S71" t="inlineStr">
         <is>
-          <t>10/11/2023 02:13</t>
+          <t>11/11/2023 12:01</t>
         </is>
       </c>
       <c r="T71" t="n">
-        <v>9.68</v>
+        <v>18.11</v>
       </c>
       <c r="U71" t="inlineStr">
         <is>
-          <t>11/11/2023 13:40</t>
+          <t>11/11/2023 12:01</t>
         </is>
       </c>
       <c r="V71" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/ael-larissa-paok/WYTxM0Cg/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/kalamata-tilikratis-lefkada/6m8bWTJR/</t>
         </is>
       </c>
     </row>
@@ -7013,71 +7013,71 @@
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>Kalamata</t>
+          <t>AEL Larissa</t>
         </is>
       </c>
       <c r="G72" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Tilikratis L.</t>
+          <t>PAOK B</t>
         </is>
       </c>
       <c r="I72" t="n">
         <v>0</v>
       </c>
       <c r="J72" t="n">
-        <v>1.13</v>
+        <v>1.43</v>
       </c>
       <c r="K72" t="inlineStr">
         <is>
-          <t>11/11/2023 12:01</t>
+          <t>10/11/2023 02:13</t>
         </is>
       </c>
       <c r="L72" t="n">
-        <v>1.13</v>
+        <v>1.33</v>
       </c>
       <c r="M72" t="inlineStr">
         <is>
-          <t>11/11/2023 12:01</t>
+          <t>11/11/2023 13:40</t>
         </is>
       </c>
       <c r="N72" t="n">
-        <v>7.63</v>
+        <v>3.99</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>11/11/2023 12:01</t>
+          <t>10/11/2023 02:13</t>
         </is>
       </c>
       <c r="P72" t="n">
-        <v>7.63</v>
+        <v>4.69</v>
       </c>
       <c r="Q72" t="inlineStr">
         <is>
-          <t>11/11/2023 12:01</t>
+          <t>11/11/2023 13:40</t>
         </is>
       </c>
       <c r="R72" t="n">
-        <v>18.11</v>
+        <v>6.04</v>
       </c>
       <c r="S72" t="inlineStr">
         <is>
-          <t>11/11/2023 12:01</t>
+          <t>10/11/2023 02:13</t>
         </is>
       </c>
       <c r="T72" t="n">
-        <v>18.11</v>
+        <v>9.68</v>
       </c>
       <c r="U72" t="inlineStr">
         <is>
-          <t>11/11/2023 12:01</t>
+          <t>11/11/2023 13:40</t>
         </is>
       </c>
       <c r="V72" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/kalamata-tilikratis-lefkada/6m8bWTJR/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/ael-larissa-paok/WYTxM0Cg/</t>
         </is>
       </c>
     </row>
@@ -7657,7 +7657,7 @@
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>Aiolikos</t>
+          <t>Iraklis 1908</t>
         </is>
       </c>
       <c r="G79" t="n">
@@ -7665,63 +7665,63 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Niki Volos</t>
+          <t>Apollon Pontou</t>
         </is>
       </c>
       <c r="I79" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J79" t="n">
-        <v>4.13</v>
+        <v>1.3</v>
       </c>
       <c r="K79" t="inlineStr">
         <is>
-          <t>14/11/2023 15:18</t>
+          <t>14/11/2023 02:12</t>
         </is>
       </c>
       <c r="L79" t="n">
-        <v>3.66</v>
+        <v>1.42</v>
       </c>
       <c r="M79" t="inlineStr">
         <is>
-          <t>15/11/2023 13:38</t>
+          <t>15/11/2023 12:58</t>
         </is>
       </c>
       <c r="N79" t="n">
-        <v>3.43</v>
+        <v>4.59</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>14/11/2023 15:18</t>
+          <t>14/11/2023 02:12</t>
         </is>
       </c>
       <c r="P79" t="n">
-        <v>3.18</v>
+        <v>4.2</v>
       </c>
       <c r="Q79" t="inlineStr">
         <is>
-          <t>15/11/2023 12:23</t>
+          <t>15/11/2023 12:58</t>
         </is>
       </c>
       <c r="R79" t="n">
-        <v>1.83</v>
+        <v>7.84</v>
       </c>
       <c r="S79" t="inlineStr">
         <is>
-          <t>14/11/2023 15:18</t>
+          <t>14/11/2023 02:12</t>
         </is>
       </c>
       <c r="T79" t="n">
-        <v>2.07</v>
+        <v>7.94</v>
       </c>
       <c r="U79" t="inlineStr">
         <is>
-          <t>15/11/2023 13:38</t>
+          <t>15/11/2023 12:58</t>
         </is>
       </c>
       <c r="V79" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/aiolikos-fc-niki-volos/rgFWffl0/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/iraklis-fc-apollon-pontou/0UPRezZg/</t>
         </is>
       </c>
     </row>
@@ -7749,7 +7749,7 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>Iraklis 1908</t>
+          <t>Aiolikos</t>
         </is>
       </c>
       <c r="G80" t="n">
@@ -7757,63 +7757,63 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Apollon Pontou</t>
+          <t>Niki Volos</t>
         </is>
       </c>
       <c r="I80" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J80" t="n">
-        <v>1.3</v>
+        <v>4.13</v>
       </c>
       <c r="K80" t="inlineStr">
         <is>
-          <t>14/11/2023 02:12</t>
+          <t>14/11/2023 15:18</t>
         </is>
       </c>
       <c r="L80" t="n">
-        <v>1.42</v>
+        <v>3.66</v>
       </c>
       <c r="M80" t="inlineStr">
         <is>
-          <t>15/11/2023 12:58</t>
+          <t>15/11/2023 13:38</t>
         </is>
       </c>
       <c r="N80" t="n">
-        <v>4.59</v>
+        <v>3.43</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>14/11/2023 02:12</t>
+          <t>14/11/2023 15:18</t>
         </is>
       </c>
       <c r="P80" t="n">
-        <v>4.2</v>
+        <v>3.18</v>
       </c>
       <c r="Q80" t="inlineStr">
         <is>
-          <t>15/11/2023 12:58</t>
+          <t>15/11/2023 12:23</t>
         </is>
       </c>
       <c r="R80" t="n">
-        <v>7.84</v>
+        <v>1.83</v>
       </c>
       <c r="S80" t="inlineStr">
         <is>
-          <t>14/11/2023 02:12</t>
+          <t>14/11/2023 15:18</t>
         </is>
       </c>
       <c r="T80" t="n">
-        <v>7.94</v>
+        <v>2.07</v>
       </c>
       <c r="U80" t="inlineStr">
         <is>
-          <t>15/11/2023 12:58</t>
+          <t>15/11/2023 13:38</t>
         </is>
       </c>
       <c r="V80" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/iraklis-fc-apollon-pontou/0UPRezZg/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/aiolikos-fc-niki-volos/rgFWffl0/</t>
         </is>
       </c>
     </row>
@@ -8025,7 +8025,7 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>Karditsa</t>
+          <t>Tilikratis L.</t>
         </is>
       </c>
       <c r="G83" t="n">
@@ -8033,14 +8033,14 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Levadiakos</t>
+          <t>Panachaiki</t>
         </is>
       </c>
       <c r="I83" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J83" t="n">
-        <v>4.29</v>
+        <v>2.27</v>
       </c>
       <c r="K83" t="inlineStr">
         <is>
@@ -8048,15 +8048,15 @@
         </is>
       </c>
       <c r="L83" t="n">
-        <v>5.74</v>
+        <v>2.31</v>
       </c>
       <c r="M83" t="inlineStr">
         <is>
-          <t>19/11/2023 13:50</t>
+          <t>19/11/2023 13:54</t>
         </is>
       </c>
       <c r="N83" t="n">
-        <v>3.08</v>
+        <v>2.92</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
@@ -8064,15 +8064,15 @@
         </is>
       </c>
       <c r="P83" t="n">
-        <v>3.31</v>
+        <v>2.95</v>
       </c>
       <c r="Q83" t="inlineStr">
         <is>
-          <t>19/11/2023 13:50</t>
+          <t>19/11/2023 13:54</t>
         </is>
       </c>
       <c r="R83" t="n">
-        <v>1.79</v>
+        <v>3.02</v>
       </c>
       <c r="S83" t="inlineStr">
         <is>
@@ -8080,16 +8080,16 @@
         </is>
       </c>
       <c r="T83" t="n">
-        <v>1.68</v>
+        <v>3.35</v>
       </c>
       <c r="U83" t="inlineStr">
         <is>
-          <t>19/11/2023 13:50</t>
+          <t>19/11/2023 13:51</t>
         </is>
       </c>
       <c r="V83" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/karditsa-levadiakos/2cncBFYt/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/tilikratis-lefkada-panachaiki/rZYSo9JE/</t>
         </is>
       </c>
     </row>
@@ -8117,71 +8117,71 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>Apollon Pontou</t>
+          <t>Kalamata</t>
         </is>
       </c>
       <c r="G84" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Aiolikos</t>
+          <t>Diagoras</t>
         </is>
       </c>
       <c r="I84" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J84" t="n">
-        <v>2.77</v>
+        <v>1.3</v>
       </c>
       <c r="K84" t="inlineStr">
         <is>
-          <t>19/11/2023 03:12</t>
+          <t>18/11/2023 02:12</t>
         </is>
       </c>
       <c r="L84" t="n">
-        <v>2.89</v>
+        <v>1.26</v>
       </c>
       <c r="M84" t="inlineStr">
         <is>
-          <t>19/11/2023 13:41</t>
+          <t>19/11/2023 13:49</t>
         </is>
       </c>
       <c r="N84" t="n">
-        <v>2.87</v>
+        <v>4.57</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
-          <t>19/11/2023 03:12</t>
+          <t>18/11/2023 02:12</t>
         </is>
       </c>
       <c r="P84" t="n">
-        <v>2.85</v>
+        <v>5.23</v>
       </c>
       <c r="Q84" t="inlineStr">
         <is>
-          <t>19/11/2023 13:24</t>
+          <t>19/11/2023 13:56</t>
         </is>
       </c>
       <c r="R84" t="n">
-        <v>2.65</v>
+        <v>8.08</v>
       </c>
       <c r="S84" t="inlineStr">
         <is>
-          <t>19/11/2023 03:12</t>
+          <t>18/11/2023 02:12</t>
         </is>
       </c>
       <c r="T84" t="n">
-        <v>2.67</v>
+        <v>12.07</v>
       </c>
       <c r="U84" t="inlineStr">
         <is>
-          <t>19/11/2023 13:41</t>
+          <t>19/11/2023 13:56</t>
         </is>
       </c>
       <c r="V84" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/apollon-pontou-aiolikos-fc/pIaVFeQP/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/kalamata-diagoras-fc/xxnsO5R7/</t>
         </is>
       </c>
     </row>
@@ -8209,71 +8209,71 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>Tilikratis L.</t>
+          <t>Apollon Pontou</t>
         </is>
       </c>
       <c r="G85" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>Panachaiki</t>
+          <t>Aiolikos</t>
         </is>
       </c>
       <c r="I85" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J85" t="n">
-        <v>2.27</v>
+        <v>2.77</v>
       </c>
       <c r="K85" t="inlineStr">
         <is>
-          <t>18/11/2023 02:12</t>
+          <t>19/11/2023 03:12</t>
         </is>
       </c>
       <c r="L85" t="n">
-        <v>2.31</v>
+        <v>2.89</v>
       </c>
       <c r="M85" t="inlineStr">
         <is>
-          <t>19/11/2023 13:54</t>
+          <t>19/11/2023 13:41</t>
         </is>
       </c>
       <c r="N85" t="n">
-        <v>2.92</v>
+        <v>2.87</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
-          <t>18/11/2023 02:12</t>
+          <t>19/11/2023 03:12</t>
         </is>
       </c>
       <c r="P85" t="n">
-        <v>2.95</v>
+        <v>2.85</v>
       </c>
       <c r="Q85" t="inlineStr">
         <is>
-          <t>19/11/2023 13:54</t>
+          <t>19/11/2023 13:24</t>
         </is>
       </c>
       <c r="R85" t="n">
-        <v>3.02</v>
+        <v>2.65</v>
       </c>
       <c r="S85" t="inlineStr">
         <is>
-          <t>18/11/2023 02:12</t>
+          <t>19/11/2023 03:12</t>
         </is>
       </c>
       <c r="T85" t="n">
-        <v>3.35</v>
+        <v>2.67</v>
       </c>
       <c r="U85" t="inlineStr">
         <is>
-          <t>19/11/2023 13:51</t>
+          <t>19/11/2023 13:41</t>
         </is>
       </c>
       <c r="V85" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/tilikratis-lefkada-panachaiki/rZYSo9JE/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/apollon-pontou-aiolikos-fc/pIaVFeQP/</t>
         </is>
       </c>
     </row>
@@ -8301,22 +8301,22 @@
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>Kampaniakos</t>
+          <t>Giouchtas</t>
         </is>
       </c>
       <c r="G86" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>Iraklis 1908</t>
+          <t>PAE Chania</t>
         </is>
       </c>
       <c r="I86" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J86" t="n">
-        <v>3.87</v>
+        <v>3.28</v>
       </c>
       <c r="K86" t="inlineStr">
         <is>
@@ -8324,15 +8324,15 @@
         </is>
       </c>
       <c r="L86" t="n">
-        <v>4.12</v>
+        <v>3.93</v>
       </c>
       <c r="M86" t="inlineStr">
         <is>
-          <t>19/11/2023 12:04</t>
+          <t>19/11/2023 13:14</t>
         </is>
       </c>
       <c r="N86" t="n">
-        <v>3.15</v>
+        <v>2.86</v>
       </c>
       <c r="O86" t="inlineStr">
         <is>
@@ -8340,15 +8340,15 @@
         </is>
       </c>
       <c r="P86" t="n">
-        <v>3.11</v>
+        <v>3.05</v>
       </c>
       <c r="Q86" t="inlineStr">
         <is>
-          <t>19/11/2023 12:52</t>
+          <t>19/11/2023 12:51</t>
         </is>
       </c>
       <c r="R86" t="n">
-        <v>1.85</v>
+        <v>2.17</v>
       </c>
       <c r="S86" t="inlineStr">
         <is>
@@ -8356,16 +8356,16 @@
         </is>
       </c>
       <c r="T86" t="n">
-        <v>1.97</v>
+        <v>2.04</v>
       </c>
       <c r="U86" t="inlineStr">
         <is>
-          <t>19/11/2023 12:52</t>
+          <t>19/11/2023 13:14</t>
         </is>
       </c>
       <c r="V86" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/kampaniakos-iraklis-fc/6R0RGyBJ/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/giouchtas-pae-chania/4rzPnk48/</t>
         </is>
       </c>
     </row>
@@ -8393,22 +8393,22 @@
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>Ionikos</t>
+          <t>Kampaniakos</t>
         </is>
       </c>
       <c r="G87" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>Athens Kallithea</t>
+          <t>Iraklis 1908</t>
         </is>
       </c>
       <c r="I87" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J87" t="n">
-        <v>3.12</v>
+        <v>3.87</v>
       </c>
       <c r="K87" t="inlineStr">
         <is>
@@ -8416,15 +8416,15 @@
         </is>
       </c>
       <c r="L87" t="n">
-        <v>2.89</v>
+        <v>4.12</v>
       </c>
       <c r="M87" t="inlineStr">
         <is>
-          <t>19/11/2023 13:29</t>
+          <t>19/11/2023 12:04</t>
         </is>
       </c>
       <c r="N87" t="n">
-        <v>2.85</v>
+        <v>3.15</v>
       </c>
       <c r="O87" t="inlineStr">
         <is>
@@ -8432,15 +8432,15 @@
         </is>
       </c>
       <c r="P87" t="n">
-        <v>2.91</v>
+        <v>3.11</v>
       </c>
       <c r="Q87" t="inlineStr">
         <is>
-          <t>19/11/2023 13:29</t>
+          <t>19/11/2023 12:52</t>
         </is>
       </c>
       <c r="R87" t="n">
-        <v>2.26</v>
+        <v>1.85</v>
       </c>
       <c r="S87" t="inlineStr">
         <is>
@@ -8448,16 +8448,16 @@
         </is>
       </c>
       <c r="T87" t="n">
-        <v>2.62</v>
+        <v>1.97</v>
       </c>
       <c r="U87" t="inlineStr">
         <is>
-          <t>19/11/2023 13:29</t>
+          <t>19/11/2023 12:52</t>
         </is>
       </c>
       <c r="V87" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/ionikos-athens-kallithea/v1SypmlR/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/kampaniakos-iraklis-fc/6R0RGyBJ/</t>
         </is>
       </c>
     </row>
@@ -8485,7 +8485,7 @@
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>Giouchtas</t>
+          <t>Ionikos</t>
         </is>
       </c>
       <c r="G88" t="n">
@@ -8493,14 +8493,14 @@
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>PAE Chania</t>
+          <t>Athens Kallithea</t>
         </is>
       </c>
       <c r="I88" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J88" t="n">
-        <v>3.28</v>
+        <v>3.12</v>
       </c>
       <c r="K88" t="inlineStr">
         <is>
@@ -8508,15 +8508,15 @@
         </is>
       </c>
       <c r="L88" t="n">
-        <v>3.93</v>
+        <v>2.89</v>
       </c>
       <c r="M88" t="inlineStr">
         <is>
-          <t>19/11/2023 13:14</t>
+          <t>19/11/2023 13:29</t>
         </is>
       </c>
       <c r="N88" t="n">
-        <v>2.86</v>
+        <v>2.85</v>
       </c>
       <c r="O88" t="inlineStr">
         <is>
@@ -8524,15 +8524,15 @@
         </is>
       </c>
       <c r="P88" t="n">
-        <v>3.05</v>
+        <v>2.91</v>
       </c>
       <c r="Q88" t="inlineStr">
         <is>
-          <t>19/11/2023 12:51</t>
+          <t>19/11/2023 13:29</t>
         </is>
       </c>
       <c r="R88" t="n">
-        <v>2.17</v>
+        <v>2.26</v>
       </c>
       <c r="S88" t="inlineStr">
         <is>
@@ -8540,16 +8540,16 @@
         </is>
       </c>
       <c r="T88" t="n">
-        <v>2.04</v>
+        <v>2.62</v>
       </c>
       <c r="U88" t="inlineStr">
         <is>
-          <t>19/11/2023 13:14</t>
+          <t>19/11/2023 13:29</t>
         </is>
       </c>
       <c r="V88" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/giouchtas-pae-chania/4rzPnk48/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/ionikos-athens-kallithea/v1SypmlR/</t>
         </is>
       </c>
     </row>
@@ -8577,22 +8577,22 @@
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>Kalamata</t>
+          <t>Karditsa</t>
         </is>
       </c>
       <c r="G89" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>Diagoras</t>
+          <t>Levadiakos</t>
         </is>
       </c>
       <c r="I89" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J89" t="n">
-        <v>1.3</v>
+        <v>4.29</v>
       </c>
       <c r="K89" t="inlineStr">
         <is>
@@ -8600,15 +8600,15 @@
         </is>
       </c>
       <c r="L89" t="n">
-        <v>1.26</v>
+        <v>5.74</v>
       </c>
       <c r="M89" t="inlineStr">
         <is>
-          <t>19/11/2023 13:49</t>
+          <t>19/11/2023 13:50</t>
         </is>
       </c>
       <c r="N89" t="n">
-        <v>4.57</v>
+        <v>3.08</v>
       </c>
       <c r="O89" t="inlineStr">
         <is>
@@ -8616,15 +8616,15 @@
         </is>
       </c>
       <c r="P89" t="n">
-        <v>5.23</v>
+        <v>3.31</v>
       </c>
       <c r="Q89" t="inlineStr">
         <is>
-          <t>19/11/2023 13:56</t>
+          <t>19/11/2023 13:50</t>
         </is>
       </c>
       <c r="R89" t="n">
-        <v>8.08</v>
+        <v>1.79</v>
       </c>
       <c r="S89" t="inlineStr">
         <is>
@@ -8632,16 +8632,16 @@
         </is>
       </c>
       <c r="T89" t="n">
-        <v>12.07</v>
+        <v>1.68</v>
       </c>
       <c r="U89" t="inlineStr">
         <is>
-          <t>19/11/2023 13:56</t>
+          <t>19/11/2023 13:50</t>
         </is>
       </c>
       <c r="V89" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/kalamata-diagoras-fc/xxnsO5R7/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/karditsa-levadiakos/2cncBFYt/</t>
         </is>
       </c>
     </row>
@@ -8761,22 +8761,22 @@
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>Iraklis 1908</t>
+          <t>Athens Kallithea</t>
         </is>
       </c>
       <c r="G91" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>AEK Athens FC B</t>
+          <t>Tilikratis L.</t>
         </is>
       </c>
       <c r="I91" t="n">
         <v>0</v>
       </c>
       <c r="J91" t="n">
-        <v>1.5</v>
+        <v>1.16</v>
       </c>
       <c r="K91" t="inlineStr">
         <is>
@@ -8784,15 +8784,15 @@
         </is>
       </c>
       <c r="L91" t="n">
-        <v>1.67</v>
+        <v>1.11</v>
       </c>
       <c r="M91" t="inlineStr">
         <is>
-          <t>25/11/2023 13:45</t>
+          <t>25/11/2023 13:09</t>
         </is>
       </c>
       <c r="N91" t="n">
-        <v>3.67</v>
+        <v>6.22</v>
       </c>
       <c r="O91" t="inlineStr">
         <is>
@@ -8800,15 +8800,15 @@
         </is>
       </c>
       <c r="P91" t="n">
-        <v>3.53</v>
+        <v>8.289999999999999</v>
       </c>
       <c r="Q91" t="inlineStr">
         <is>
-          <t>25/11/2023 13:45</t>
+          <t>25/11/2023 13:10</t>
         </is>
       </c>
       <c r="R91" t="n">
-        <v>5.66</v>
+        <v>12.53</v>
       </c>
       <c r="S91" t="inlineStr">
         <is>
@@ -8816,16 +8816,16 @@
         </is>
       </c>
       <c r="T91" t="n">
-        <v>5.3</v>
+        <v>23.73</v>
       </c>
       <c r="U91" t="inlineStr">
         <is>
-          <t>25/11/2023 13:45</t>
+          <t>25/11/2023 13:10</t>
         </is>
       </c>
       <c r="V91" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/iraklis-fc-aek/zmvA8DIa/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/athens-kallithea-tilikratis-lefkada/QL6KyPe7/</t>
         </is>
       </c>
     </row>
@@ -8945,22 +8945,22 @@
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>Athens Kallithea</t>
+          <t>Iraklis 1908</t>
         </is>
       </c>
       <c r="G93" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H93" t="inlineStr">
         <is>
-          <t>Tilikratis L.</t>
+          <t>AEK Athens FC B</t>
         </is>
       </c>
       <c r="I93" t="n">
         <v>0</v>
       </c>
       <c r="J93" t="n">
-        <v>1.16</v>
+        <v>1.5</v>
       </c>
       <c r="K93" t="inlineStr">
         <is>
@@ -8968,15 +8968,15 @@
         </is>
       </c>
       <c r="L93" t="n">
-        <v>1.11</v>
+        <v>1.67</v>
       </c>
       <c r="M93" t="inlineStr">
         <is>
-          <t>25/11/2023 13:09</t>
+          <t>25/11/2023 13:45</t>
         </is>
       </c>
       <c r="N93" t="n">
-        <v>6.22</v>
+        <v>3.67</v>
       </c>
       <c r="O93" t="inlineStr">
         <is>
@@ -8984,15 +8984,15 @@
         </is>
       </c>
       <c r="P93" t="n">
-        <v>8.289999999999999</v>
+        <v>3.53</v>
       </c>
       <c r="Q93" t="inlineStr">
         <is>
-          <t>25/11/2023 13:10</t>
+          <t>25/11/2023 13:45</t>
         </is>
       </c>
       <c r="R93" t="n">
-        <v>12.53</v>
+        <v>5.66</v>
       </c>
       <c r="S93" t="inlineStr">
         <is>
@@ -9000,16 +9000,16 @@
         </is>
       </c>
       <c r="T93" t="n">
-        <v>23.73</v>
+        <v>5.3</v>
       </c>
       <c r="U93" t="inlineStr">
         <is>
-          <t>25/11/2023 13:10</t>
+          <t>25/11/2023 13:45</t>
         </is>
       </c>
       <c r="V93" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/athens-kallithea-tilikratis-lefkada/QL6KyPe7/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/iraklis-fc-aek/zmvA8DIa/</t>
         </is>
       </c>
     </row>
@@ -9129,22 +9129,22 @@
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>PAE Chania</t>
+          <t>Ilioupoli</t>
         </is>
       </c>
       <c r="G95" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H95" t="inlineStr">
         <is>
-          <t>PAE Egaleo</t>
+          <t>Giouchtas</t>
         </is>
       </c>
       <c r="I95" t="n">
         <v>0</v>
       </c>
       <c r="J95" t="n">
-        <v>1.55</v>
+        <v>1.97</v>
       </c>
       <c r="K95" t="inlineStr">
         <is>
@@ -9152,15 +9152,15 @@
         </is>
       </c>
       <c r="L95" t="n">
-        <v>1.2</v>
+        <v>2.19</v>
       </c>
       <c r="M95" t="inlineStr">
         <is>
-          <t>26/11/2023 13:55</t>
+          <t>26/11/2023 13:59</t>
         </is>
       </c>
       <c r="N95" t="n">
-        <v>3.48</v>
+        <v>3.02</v>
       </c>
       <c r="O95" t="inlineStr">
         <is>
@@ -9168,15 +9168,15 @@
         </is>
       </c>
       <c r="P95" t="n">
-        <v>6.56</v>
+        <v>3.19</v>
       </c>
       <c r="Q95" t="inlineStr">
         <is>
-          <t>26/11/2023 13:58</t>
+          <t>26/11/2023 13:59</t>
         </is>
       </c>
       <c r="R95" t="n">
-        <v>5.44</v>
+        <v>3.62</v>
       </c>
       <c r="S95" t="inlineStr">
         <is>
@@ -9184,16 +9184,16 @@
         </is>
       </c>
       <c r="T95" t="n">
-        <v>11.76</v>
+        <v>3.32</v>
       </c>
       <c r="U95" t="inlineStr">
         <is>
-          <t>26/11/2023 13:58</t>
+          <t>26/11/2023 13:59</t>
         </is>
       </c>
       <c r="V95" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/pae-chania-pae-egaleo/zXD7vRBl/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/ilioupoli-giouchtas/Wb7Gx5t1/</t>
         </is>
       </c>
     </row>
@@ -9221,7 +9221,7 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>Karditsa</t>
+          <t>PAE Chania</t>
         </is>
       </c>
       <c r="G96" t="n">
@@ -9229,14 +9229,14 @@
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>Niki Volos</t>
+          <t>PAE Egaleo</t>
         </is>
       </c>
       <c r="I96" t="n">
         <v>0</v>
       </c>
       <c r="J96" t="n">
-        <v>3.26</v>
+        <v>1.55</v>
       </c>
       <c r="K96" t="inlineStr">
         <is>
@@ -9244,15 +9244,15 @@
         </is>
       </c>
       <c r="L96" t="n">
-        <v>3.72</v>
+        <v>1.2</v>
       </c>
       <c r="M96" t="inlineStr">
         <is>
-          <t>26/11/2023 13:46</t>
+          <t>26/11/2023 13:55</t>
         </is>
       </c>
       <c r="N96" t="n">
-        <v>2.83</v>
+        <v>3.48</v>
       </c>
       <c r="O96" t="inlineStr">
         <is>
@@ -9260,15 +9260,15 @@
         </is>
       </c>
       <c r="P96" t="n">
-        <v>2.91</v>
+        <v>6.56</v>
       </c>
       <c r="Q96" t="inlineStr">
         <is>
-          <t>26/11/2023 13:46</t>
+          <t>26/11/2023 13:58</t>
         </is>
       </c>
       <c r="R96" t="n">
-        <v>2.2</v>
+        <v>5.44</v>
       </c>
       <c r="S96" t="inlineStr">
         <is>
@@ -9276,16 +9276,16 @@
         </is>
       </c>
       <c r="T96" t="n">
-        <v>2.18</v>
+        <v>11.76</v>
       </c>
       <c r="U96" t="inlineStr">
         <is>
-          <t>26/11/2023 13:46</t>
+          <t>26/11/2023 13:58</t>
         </is>
       </c>
       <c r="V96" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/karditsa-niki-volos/vuyR4VHO/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/pae-chania-pae-egaleo/zXD7vRBl/</t>
         </is>
       </c>
     </row>
@@ -9313,22 +9313,22 @@
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>Makedonikos</t>
+          <t>Panachaiki</t>
         </is>
       </c>
       <c r="G97" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>Apollon Pontou</t>
+          <t>Diagoras</t>
         </is>
       </c>
       <c r="I97" t="n">
         <v>1</v>
       </c>
       <c r="J97" t="n">
-        <v>1.53</v>
+        <v>2.77</v>
       </c>
       <c r="K97" t="inlineStr">
         <is>
@@ -9336,15 +9336,15 @@
         </is>
       </c>
       <c r="L97" t="n">
-        <v>1.54</v>
+        <v>2.63</v>
       </c>
       <c r="M97" t="inlineStr">
         <is>
-          <t>26/11/2023 13:44</t>
+          <t>26/11/2023 13:40</t>
         </is>
       </c>
       <c r="N97" t="n">
-        <v>3.51</v>
+        <v>2.87</v>
       </c>
       <c r="O97" t="inlineStr">
         <is>
@@ -9352,15 +9352,15 @@
         </is>
       </c>
       <c r="P97" t="n">
-        <v>3.65</v>
+        <v>2.72</v>
       </c>
       <c r="Q97" t="inlineStr">
         <is>
-          <t>26/11/2023 13:59</t>
+          <t>26/11/2023 13:40</t>
         </is>
       </c>
       <c r="R97" t="n">
-        <v>5.58</v>
+        <v>2.47</v>
       </c>
       <c r="S97" t="inlineStr">
         <is>
@@ -9368,16 +9368,16 @@
         </is>
       </c>
       <c r="T97" t="n">
-        <v>6.81</v>
+        <v>3.09</v>
       </c>
       <c r="U97" t="inlineStr">
         <is>
-          <t>26/11/2023 13:59</t>
+          <t>26/11/2023 13:40</t>
         </is>
       </c>
       <c r="V97" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/makedonikos-neapolis-apollon-pontou/QyXM5B2I/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/panachaiki-diagoras-fc/h88CwoRf/</t>
         </is>
       </c>
     </row>
@@ -9405,22 +9405,22 @@
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>Ilioupoli</t>
+          <t>Karditsa</t>
         </is>
       </c>
       <c r="G98" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t>Giouchtas</t>
+          <t>Niki Volos</t>
         </is>
       </c>
       <c r="I98" t="n">
         <v>0</v>
       </c>
       <c r="J98" t="n">
-        <v>1.97</v>
+        <v>3.26</v>
       </c>
       <c r="K98" t="inlineStr">
         <is>
@@ -9428,15 +9428,15 @@
         </is>
       </c>
       <c r="L98" t="n">
-        <v>2.19</v>
+        <v>3.72</v>
       </c>
       <c r="M98" t="inlineStr">
         <is>
-          <t>26/11/2023 13:59</t>
+          <t>26/11/2023 13:46</t>
         </is>
       </c>
       <c r="N98" t="n">
-        <v>3.02</v>
+        <v>2.83</v>
       </c>
       <c r="O98" t="inlineStr">
         <is>
@@ -9444,15 +9444,15 @@
         </is>
       </c>
       <c r="P98" t="n">
-        <v>3.19</v>
+        <v>2.91</v>
       </c>
       <c r="Q98" t="inlineStr">
         <is>
-          <t>26/11/2023 13:59</t>
+          <t>26/11/2023 13:46</t>
         </is>
       </c>
       <c r="R98" t="n">
-        <v>3.62</v>
+        <v>2.2</v>
       </c>
       <c r="S98" t="inlineStr">
         <is>
@@ -9460,16 +9460,16 @@
         </is>
       </c>
       <c r="T98" t="n">
-        <v>3.32</v>
+        <v>2.18</v>
       </c>
       <c r="U98" t="inlineStr">
         <is>
-          <t>26/11/2023 13:59</t>
+          <t>26/11/2023 13:46</t>
         </is>
       </c>
       <c r="V98" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/ilioupoli-giouchtas/Wb7Gx5t1/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/karditsa-niki-volos/vuyR4VHO/</t>
         </is>
       </c>
     </row>
@@ -9497,22 +9497,22 @@
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>Panachaiki</t>
+          <t>Makedonikos</t>
         </is>
       </c>
       <c r="G99" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>Diagoras</t>
+          <t>Apollon Pontou</t>
         </is>
       </c>
       <c r="I99" t="n">
         <v>1</v>
       </c>
       <c r="J99" t="n">
-        <v>2.77</v>
+        <v>1.53</v>
       </c>
       <c r="K99" t="inlineStr">
         <is>
@@ -9520,15 +9520,15 @@
         </is>
       </c>
       <c r="L99" t="n">
-        <v>2.63</v>
+        <v>1.54</v>
       </c>
       <c r="M99" t="inlineStr">
         <is>
-          <t>26/11/2023 13:40</t>
+          <t>26/11/2023 13:44</t>
         </is>
       </c>
       <c r="N99" t="n">
-        <v>2.87</v>
+        <v>3.51</v>
       </c>
       <c r="O99" t="inlineStr">
         <is>
@@ -9536,15 +9536,15 @@
         </is>
       </c>
       <c r="P99" t="n">
-        <v>2.72</v>
+        <v>3.65</v>
       </c>
       <c r="Q99" t="inlineStr">
         <is>
-          <t>26/11/2023 13:40</t>
+          <t>26/11/2023 13:59</t>
         </is>
       </c>
       <c r="R99" t="n">
-        <v>2.47</v>
+        <v>5.58</v>
       </c>
       <c r="S99" t="inlineStr">
         <is>
@@ -9552,16 +9552,16 @@
         </is>
       </c>
       <c r="T99" t="n">
-        <v>3.09</v>
+        <v>6.81</v>
       </c>
       <c r="U99" t="inlineStr">
         <is>
-          <t>26/11/2023 13:40</t>
+          <t>26/11/2023 13:59</t>
         </is>
       </c>
       <c r="V99" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/panachaiki-diagoras-fc/h88CwoRf/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/makedonikos-neapolis-apollon-pontou/QyXM5B2I/</t>
         </is>
       </c>
     </row>
@@ -9773,7 +9773,7 @@
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>Kozani FC</t>
+          <t>Panathinaikos B</t>
         </is>
       </c>
       <c r="G102" t="n">
@@ -9781,63 +9781,63 @@
       </c>
       <c r="H102" t="inlineStr">
         <is>
-          <t>PAOK B</t>
+          <t>Ilioupoli</t>
         </is>
       </c>
       <c r="I102" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J102" t="n">
-        <v>2.15</v>
+        <v>2.39</v>
       </c>
       <c r="K102" t="inlineStr">
         <is>
-          <t>14/11/2023 02:12</t>
+          <t>28/11/2023 02:12</t>
         </is>
       </c>
       <c r="L102" t="n">
-        <v>1.95</v>
+        <v>3.1</v>
       </c>
       <c r="M102" t="inlineStr">
         <is>
-          <t>29/11/2023 12:20</t>
+          <t>29/11/2023 13:58</t>
         </is>
       </c>
       <c r="N102" t="n">
-        <v>2.95</v>
+        <v>2.88</v>
       </c>
       <c r="O102" t="inlineStr">
         <is>
-          <t>14/11/2023 02:12</t>
+          <t>28/11/2023 02:12</t>
         </is>
       </c>
       <c r="P102" t="n">
-        <v>3.2</v>
+        <v>2.93</v>
       </c>
       <c r="Q102" t="inlineStr">
         <is>
-          <t>29/11/2023 12:23</t>
+          <t>29/11/2023 13:57</t>
         </is>
       </c>
       <c r="R102" t="n">
-        <v>3.23</v>
+        <v>2.86</v>
       </c>
       <c r="S102" t="inlineStr">
         <is>
-          <t>14/11/2023 02:12</t>
+          <t>28/11/2023 02:12</t>
         </is>
       </c>
       <c r="T102" t="n">
-        <v>4.06</v>
+        <v>2.46</v>
       </c>
       <c r="U102" t="inlineStr">
         <is>
-          <t>29/11/2023 12:20</t>
+          <t>29/11/2023 13:58</t>
         </is>
       </c>
       <c r="V102" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/kozani-fc-paok/S2CKcd4s/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/panathinaikos-ilioupoli/QcOXpTYK/</t>
         </is>
       </c>
     </row>
@@ -9865,7 +9865,7 @@
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>Panathinaikos B</t>
+          <t>Kozani FC</t>
         </is>
       </c>
       <c r="G103" t="n">
@@ -9873,63 +9873,63 @@
       </c>
       <c r="H103" t="inlineStr">
         <is>
-          <t>Ilioupoli</t>
+          <t>PAOK B</t>
         </is>
       </c>
       <c r="I103" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J103" t="n">
-        <v>2.39</v>
+        <v>2.15</v>
       </c>
       <c r="K103" t="inlineStr">
         <is>
-          <t>28/11/2023 02:12</t>
+          <t>14/11/2023 02:12</t>
         </is>
       </c>
       <c r="L103" t="n">
-        <v>3.1</v>
+        <v>1.95</v>
       </c>
       <c r="M103" t="inlineStr">
         <is>
-          <t>29/11/2023 13:58</t>
+          <t>29/11/2023 12:20</t>
         </is>
       </c>
       <c r="N103" t="n">
-        <v>2.88</v>
+        <v>2.95</v>
       </c>
       <c r="O103" t="inlineStr">
         <is>
-          <t>28/11/2023 02:12</t>
+          <t>14/11/2023 02:12</t>
         </is>
       </c>
       <c r="P103" t="n">
-        <v>2.93</v>
+        <v>3.2</v>
       </c>
       <c r="Q103" t="inlineStr">
         <is>
-          <t>29/11/2023 13:57</t>
+          <t>29/11/2023 12:23</t>
         </is>
       </c>
       <c r="R103" t="n">
-        <v>2.86</v>
+        <v>3.23</v>
       </c>
       <c r="S103" t="inlineStr">
         <is>
-          <t>28/11/2023 02:12</t>
+          <t>14/11/2023 02:12</t>
         </is>
       </c>
       <c r="T103" t="n">
-        <v>2.46</v>
+        <v>4.06</v>
       </c>
       <c r="U103" t="inlineStr">
         <is>
-          <t>29/11/2023 13:58</t>
+          <t>29/11/2023 12:20</t>
         </is>
       </c>
       <c r="V103" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/panathinaikos-ilioupoli/QcOXpTYK/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/kozani-fc-paok/S2CKcd4s/</t>
         </is>
       </c>
     </row>
@@ -10141,22 +10141,22 @@
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>Giouchtas</t>
+          <t>AEL Larissa</t>
         </is>
       </c>
       <c r="G106" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H106" t="inlineStr">
         <is>
-          <t>Ionikos</t>
+          <t>Niki Volos</t>
         </is>
       </c>
       <c r="I106" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J106" t="n">
-        <v>3.23</v>
+        <v>1.86</v>
       </c>
       <c r="K106" t="inlineStr">
         <is>
@@ -10164,15 +10164,15 @@
         </is>
       </c>
       <c r="L106" t="n">
-        <v>3.35</v>
+        <v>1.88</v>
       </c>
       <c r="M106" t="inlineStr">
         <is>
-          <t>03/12/2023 13:39</t>
+          <t>03/12/2023 13:59</t>
         </is>
       </c>
       <c r="N106" t="n">
-        <v>2.8</v>
+        <v>2.96</v>
       </c>
       <c r="O106" t="inlineStr">
         <is>
@@ -10180,15 +10180,15 @@
         </is>
       </c>
       <c r="P106" t="n">
-        <v>2.79</v>
+        <v>3.11</v>
       </c>
       <c r="Q106" t="inlineStr">
         <is>
-          <t>03/12/2023 13:39</t>
+          <t>03/12/2023 13:59</t>
         </is>
       </c>
       <c r="R106" t="n">
-        <v>2.28</v>
+        <v>4.28</v>
       </c>
       <c r="S106" t="inlineStr">
         <is>
@@ -10196,16 +10196,16 @@
         </is>
       </c>
       <c r="T106" t="n">
-        <v>2.42</v>
+        <v>4.59</v>
       </c>
       <c r="U106" t="inlineStr">
         <is>
-          <t>03/12/2023 13:39</t>
+          <t>03/12/2023 13:59</t>
         </is>
       </c>
       <c r="V106" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/giouchtas-ionikos/YFwVHu7U/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/ael-larissa-niki-volos/8GQuMWna/</t>
         </is>
       </c>
     </row>
@@ -10233,71 +10233,71 @@
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>Ilioupoli</t>
+          <t>Iraklis 1908</t>
         </is>
       </c>
       <c r="G107" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H107" t="inlineStr">
         <is>
-          <t>PAE Egaleo</t>
+          <t>Kozani FC</t>
         </is>
       </c>
       <c r="I107" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J107" t="n">
-        <v>2.1</v>
+        <v>1.75</v>
       </c>
       <c r="K107" t="inlineStr">
         <is>
-          <t>02/12/2023 02:42</t>
+          <t>02/12/2023 02:13</t>
         </is>
       </c>
       <c r="L107" t="n">
-        <v>1.85</v>
+        <v>1.91</v>
       </c>
       <c r="M107" t="inlineStr">
         <is>
-          <t>03/12/2023 13:55</t>
+          <t>03/12/2023 13:50</t>
         </is>
       </c>
       <c r="N107" t="n">
-        <v>2.97</v>
+        <v>3.12</v>
       </c>
       <c r="O107" t="inlineStr">
         <is>
-          <t>02/12/2023 02:42</t>
+          <t>02/12/2023 02:13</t>
         </is>
       </c>
       <c r="P107" t="n">
-        <v>3.16</v>
+        <v>3.12</v>
       </c>
       <c r="Q107" t="inlineStr">
         <is>
-          <t>03/12/2023 13:55</t>
+          <t>03/12/2023 13:50</t>
         </is>
       </c>
       <c r="R107" t="n">
-        <v>3.39</v>
+        <v>4.71</v>
       </c>
       <c r="S107" t="inlineStr">
         <is>
-          <t>02/12/2023 02:42</t>
+          <t>02/12/2023 02:13</t>
         </is>
       </c>
       <c r="T107" t="n">
-        <v>4.65</v>
+        <v>4.4</v>
       </c>
       <c r="U107" t="inlineStr">
         <is>
-          <t>03/12/2023 13:55</t>
+          <t>03/12/2023 13:50</t>
         </is>
       </c>
       <c r="V107" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/ilioupoli-pae-egaleo/fPvRILiO/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/iraklis-fc-kozani-fc/hrP8TEfP/</t>
         </is>
       </c>
     </row>
@@ -10325,22 +10325,22 @@
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>Kalamata</t>
+          <t>Apollon Pontou</t>
         </is>
       </c>
       <c r="G108" t="n">
+        <v>2</v>
+      </c>
+      <c r="H108" t="inlineStr">
+        <is>
+          <t>Karditsa</t>
+        </is>
+      </c>
+      <c r="I108" t="n">
         <v>1</v>
       </c>
-      <c r="H108" t="inlineStr">
-        <is>
-          <t>Panachaiki</t>
-        </is>
-      </c>
-      <c r="I108" t="n">
-        <v>0</v>
-      </c>
       <c r="J108" t="n">
-        <v>1.25</v>
+        <v>3.51</v>
       </c>
       <c r="K108" t="inlineStr">
         <is>
@@ -10348,15 +10348,15 @@
         </is>
       </c>
       <c r="L108" t="n">
-        <v>1.21</v>
+        <v>3.95</v>
       </c>
       <c r="M108" t="inlineStr">
         <is>
-          <t>03/12/2023 13:50</t>
+          <t>03/12/2023 13:33</t>
         </is>
       </c>
       <c r="N108" t="n">
-        <v>5.02</v>
+        <v>2.83</v>
       </c>
       <c r="O108" t="inlineStr">
         <is>
@@ -10364,15 +10364,15 @@
         </is>
       </c>
       <c r="P108" t="n">
-        <v>5.58</v>
+        <v>2.85</v>
       </c>
       <c r="Q108" t="inlineStr">
         <is>
-          <t>03/12/2023 13:50</t>
+          <t>03/12/2023 13:33</t>
         </is>
       </c>
       <c r="R108" t="n">
-        <v>9.9</v>
+        <v>2.14</v>
       </c>
       <c r="S108" t="inlineStr">
         <is>
@@ -10380,16 +10380,16 @@
         </is>
       </c>
       <c r="T108" t="n">
-        <v>14.57</v>
+        <v>2.14</v>
       </c>
       <c r="U108" t="inlineStr">
         <is>
-          <t>03/12/2023 13:50</t>
+          <t>03/12/2023 13:33</t>
         </is>
       </c>
       <c r="V108" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/kalamata-panachaiki/Ct9uxqhn/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/apollon-pontou-karditsa/MJUqLj25/</t>
         </is>
       </c>
     </row>
@@ -10417,22 +10417,22 @@
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>Olympiacos Piraeus B</t>
+          <t>PAOK B</t>
         </is>
       </c>
       <c r="G109" t="n">
+        <v>1</v>
+      </c>
+      <c r="H109" t="inlineStr">
+        <is>
+          <t>Levadiakos</t>
+        </is>
+      </c>
+      <c r="I109" t="n">
         <v>3</v>
       </c>
-      <c r="H109" t="inlineStr">
-        <is>
-          <t>PAE Chania</t>
-        </is>
-      </c>
-      <c r="I109" t="n">
-        <v>0</v>
-      </c>
       <c r="J109" t="n">
-        <v>2.78</v>
+        <v>4.7</v>
       </c>
       <c r="K109" t="inlineStr">
         <is>
@@ -10440,7 +10440,7 @@
         </is>
       </c>
       <c r="L109" t="n">
-        <v>4.33</v>
+        <v>6.1</v>
       </c>
       <c r="M109" t="inlineStr">
         <is>
@@ -10448,7 +10448,7 @@
         </is>
       </c>
       <c r="N109" t="n">
-        <v>2.77</v>
+        <v>3.28</v>
       </c>
       <c r="O109" t="inlineStr">
         <is>
@@ -10456,15 +10456,15 @@
         </is>
       </c>
       <c r="P109" t="n">
-        <v>3.05</v>
+        <v>3.7</v>
       </c>
       <c r="Q109" t="inlineStr">
         <is>
-          <t>03/12/2023 13:50</t>
+          <t>03/12/2023 13:52</t>
         </is>
       </c>
       <c r="R109" t="n">
-        <v>2.6</v>
+        <v>1.7</v>
       </c>
       <c r="S109" t="inlineStr">
         <is>
@@ -10472,16 +10472,16 @@
         </is>
       </c>
       <c r="T109" t="n">
-        <v>1.95</v>
+        <v>1.57</v>
       </c>
       <c r="U109" t="inlineStr">
         <is>
-          <t>03/12/2023 13:50</t>
+          <t>03/12/2023 13:52</t>
         </is>
       </c>
       <c r="V109" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/olympiacos-piraeus-pae-chania/02uNJ1xI/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/paok-levadiakos/z3SXNhIn/</t>
         </is>
       </c>
     </row>
@@ -10509,7 +10509,7 @@
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>Panathinaikos B</t>
+          <t>AEK Athens FC B</t>
         </is>
       </c>
       <c r="G110" t="n">
@@ -10517,14 +10517,14 @@
       </c>
       <c r="H110" t="inlineStr">
         <is>
-          <t>Tilikratis L.</t>
+          <t>Aiolikos</t>
         </is>
       </c>
       <c r="I110" t="n">
         <v>1</v>
       </c>
       <c r="J110" t="n">
-        <v>1.81</v>
+        <v>2.83</v>
       </c>
       <c r="K110" t="inlineStr">
         <is>
@@ -10532,15 +10532,15 @@
         </is>
       </c>
       <c r="L110" t="n">
-        <v>1.6</v>
+        <v>2.43</v>
       </c>
       <c r="M110" t="inlineStr">
         <is>
-          <t>03/12/2023 13:45</t>
+          <t>03/12/2023 13:42</t>
         </is>
       </c>
       <c r="N110" t="n">
-        <v>3.18</v>
+        <v>2.72</v>
       </c>
       <c r="O110" t="inlineStr">
         <is>
@@ -10548,15 +10548,15 @@
         </is>
       </c>
       <c r="P110" t="n">
-        <v>3.87</v>
+        <v>2.98</v>
       </c>
       <c r="Q110" t="inlineStr">
         <is>
-          <t>03/12/2023 13:45</t>
+          <t>03/12/2023 13:42</t>
         </is>
       </c>
       <c r="R110" t="n">
-        <v>4.19</v>
+        <v>2.61</v>
       </c>
       <c r="S110" t="inlineStr">
         <is>
@@ -10564,16 +10564,16 @@
         </is>
       </c>
       <c r="T110" t="n">
-        <v>5.39</v>
+        <v>3.09</v>
       </c>
       <c r="U110" t="inlineStr">
         <is>
-          <t>03/12/2023 13:45</t>
+          <t>03/12/2023 13:42</t>
         </is>
       </c>
       <c r="V110" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/panathinaikos-tilikratis-lefkada/YkAywPxt/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/aek-aiolikos-fc/fiBzPY2t/</t>
         </is>
       </c>
     </row>
@@ -10601,7 +10601,7 @@
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>AEK Athens FC B</t>
+          <t>Giouchtas</t>
         </is>
       </c>
       <c r="G111" t="n">
@@ -10609,14 +10609,14 @@
       </c>
       <c r="H111" t="inlineStr">
         <is>
-          <t>Aiolikos</t>
+          <t>Ionikos</t>
         </is>
       </c>
       <c r="I111" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J111" t="n">
-        <v>2.83</v>
+        <v>3.23</v>
       </c>
       <c r="K111" t="inlineStr">
         <is>
@@ -10624,15 +10624,15 @@
         </is>
       </c>
       <c r="L111" t="n">
-        <v>2.43</v>
+        <v>3.35</v>
       </c>
       <c r="M111" t="inlineStr">
         <is>
-          <t>03/12/2023 13:42</t>
+          <t>03/12/2023 13:39</t>
         </is>
       </c>
       <c r="N111" t="n">
-        <v>2.72</v>
+        <v>2.8</v>
       </c>
       <c r="O111" t="inlineStr">
         <is>
@@ -10640,15 +10640,15 @@
         </is>
       </c>
       <c r="P111" t="n">
-        <v>2.98</v>
+        <v>2.79</v>
       </c>
       <c r="Q111" t="inlineStr">
         <is>
-          <t>03/12/2023 13:42</t>
+          <t>03/12/2023 13:39</t>
         </is>
       </c>
       <c r="R111" t="n">
-        <v>2.61</v>
+        <v>2.28</v>
       </c>
       <c r="S111" t="inlineStr">
         <is>
@@ -10656,16 +10656,16 @@
         </is>
       </c>
       <c r="T111" t="n">
-        <v>3.09</v>
+        <v>2.42</v>
       </c>
       <c r="U111" t="inlineStr">
         <is>
-          <t>03/12/2023 13:42</t>
+          <t>03/12/2023 13:39</t>
         </is>
       </c>
       <c r="V111" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/aek-aiolikos-fc/fiBzPY2t/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/giouchtas-ionikos/YFwVHu7U/</t>
         </is>
       </c>
     </row>
@@ -10693,22 +10693,22 @@
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>AEL Larissa</t>
+          <t>Olympiacos Piraeus B</t>
         </is>
       </c>
       <c r="G112" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H112" t="inlineStr">
         <is>
-          <t>Niki Volos</t>
+          <t>PAE Chania</t>
         </is>
       </c>
       <c r="I112" t="n">
         <v>0</v>
       </c>
       <c r="J112" t="n">
-        <v>1.86</v>
+        <v>2.78</v>
       </c>
       <c r="K112" t="inlineStr">
         <is>
@@ -10716,15 +10716,15 @@
         </is>
       </c>
       <c r="L112" t="n">
-        <v>1.88</v>
+        <v>4.33</v>
       </c>
       <c r="M112" t="inlineStr">
         <is>
-          <t>03/12/2023 13:59</t>
+          <t>03/12/2023 13:52</t>
         </is>
       </c>
       <c r="N112" t="n">
-        <v>2.96</v>
+        <v>2.77</v>
       </c>
       <c r="O112" t="inlineStr">
         <is>
@@ -10732,15 +10732,15 @@
         </is>
       </c>
       <c r="P112" t="n">
-        <v>3.11</v>
+        <v>3.05</v>
       </c>
       <c r="Q112" t="inlineStr">
         <is>
-          <t>03/12/2023 13:59</t>
+          <t>03/12/2023 13:50</t>
         </is>
       </c>
       <c r="R112" t="n">
-        <v>4.28</v>
+        <v>2.6</v>
       </c>
       <c r="S112" t="inlineStr">
         <is>
@@ -10748,16 +10748,16 @@
         </is>
       </c>
       <c r="T112" t="n">
-        <v>4.59</v>
+        <v>1.95</v>
       </c>
       <c r="U112" t="inlineStr">
         <is>
-          <t>03/12/2023 13:59</t>
+          <t>03/12/2023 13:50</t>
         </is>
       </c>
       <c r="V112" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/ael-larissa-niki-volos/8GQuMWna/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/olympiacos-piraeus-pae-chania/02uNJ1xI/</t>
         </is>
       </c>
     </row>
@@ -10785,22 +10785,22 @@
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>Apollon Pontou</t>
+          <t>Kalamata</t>
         </is>
       </c>
       <c r="G113" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H113" t="inlineStr">
         <is>
-          <t>Karditsa</t>
+          <t>Panachaiki</t>
         </is>
       </c>
       <c r="I113" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J113" t="n">
-        <v>3.51</v>
+        <v>1.25</v>
       </c>
       <c r="K113" t="inlineStr">
         <is>
@@ -10808,15 +10808,15 @@
         </is>
       </c>
       <c r="L113" t="n">
-        <v>3.95</v>
+        <v>1.21</v>
       </c>
       <c r="M113" t="inlineStr">
         <is>
-          <t>03/12/2023 13:33</t>
+          <t>03/12/2023 13:50</t>
         </is>
       </c>
       <c r="N113" t="n">
-        <v>2.83</v>
+        <v>5.02</v>
       </c>
       <c r="O113" t="inlineStr">
         <is>
@@ -10824,15 +10824,15 @@
         </is>
       </c>
       <c r="P113" t="n">
-        <v>2.85</v>
+        <v>5.58</v>
       </c>
       <c r="Q113" t="inlineStr">
         <is>
-          <t>03/12/2023 13:33</t>
+          <t>03/12/2023 13:50</t>
         </is>
       </c>
       <c r="R113" t="n">
-        <v>2.14</v>
+        <v>9.9</v>
       </c>
       <c r="S113" t="inlineStr">
         <is>
@@ -10840,16 +10840,16 @@
         </is>
       </c>
       <c r="T113" t="n">
-        <v>2.14</v>
+        <v>14.57</v>
       </c>
       <c r="U113" t="inlineStr">
         <is>
-          <t>03/12/2023 13:33</t>
+          <t>03/12/2023 13:50</t>
         </is>
       </c>
       <c r="V113" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/apollon-pontou-karditsa/MJUqLj25/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/kalamata-panachaiki/Ct9uxqhn/</t>
         </is>
       </c>
     </row>
@@ -10877,71 +10877,71 @@
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>Iraklis 1908</t>
+          <t>Ilioupoli</t>
         </is>
       </c>
       <c r="G114" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H114" t="inlineStr">
         <is>
-          <t>Kozani FC</t>
+          <t>PAE Egaleo</t>
         </is>
       </c>
       <c r="I114" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J114" t="n">
-        <v>1.75</v>
+        <v>2.1</v>
       </c>
       <c r="K114" t="inlineStr">
         <is>
-          <t>02/12/2023 02:13</t>
+          <t>02/12/2023 02:42</t>
         </is>
       </c>
       <c r="L114" t="n">
-        <v>1.91</v>
+        <v>1.85</v>
       </c>
       <c r="M114" t="inlineStr">
         <is>
-          <t>03/12/2023 13:50</t>
+          <t>03/12/2023 13:55</t>
         </is>
       </c>
       <c r="N114" t="n">
-        <v>3.12</v>
+        <v>2.97</v>
       </c>
       <c r="O114" t="inlineStr">
         <is>
-          <t>02/12/2023 02:13</t>
+          <t>02/12/2023 02:42</t>
         </is>
       </c>
       <c r="P114" t="n">
-        <v>3.12</v>
+        <v>3.16</v>
       </c>
       <c r="Q114" t="inlineStr">
         <is>
-          <t>03/12/2023 13:50</t>
+          <t>03/12/2023 13:55</t>
         </is>
       </c>
       <c r="R114" t="n">
-        <v>4.71</v>
+        <v>3.39</v>
       </c>
       <c r="S114" t="inlineStr">
         <is>
-          <t>02/12/2023 02:13</t>
+          <t>02/12/2023 02:42</t>
         </is>
       </c>
       <c r="T114" t="n">
-        <v>4.4</v>
+        <v>4.65</v>
       </c>
       <c r="U114" t="inlineStr">
         <is>
-          <t>03/12/2023 13:50</t>
+          <t>03/12/2023 13:55</t>
         </is>
       </c>
       <c r="V114" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/iraklis-fc-kozani-fc/hrP8TEfP/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/ilioupoli-pae-egaleo/fPvRILiO/</t>
         </is>
       </c>
     </row>
@@ -10969,22 +10969,22 @@
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>PAOK B</t>
+          <t>Panathinaikos B</t>
         </is>
       </c>
       <c r="G115" t="n">
+        <v>2</v>
+      </c>
+      <c r="H115" t="inlineStr">
+        <is>
+          <t>Tilikratis L.</t>
+        </is>
+      </c>
+      <c r="I115" t="n">
         <v>1</v>
       </c>
-      <c r="H115" t="inlineStr">
-        <is>
-          <t>Levadiakos</t>
-        </is>
-      </c>
-      <c r="I115" t="n">
-        <v>3</v>
-      </c>
       <c r="J115" t="n">
-        <v>4.7</v>
+        <v>1.81</v>
       </c>
       <c r="K115" t="inlineStr">
         <is>
@@ -10992,15 +10992,15 @@
         </is>
       </c>
       <c r="L115" t="n">
-        <v>6.1</v>
+        <v>1.6</v>
       </c>
       <c r="M115" t="inlineStr">
         <is>
-          <t>03/12/2023 13:52</t>
+          <t>03/12/2023 13:45</t>
         </is>
       </c>
       <c r="N115" t="n">
-        <v>3.28</v>
+        <v>3.18</v>
       </c>
       <c r="O115" t="inlineStr">
         <is>
@@ -11008,15 +11008,15 @@
         </is>
       </c>
       <c r="P115" t="n">
-        <v>3.7</v>
+        <v>3.87</v>
       </c>
       <c r="Q115" t="inlineStr">
         <is>
-          <t>03/12/2023 13:52</t>
+          <t>03/12/2023 13:45</t>
         </is>
       </c>
       <c r="R115" t="n">
-        <v>1.7</v>
+        <v>4.19</v>
       </c>
       <c r="S115" t="inlineStr">
         <is>
@@ -11024,16 +11024,16 @@
         </is>
       </c>
       <c r="T115" t="n">
-        <v>1.57</v>
+        <v>5.39</v>
       </c>
       <c r="U115" t="inlineStr">
         <is>
-          <t>03/12/2023 13:52</t>
+          <t>03/12/2023 13:45</t>
         </is>
       </c>
       <c r="V115" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/paok-levadiakos/z3SXNhIn/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/panathinaikos-tilikratis-lefkada/YkAywPxt/</t>
         </is>
       </c>
     </row>
@@ -11429,71 +11429,71 @@
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>Karditsa</t>
+          <t>Athens Kallithea</t>
         </is>
       </c>
       <c r="G120" t="n">
+        <v>1</v>
+      </c>
+      <c r="H120" t="inlineStr">
+        <is>
+          <t>Kalamata</t>
+        </is>
+      </c>
+      <c r="I120" t="n">
         <v>0</v>
       </c>
-      <c r="H120" t="inlineStr">
-        <is>
-          <t>Kampaniakos</t>
-        </is>
-      </c>
-      <c r="I120" t="n">
-        <v>1</v>
-      </c>
       <c r="J120" t="n">
-        <v>1.59</v>
+        <v>1.81</v>
       </c>
       <c r="K120" t="inlineStr">
         <is>
-          <t>09/12/2023 02:13</t>
+          <t>09/12/2023 02:12</t>
         </is>
       </c>
       <c r="L120" t="n">
-        <v>1.78</v>
+        <v>2.1</v>
       </c>
       <c r="M120" t="inlineStr">
         <is>
-          <t>10/12/2023 13:57</t>
+          <t>10/12/2023 13:38</t>
         </is>
       </c>
       <c r="N120" t="n">
-        <v>3.45</v>
+        <v>2.99</v>
       </c>
       <c r="O120" t="inlineStr">
         <is>
-          <t>09/12/2023 02:13</t>
+          <t>09/12/2023 02:12</t>
         </is>
       </c>
       <c r="P120" t="n">
-        <v>3.23</v>
+        <v>2.86</v>
       </c>
       <c r="Q120" t="inlineStr">
         <is>
-          <t>10/12/2023 13:57</t>
+          <t>10/12/2023 13:38</t>
         </is>
       </c>
       <c r="R120" t="n">
-        <v>5.3</v>
+        <v>4.56</v>
       </c>
       <c r="S120" t="inlineStr">
         <is>
-          <t>09/12/2023 02:13</t>
+          <t>09/12/2023 02:12</t>
         </is>
       </c>
       <c r="T120" t="n">
-        <v>5.01</v>
+        <v>4.09</v>
       </c>
       <c r="U120" t="inlineStr">
         <is>
-          <t>10/12/2023 13:57</t>
+          <t>10/12/2023 13:38</t>
         </is>
       </c>
       <c r="V120" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/karditsa-kampaniakos/jwP8P5gi/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/athens-kallithea-kalamata/8KYRfH7p/</t>
         </is>
       </c>
     </row>
@@ -11521,71 +11521,71 @@
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>Aiolikos</t>
+          <t>Tilikratis L.</t>
         </is>
       </c>
       <c r="G121" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H121" t="inlineStr">
         <is>
-          <t>Iraklis 1908</t>
+          <t>Giouchtas</t>
         </is>
       </c>
       <c r="I121" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J121" t="n">
-        <v>2.99</v>
+        <v>3.25</v>
       </c>
       <c r="K121" t="inlineStr">
         <is>
-          <t>09/12/2023 02:12</t>
+          <t>09/12/2023 02:13</t>
         </is>
       </c>
       <c r="L121" t="n">
-        <v>3.46</v>
+        <v>3.21</v>
       </c>
       <c r="M121" t="inlineStr">
         <is>
-          <t>10/12/2023 13:58</t>
+          <t>10/12/2023 13:17</t>
         </is>
       </c>
       <c r="N121" t="n">
-        <v>2.76</v>
+        <v>2.94</v>
       </c>
       <c r="O121" t="inlineStr">
         <is>
-          <t>09/12/2023 02:12</t>
+          <t>09/12/2023 02:13</t>
         </is>
       </c>
       <c r="P121" t="n">
-        <v>3.02</v>
+        <v>3.03</v>
       </c>
       <c r="Q121" t="inlineStr">
         <is>
-          <t>10/12/2023 13:58</t>
+          <t>10/12/2023 13:17</t>
         </is>
       </c>
       <c r="R121" t="n">
-        <v>2.44</v>
+        <v>2.18</v>
       </c>
       <c r="S121" t="inlineStr">
         <is>
-          <t>09/12/2023 02:12</t>
+          <t>09/12/2023 02:13</t>
         </is>
       </c>
       <c r="T121" t="n">
-        <v>2.21</v>
+        <v>2.33</v>
       </c>
       <c r="U121" t="inlineStr">
         <is>
-          <t>10/12/2023 13:58</t>
+          <t>10/12/2023 13:17</t>
         </is>
       </c>
       <c r="V121" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/aiolikos-fc-iraklis-fc/rZIhJUWH/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/tilikratis-lefkada-giouchtas/nwxes3fR/</t>
         </is>
       </c>
     </row>
@@ -11613,7 +11613,7 @@
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>Athens Kallithea</t>
+          <t>Aiolikos</t>
         </is>
       </c>
       <c r="G122" t="n">
@@ -11621,14 +11621,14 @@
       </c>
       <c r="H122" t="inlineStr">
         <is>
-          <t>Kalamata</t>
+          <t>Iraklis 1908</t>
         </is>
       </c>
       <c r="I122" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J122" t="n">
-        <v>1.81</v>
+        <v>2.99</v>
       </c>
       <c r="K122" t="inlineStr">
         <is>
@@ -11636,15 +11636,15 @@
         </is>
       </c>
       <c r="L122" t="n">
-        <v>2.1</v>
+        <v>3.46</v>
       </c>
       <c r="M122" t="inlineStr">
         <is>
-          <t>10/12/2023 13:38</t>
+          <t>10/12/2023 13:58</t>
         </is>
       </c>
       <c r="N122" t="n">
-        <v>2.99</v>
+        <v>2.76</v>
       </c>
       <c r="O122" t="inlineStr">
         <is>
@@ -11652,15 +11652,15 @@
         </is>
       </c>
       <c r="P122" t="n">
-        <v>2.86</v>
+        <v>3.02</v>
       </c>
       <c r="Q122" t="inlineStr">
         <is>
-          <t>10/12/2023 13:38</t>
+          <t>10/12/2023 13:58</t>
         </is>
       </c>
       <c r="R122" t="n">
-        <v>4.56</v>
+        <v>2.44</v>
       </c>
       <c r="S122" t="inlineStr">
         <is>
@@ -11668,16 +11668,16 @@
         </is>
       </c>
       <c r="T122" t="n">
-        <v>4.09</v>
+        <v>2.21</v>
       </c>
       <c r="U122" t="inlineStr">
         <is>
-          <t>10/12/2023 13:38</t>
+          <t>10/12/2023 13:58</t>
         </is>
       </c>
       <c r="V122" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/athens-kallithea-kalamata/8KYRfH7p/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/aiolikos-fc-iraklis-fc/rZIhJUWH/</t>
         </is>
       </c>
     </row>
@@ -11705,7 +11705,7 @@
       </c>
       <c r="F123" t="inlineStr">
         <is>
-          <t>Tilikratis L.</t>
+          <t>Karditsa</t>
         </is>
       </c>
       <c r="G123" t="n">
@@ -11713,14 +11713,14 @@
       </c>
       <c r="H123" t="inlineStr">
         <is>
-          <t>Giouchtas</t>
+          <t>Kampaniakos</t>
         </is>
       </c>
       <c r="I123" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J123" t="n">
-        <v>3.25</v>
+        <v>1.59</v>
       </c>
       <c r="K123" t="inlineStr">
         <is>
@@ -11728,15 +11728,15 @@
         </is>
       </c>
       <c r="L123" t="n">
-        <v>3.21</v>
+        <v>1.78</v>
       </c>
       <c r="M123" t="inlineStr">
         <is>
-          <t>10/12/2023 13:17</t>
+          <t>10/12/2023 13:57</t>
         </is>
       </c>
       <c r="N123" t="n">
-        <v>2.94</v>
+        <v>3.45</v>
       </c>
       <c r="O123" t="inlineStr">
         <is>
@@ -11744,15 +11744,15 @@
         </is>
       </c>
       <c r="P123" t="n">
-        <v>3.03</v>
+        <v>3.23</v>
       </c>
       <c r="Q123" t="inlineStr">
         <is>
-          <t>10/12/2023 13:17</t>
+          <t>10/12/2023 13:57</t>
         </is>
       </c>
       <c r="R123" t="n">
-        <v>2.18</v>
+        <v>5.3</v>
       </c>
       <c r="S123" t="inlineStr">
         <is>
@@ -11760,16 +11760,16 @@
         </is>
       </c>
       <c r="T123" t="n">
-        <v>2.33</v>
+        <v>5.01</v>
       </c>
       <c r="U123" t="inlineStr">
         <is>
-          <t>10/12/2023 13:17</t>
+          <t>10/12/2023 13:57</t>
         </is>
       </c>
       <c r="V123" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/tilikratis-lefkada-giouchtas/nwxes3fR/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/karditsa-kampaniakos/jwP8P5gi/</t>
         </is>
       </c>
     </row>
@@ -11797,7 +11797,7 @@
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>AEL Larissa</t>
+          <t>Niki Volos</t>
         </is>
       </c>
       <c r="G124" t="n">
@@ -11805,14 +11805,14 @@
       </c>
       <c r="H124" t="inlineStr">
         <is>
-          <t>Apollon Pontou</t>
+          <t>PAOK B</t>
         </is>
       </c>
       <c r="I124" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J124" t="n">
-        <v>1.19</v>
+        <v>1.57</v>
       </c>
       <c r="K124" t="inlineStr">
         <is>
@@ -11820,15 +11820,15 @@
         </is>
       </c>
       <c r="L124" t="n">
-        <v>1.18</v>
+        <v>1.5</v>
       </c>
       <c r="M124" t="inlineStr">
         <is>
-          <t>11/12/2023 13:57</t>
+          <t>11/12/2023 13:51</t>
         </is>
       </c>
       <c r="N124" t="n">
-        <v>5.42</v>
+        <v>3.5</v>
       </c>
       <c r="O124" t="inlineStr">
         <is>
@@ -11836,15 +11836,15 @@
         </is>
       </c>
       <c r="P124" t="n">
-        <v>6.03</v>
+        <v>3.83</v>
       </c>
       <c r="Q124" t="inlineStr">
         <is>
-          <t>11/12/2023 13:57</t>
+          <t>11/12/2023 13:58</t>
         </is>
       </c>
       <c r="R124" t="n">
-        <v>11.94</v>
+        <v>5.09</v>
       </c>
       <c r="S124" t="inlineStr">
         <is>
@@ -11852,16 +11852,16 @@
         </is>
       </c>
       <c r="T124" t="n">
-        <v>16.47</v>
+        <v>7</v>
       </c>
       <c r="U124" t="inlineStr">
         <is>
-          <t>11/12/2023 13:57</t>
+          <t>11/12/2023 13:58</t>
         </is>
       </c>
       <c r="V124" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/ael-larissa-apollon-pontou/lOsCOP8c/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/niki-volos-paok/lYpQ0MGj/</t>
         </is>
       </c>
     </row>
@@ -11889,7 +11889,7 @@
       </c>
       <c r="F125" t="inlineStr">
         <is>
-          <t>Niki Volos</t>
+          <t>AEL Larissa</t>
         </is>
       </c>
       <c r="G125" t="n">
@@ -11897,14 +11897,14 @@
       </c>
       <c r="H125" t="inlineStr">
         <is>
-          <t>PAOK B</t>
+          <t>Apollon Pontou</t>
         </is>
       </c>
       <c r="I125" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J125" t="n">
-        <v>1.57</v>
+        <v>1.19</v>
       </c>
       <c r="K125" t="inlineStr">
         <is>
@@ -11912,15 +11912,15 @@
         </is>
       </c>
       <c r="L125" t="n">
-        <v>1.5</v>
+        <v>1.18</v>
       </c>
       <c r="M125" t="inlineStr">
         <is>
-          <t>11/12/2023 13:51</t>
+          <t>11/12/2023 13:57</t>
         </is>
       </c>
       <c r="N125" t="n">
-        <v>3.5</v>
+        <v>5.42</v>
       </c>
       <c r="O125" t="inlineStr">
         <is>
@@ -11928,15 +11928,15 @@
         </is>
       </c>
       <c r="P125" t="n">
-        <v>3.83</v>
+        <v>6.03</v>
       </c>
       <c r="Q125" t="inlineStr">
         <is>
-          <t>11/12/2023 13:58</t>
+          <t>11/12/2023 13:57</t>
         </is>
       </c>
       <c r="R125" t="n">
-        <v>5.09</v>
+        <v>11.94</v>
       </c>
       <c r="S125" t="inlineStr">
         <is>
@@ -11944,16 +11944,16 @@
         </is>
       </c>
       <c r="T125" t="n">
-        <v>7</v>
+        <v>16.47</v>
       </c>
       <c r="U125" t="inlineStr">
         <is>
-          <t>11/12/2023 13:58</t>
+          <t>11/12/2023 13:57</t>
         </is>
       </c>
       <c r="V125" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/niki-volos-paok/lYpQ0MGj/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/ael-larissa-apollon-pontou/lOsCOP8c/</t>
         </is>
       </c>
     </row>
@@ -12165,7 +12165,7 @@
       </c>
       <c r="F128" t="inlineStr">
         <is>
-          <t>Kampaniakos</t>
+          <t>Ilioupoli</t>
         </is>
       </c>
       <c r="G128" t="n">
@@ -12173,14 +12173,14 @@
       </c>
       <c r="H128" t="inlineStr">
         <is>
-          <t>AEL Larissa</t>
+          <t>Olympiacos Piraeus B</t>
         </is>
       </c>
       <c r="I128" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J128" t="n">
-        <v>6.83</v>
+        <v>2.57</v>
       </c>
       <c r="K128" t="inlineStr">
         <is>
@@ -12188,7 +12188,7 @@
         </is>
       </c>
       <c r="L128" t="n">
-        <v>9.07</v>
+        <v>2.27</v>
       </c>
       <c r="M128" t="inlineStr">
         <is>
@@ -12196,7 +12196,7 @@
         </is>
       </c>
       <c r="N128" t="n">
-        <v>3.73</v>
+        <v>2.75</v>
       </c>
       <c r="O128" t="inlineStr">
         <is>
@@ -12204,7 +12204,7 @@
         </is>
       </c>
       <c r="P128" t="n">
-        <v>4.29</v>
+        <v>2.86</v>
       </c>
       <c r="Q128" t="inlineStr">
         <is>
@@ -12212,7 +12212,7 @@
         </is>
       </c>
       <c r="R128" t="n">
-        <v>1.45</v>
+        <v>2.84</v>
       </c>
       <c r="S128" t="inlineStr">
         <is>
@@ -12220,16 +12220,16 @@
         </is>
       </c>
       <c r="T128" t="n">
-        <v>1.38</v>
+        <v>3.56</v>
       </c>
       <c r="U128" t="inlineStr">
         <is>
-          <t>16/12/2023 13:50</t>
+          <t>16/12/2023 13:57</t>
         </is>
       </c>
       <c r="V128" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/kampaniakos-ael-larissa/lnQbFLVq/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/ilioupoli-olympiacos-piraeus/Y9Y9xAR3/</t>
         </is>
       </c>
     </row>
@@ -12257,7 +12257,7 @@
       </c>
       <c r="F129" t="inlineStr">
         <is>
-          <t>Ilioupoli</t>
+          <t>Kalamata</t>
         </is>
       </c>
       <c r="G129" t="n">
@@ -12265,14 +12265,14 @@
       </c>
       <c r="H129" t="inlineStr">
         <is>
-          <t>Olympiacos Piraeus B</t>
+          <t>Panathinaikos B</t>
         </is>
       </c>
       <c r="I129" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J129" t="n">
-        <v>2.57</v>
+        <v>1.25</v>
       </c>
       <c r="K129" t="inlineStr">
         <is>
@@ -12280,15 +12280,15 @@
         </is>
       </c>
       <c r="L129" t="n">
-        <v>2.27</v>
+        <v>1.23</v>
       </c>
       <c r="M129" t="inlineStr">
         <is>
-          <t>16/12/2023 13:57</t>
+          <t>16/12/2023 13:59</t>
         </is>
       </c>
       <c r="N129" t="n">
-        <v>2.75</v>
+        <v>4.89</v>
       </c>
       <c r="O129" t="inlineStr">
         <is>
@@ -12296,15 +12296,15 @@
         </is>
       </c>
       <c r="P129" t="n">
-        <v>2.86</v>
+        <v>5.6</v>
       </c>
       <c r="Q129" t="inlineStr">
         <is>
-          <t>16/12/2023 13:57</t>
+          <t>16/12/2023 13:59</t>
         </is>
       </c>
       <c r="R129" t="n">
-        <v>2.84</v>
+        <v>10.18</v>
       </c>
       <c r="S129" t="inlineStr">
         <is>
@@ -12312,16 +12312,16 @@
         </is>
       </c>
       <c r="T129" t="n">
-        <v>3.56</v>
+        <v>11.89</v>
       </c>
       <c r="U129" t="inlineStr">
         <is>
-          <t>16/12/2023 13:57</t>
+          <t>16/12/2023 13:59</t>
         </is>
       </c>
       <c r="V129" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/ilioupoli-olympiacos-piraeus/Y9Y9xAR3/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/kalamata-panathinaikos/KQzMZ7BM/</t>
         </is>
       </c>
     </row>
@@ -12349,7 +12349,7 @@
       </c>
       <c r="F130" t="inlineStr">
         <is>
-          <t>Kalamata</t>
+          <t>Kampaniakos</t>
         </is>
       </c>
       <c r="G130" t="n">
@@ -12357,14 +12357,14 @@
       </c>
       <c r="H130" t="inlineStr">
         <is>
-          <t>Panathinaikos B</t>
+          <t>AEL Larissa</t>
         </is>
       </c>
       <c r="I130" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J130" t="n">
-        <v>1.25</v>
+        <v>6.83</v>
       </c>
       <c r="K130" t="inlineStr">
         <is>
@@ -12372,15 +12372,15 @@
         </is>
       </c>
       <c r="L130" t="n">
-        <v>1.23</v>
+        <v>9.07</v>
       </c>
       <c r="M130" t="inlineStr">
         <is>
-          <t>16/12/2023 13:59</t>
+          <t>16/12/2023 13:57</t>
         </is>
       </c>
       <c r="N130" t="n">
-        <v>4.89</v>
+        <v>3.73</v>
       </c>
       <c r="O130" t="inlineStr">
         <is>
@@ -12388,15 +12388,15 @@
         </is>
       </c>
       <c r="P130" t="n">
-        <v>5.6</v>
+        <v>4.29</v>
       </c>
       <c r="Q130" t="inlineStr">
         <is>
-          <t>16/12/2023 13:59</t>
+          <t>16/12/2023 13:57</t>
         </is>
       </c>
       <c r="R130" t="n">
-        <v>10.18</v>
+        <v>1.45</v>
       </c>
       <c r="S130" t="inlineStr">
         <is>
@@ -12404,16 +12404,16 @@
         </is>
       </c>
       <c r="T130" t="n">
-        <v>11.89</v>
+        <v>1.38</v>
       </c>
       <c r="U130" t="inlineStr">
         <is>
-          <t>16/12/2023 13:59</t>
+          <t>16/12/2023 13:50</t>
         </is>
       </c>
       <c r="V130" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/kalamata-panathinaikos/KQzMZ7BM/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/kampaniakos-ael-larissa/lnQbFLVq/</t>
         </is>
       </c>
     </row>
@@ -13150,6 +13150,282 @@
       <c r="V138" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/greece/super-league-2/pae-chania-ionikos/6NWHzldG/</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="1" t="n">
+        <v>138</v>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>greece</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>super-league-2</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E139" s="2" t="n">
+        <v>45294.58333333334</v>
+      </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>Kozani FC</t>
+        </is>
+      </c>
+      <c r="G139" t="n">
+        <v>0</v>
+      </c>
+      <c r="H139" t="inlineStr">
+        <is>
+          <t>Levadiakos</t>
+        </is>
+      </c>
+      <c r="I139" t="n">
+        <v>0</v>
+      </c>
+      <c r="J139" t="n">
+        <v>5.26</v>
+      </c>
+      <c r="K139" t="inlineStr">
+        <is>
+          <t>02/01/2024 03:12</t>
+        </is>
+      </c>
+      <c r="L139" t="n">
+        <v>5.66</v>
+      </c>
+      <c r="M139" t="inlineStr">
+        <is>
+          <t>03/01/2024 13:03</t>
+        </is>
+      </c>
+      <c r="N139" t="n">
+        <v>3.18</v>
+      </c>
+      <c r="O139" t="inlineStr">
+        <is>
+          <t>02/01/2024 03:12</t>
+        </is>
+      </c>
+      <c r="P139" t="n">
+        <v>3.17</v>
+      </c>
+      <c r="Q139" t="inlineStr">
+        <is>
+          <t>03/01/2024 12:54</t>
+        </is>
+      </c>
+      <c r="R139" t="n">
+        <v>1.66</v>
+      </c>
+      <c r="S139" t="inlineStr">
+        <is>
+          <t>02/01/2024 03:12</t>
+        </is>
+      </c>
+      <c r="T139" t="n">
+        <v>1.73</v>
+      </c>
+      <c r="U139" t="inlineStr">
+        <is>
+          <t>03/01/2024 13:03</t>
+        </is>
+      </c>
+      <c r="V139" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/kozani-fc-levadiakos/A1E7Da0d/</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="1" t="n">
+        <v>139</v>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>greece</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>super-league-2</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E140" s="2" t="n">
+        <v>45294.58333333334</v>
+      </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>Karditsa</t>
+        </is>
+      </c>
+      <c r="G140" t="n">
+        <v>2</v>
+      </c>
+      <c r="H140" t="inlineStr">
+        <is>
+          <t>Iraklis 1908</t>
+        </is>
+      </c>
+      <c r="I140" t="n">
+        <v>1</v>
+      </c>
+      <c r="J140" t="n">
+        <v>2.86</v>
+      </c>
+      <c r="K140" t="inlineStr">
+        <is>
+          <t>02/01/2024 03:12</t>
+        </is>
+      </c>
+      <c r="L140" t="n">
+        <v>3.39</v>
+      </c>
+      <c r="M140" t="inlineStr">
+        <is>
+          <t>03/01/2024 13:59</t>
+        </is>
+      </c>
+      <c r="N140" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="O140" t="inlineStr">
+        <is>
+          <t>02/01/2024 03:12</t>
+        </is>
+      </c>
+      <c r="P140" t="n">
+        <v>2.42</v>
+      </c>
+      <c r="Q140" t="inlineStr">
+        <is>
+          <t>03/01/2024 13:58</t>
+        </is>
+      </c>
+      <c r="R140" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="S140" t="inlineStr">
+        <is>
+          <t>02/01/2024 03:12</t>
+        </is>
+      </c>
+      <c r="T140" t="n">
+        <v>2.75</v>
+      </c>
+      <c r="U140" t="inlineStr">
+        <is>
+          <t>03/01/2024 13:58</t>
+        </is>
+      </c>
+      <c r="V140" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/karditsa-iraklis-fc/Gb1gy3h3/</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>greece</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>super-league-2</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E141" s="2" t="n">
+        <v>45294.58333333334</v>
+      </c>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>Makedonikos</t>
+        </is>
+      </c>
+      <c r="G141" t="n">
+        <v>1</v>
+      </c>
+      <c r="H141" t="inlineStr">
+        <is>
+          <t>Aiolikos</t>
+        </is>
+      </c>
+      <c r="I141" t="n">
+        <v>1</v>
+      </c>
+      <c r="J141" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="K141" t="inlineStr">
+        <is>
+          <t>02/01/2024 03:12</t>
+        </is>
+      </c>
+      <c r="L141" t="n">
+        <v>2.02</v>
+      </c>
+      <c r="M141" t="inlineStr">
+        <is>
+          <t>03/01/2024 13:59</t>
+        </is>
+      </c>
+      <c r="N141" t="n">
+        <v>3.08</v>
+      </c>
+      <c r="O141" t="inlineStr">
+        <is>
+          <t>02/01/2024 03:12</t>
+        </is>
+      </c>
+      <c r="P141" t="n">
+        <v>3.13</v>
+      </c>
+      <c r="Q141" t="inlineStr">
+        <is>
+          <t>03/01/2024 13:59</t>
+        </is>
+      </c>
+      <c r="R141" t="n">
+        <v>4.42</v>
+      </c>
+      <c r="S141" t="inlineStr">
+        <is>
+          <t>02/01/2024 03:12</t>
+        </is>
+      </c>
+      <c r="T141" t="n">
+        <v>3.89</v>
+      </c>
+      <c r="U141" t="inlineStr">
+        <is>
+          <t>03/01/2024 13:59</t>
+        </is>
+      </c>
+      <c r="V141" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/makedonikos-neapolis-aiolikos-fc/x82kxqwc/</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualizado por script em 04-01-2024 14:45
</commit_message>
<xml_diff>
--- a/2023/greece_super-league-2_2023-2024.xlsx
+++ b/2023/greece_super-league-2_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V141"/>
+  <dimension ref="A1:V143"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6737,22 +6737,22 @@
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>Kampaniakos</t>
+          <t>Apollon Pontou</t>
         </is>
       </c>
       <c r="G69" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Kozani FC</t>
+          <t>AEK Athens FC B</t>
         </is>
       </c>
       <c r="I69" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J69" t="n">
-        <v>2.61</v>
+        <v>2.52</v>
       </c>
       <c r="K69" t="inlineStr">
         <is>
@@ -6760,15 +6760,15 @@
         </is>
       </c>
       <c r="L69" t="n">
-        <v>2.94</v>
+        <v>3.36</v>
       </c>
       <c r="M69" t="inlineStr">
         <is>
-          <t>11/11/2023 13:03</t>
+          <t>11/11/2023 13:49</t>
         </is>
       </c>
       <c r="N69" t="n">
-        <v>2.87</v>
+        <v>2.82</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
@@ -6776,15 +6776,15 @@
         </is>
       </c>
       <c r="P69" t="n">
-        <v>2.79</v>
+        <v>2.73</v>
       </c>
       <c r="Q69" t="inlineStr">
         <is>
-          <t>11/11/2023 13:03</t>
+          <t>11/11/2023 13:49</t>
         </is>
       </c>
       <c r="R69" t="n">
-        <v>2.61</v>
+        <v>2.83</v>
       </c>
       <c r="S69" t="inlineStr">
         <is>
@@ -6792,16 +6792,16 @@
         </is>
       </c>
       <c r="T69" t="n">
-        <v>2.68</v>
+        <v>2.45</v>
       </c>
       <c r="U69" t="inlineStr">
         <is>
-          <t>11/11/2023 13:03</t>
+          <t>11/11/2023 13:49</t>
         </is>
       </c>
       <c r="V69" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/kampaniakos-kozani-fc/xCUYMtcm/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/apollon-pontou-aek/APStLKRa/</t>
         </is>
       </c>
     </row>
@@ -6829,22 +6829,22 @@
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>Apollon Pontou</t>
+          <t>Kampaniakos</t>
         </is>
       </c>
       <c r="G70" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>AEK Athens FC B</t>
+          <t>Kozani FC</t>
         </is>
       </c>
       <c r="I70" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J70" t="n">
-        <v>2.52</v>
+        <v>2.61</v>
       </c>
       <c r="K70" t="inlineStr">
         <is>
@@ -6852,15 +6852,15 @@
         </is>
       </c>
       <c r="L70" t="n">
-        <v>3.36</v>
+        <v>2.94</v>
       </c>
       <c r="M70" t="inlineStr">
         <is>
-          <t>11/11/2023 13:49</t>
+          <t>11/11/2023 13:03</t>
         </is>
       </c>
       <c r="N70" t="n">
-        <v>2.82</v>
+        <v>2.87</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
@@ -6868,15 +6868,15 @@
         </is>
       </c>
       <c r="P70" t="n">
-        <v>2.73</v>
+        <v>2.79</v>
       </c>
       <c r="Q70" t="inlineStr">
         <is>
-          <t>11/11/2023 13:49</t>
+          <t>11/11/2023 13:03</t>
         </is>
       </c>
       <c r="R70" t="n">
-        <v>2.83</v>
+        <v>2.61</v>
       </c>
       <c r="S70" t="inlineStr">
         <is>
@@ -6884,16 +6884,16 @@
         </is>
       </c>
       <c r="T70" t="n">
-        <v>2.45</v>
+        <v>2.68</v>
       </c>
       <c r="U70" t="inlineStr">
         <is>
-          <t>11/11/2023 13:49</t>
+          <t>11/11/2023 13:03</t>
         </is>
       </c>
       <c r="V70" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/apollon-pontou-aek/APStLKRa/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/kampaniakos-kozani-fc/xCUYMtcm/</t>
         </is>
       </c>
     </row>
@@ -7657,22 +7657,22 @@
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>Iraklis 1908</t>
+          <t>Makedonikos</t>
         </is>
       </c>
       <c r="G79" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Apollon Pontou</t>
+          <t>Levadiakos</t>
         </is>
       </c>
       <c r="I79" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J79" t="n">
-        <v>1.3</v>
+        <v>3.73</v>
       </c>
       <c r="K79" t="inlineStr">
         <is>
@@ -7680,15 +7680,15 @@
         </is>
       </c>
       <c r="L79" t="n">
-        <v>1.42</v>
+        <v>5.2</v>
       </c>
       <c r="M79" t="inlineStr">
         <is>
-          <t>15/11/2023 12:58</t>
+          <t>15/11/2023 13:31</t>
         </is>
       </c>
       <c r="N79" t="n">
-        <v>4.59</v>
+        <v>2.94</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
@@ -7696,15 +7696,15 @@
         </is>
       </c>
       <c r="P79" t="n">
-        <v>4.2</v>
+        <v>3.1</v>
       </c>
       <c r="Q79" t="inlineStr">
         <is>
-          <t>15/11/2023 12:58</t>
+          <t>15/11/2023 13:49</t>
         </is>
       </c>
       <c r="R79" t="n">
-        <v>7.84</v>
+        <v>1.97</v>
       </c>
       <c r="S79" t="inlineStr">
         <is>
@@ -7712,16 +7712,16 @@
         </is>
       </c>
       <c r="T79" t="n">
-        <v>7.94</v>
+        <v>1.78</v>
       </c>
       <c r="U79" t="inlineStr">
         <is>
-          <t>15/11/2023 12:58</t>
+          <t>15/11/2023 13:11</t>
         </is>
       </c>
       <c r="V79" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/iraklis-fc-apollon-pontou/0UPRezZg/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/makedonikos-neapolis-levadiakos/ddJzfE36/</t>
         </is>
       </c>
     </row>
@@ -7749,7 +7749,7 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>Aiolikos</t>
+          <t>Iraklis 1908</t>
         </is>
       </c>
       <c r="G80" t="n">
@@ -7757,63 +7757,63 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Niki Volos</t>
+          <t>Apollon Pontou</t>
         </is>
       </c>
       <c r="I80" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J80" t="n">
-        <v>4.13</v>
+        <v>1.3</v>
       </c>
       <c r="K80" t="inlineStr">
         <is>
-          <t>14/11/2023 15:18</t>
+          <t>14/11/2023 02:12</t>
         </is>
       </c>
       <c r="L80" t="n">
-        <v>3.66</v>
+        <v>1.42</v>
       </c>
       <c r="M80" t="inlineStr">
         <is>
-          <t>15/11/2023 13:38</t>
+          <t>15/11/2023 12:58</t>
         </is>
       </c>
       <c r="N80" t="n">
-        <v>3.43</v>
+        <v>4.59</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>14/11/2023 15:18</t>
+          <t>14/11/2023 02:12</t>
         </is>
       </c>
       <c r="P80" t="n">
-        <v>3.18</v>
+        <v>4.2</v>
       </c>
       <c r="Q80" t="inlineStr">
         <is>
-          <t>15/11/2023 12:23</t>
+          <t>15/11/2023 12:58</t>
         </is>
       </c>
       <c r="R80" t="n">
-        <v>1.83</v>
+        <v>7.84</v>
       </c>
       <c r="S80" t="inlineStr">
         <is>
-          <t>14/11/2023 15:18</t>
+          <t>14/11/2023 02:12</t>
         </is>
       </c>
       <c r="T80" t="n">
-        <v>2.07</v>
+        <v>7.94</v>
       </c>
       <c r="U80" t="inlineStr">
         <is>
-          <t>15/11/2023 13:38</t>
+          <t>15/11/2023 12:58</t>
         </is>
       </c>
       <c r="V80" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/aiolikos-fc-niki-volos/rgFWffl0/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/iraklis-fc-apollon-pontou/0UPRezZg/</t>
         </is>
       </c>
     </row>
@@ -7841,71 +7841,71 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>Makedonikos</t>
+          <t>Aiolikos</t>
         </is>
       </c>
       <c r="G81" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Levadiakos</t>
+          <t>Niki Volos</t>
         </is>
       </c>
       <c r="I81" t="n">
         <v>2</v>
       </c>
       <c r="J81" t="n">
-        <v>3.73</v>
+        <v>4.13</v>
       </c>
       <c r="K81" t="inlineStr">
         <is>
-          <t>14/11/2023 02:12</t>
+          <t>14/11/2023 15:18</t>
         </is>
       </c>
       <c r="L81" t="n">
-        <v>5.2</v>
+        <v>3.66</v>
       </c>
       <c r="M81" t="inlineStr">
         <is>
-          <t>15/11/2023 13:31</t>
+          <t>15/11/2023 13:38</t>
         </is>
       </c>
       <c r="N81" t="n">
-        <v>2.94</v>
+        <v>3.43</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>14/11/2023 02:12</t>
+          <t>14/11/2023 15:18</t>
         </is>
       </c>
       <c r="P81" t="n">
-        <v>3.1</v>
+        <v>3.18</v>
       </c>
       <c r="Q81" t="inlineStr">
         <is>
-          <t>15/11/2023 13:49</t>
+          <t>15/11/2023 12:23</t>
         </is>
       </c>
       <c r="R81" t="n">
-        <v>1.97</v>
+        <v>1.83</v>
       </c>
       <c r="S81" t="inlineStr">
         <is>
-          <t>14/11/2023 02:12</t>
+          <t>14/11/2023 15:18</t>
         </is>
       </c>
       <c r="T81" t="n">
-        <v>1.78</v>
+        <v>2.07</v>
       </c>
       <c r="U81" t="inlineStr">
         <is>
-          <t>15/11/2023 13:11</t>
+          <t>15/11/2023 13:38</t>
         </is>
       </c>
       <c r="V81" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/makedonikos-neapolis-levadiakos/ddJzfE36/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/aiolikos-fc-niki-volos/rgFWffl0/</t>
         </is>
       </c>
     </row>
@@ -8025,22 +8025,22 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>Tilikratis L.</t>
+          <t>Giouchtas</t>
         </is>
       </c>
       <c r="G83" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Panachaiki</t>
+          <t>PAE Chania</t>
         </is>
       </c>
       <c r="I83" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J83" t="n">
-        <v>2.27</v>
+        <v>3.28</v>
       </c>
       <c r="K83" t="inlineStr">
         <is>
@@ -8048,15 +8048,15 @@
         </is>
       </c>
       <c r="L83" t="n">
-        <v>2.31</v>
+        <v>3.93</v>
       </c>
       <c r="M83" t="inlineStr">
         <is>
-          <t>19/11/2023 13:54</t>
+          <t>19/11/2023 13:14</t>
         </is>
       </c>
       <c r="N83" t="n">
-        <v>2.92</v>
+        <v>2.86</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
@@ -8064,15 +8064,15 @@
         </is>
       </c>
       <c r="P83" t="n">
-        <v>2.95</v>
+        <v>3.05</v>
       </c>
       <c r="Q83" t="inlineStr">
         <is>
-          <t>19/11/2023 13:54</t>
+          <t>19/11/2023 12:51</t>
         </is>
       </c>
       <c r="R83" t="n">
-        <v>3.02</v>
+        <v>2.17</v>
       </c>
       <c r="S83" t="inlineStr">
         <is>
@@ -8080,16 +8080,16 @@
         </is>
       </c>
       <c r="T83" t="n">
-        <v>3.35</v>
+        <v>2.04</v>
       </c>
       <c r="U83" t="inlineStr">
         <is>
-          <t>19/11/2023 13:51</t>
+          <t>19/11/2023 13:14</t>
         </is>
       </c>
       <c r="V83" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/tilikratis-lefkada-panachaiki/rZYSo9JE/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/giouchtas-pae-chania/4rzPnk48/</t>
         </is>
       </c>
     </row>
@@ -8117,22 +8117,22 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>Kalamata</t>
+          <t>Ionikos</t>
         </is>
       </c>
       <c r="G84" t="n">
+        <v>0</v>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>Athens Kallithea</t>
+        </is>
+      </c>
+      <c r="I84" t="n">
         <v>1</v>
       </c>
-      <c r="H84" t="inlineStr">
-        <is>
-          <t>Diagoras</t>
-        </is>
-      </c>
-      <c r="I84" t="n">
-        <v>2</v>
-      </c>
       <c r="J84" t="n">
-        <v>1.3</v>
+        <v>3.12</v>
       </c>
       <c r="K84" t="inlineStr">
         <is>
@@ -8140,15 +8140,15 @@
         </is>
       </c>
       <c r="L84" t="n">
-        <v>1.26</v>
+        <v>2.89</v>
       </c>
       <c r="M84" t="inlineStr">
         <is>
-          <t>19/11/2023 13:49</t>
+          <t>19/11/2023 13:29</t>
         </is>
       </c>
       <c r="N84" t="n">
-        <v>4.57</v>
+        <v>2.85</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
@@ -8156,15 +8156,15 @@
         </is>
       </c>
       <c r="P84" t="n">
-        <v>5.23</v>
+        <v>2.91</v>
       </c>
       <c r="Q84" t="inlineStr">
         <is>
-          <t>19/11/2023 13:56</t>
+          <t>19/11/2023 13:29</t>
         </is>
       </c>
       <c r="R84" t="n">
-        <v>8.08</v>
+        <v>2.26</v>
       </c>
       <c r="S84" t="inlineStr">
         <is>
@@ -8172,16 +8172,16 @@
         </is>
       </c>
       <c r="T84" t="n">
-        <v>12.07</v>
+        <v>2.62</v>
       </c>
       <c r="U84" t="inlineStr">
         <is>
-          <t>19/11/2023 13:56</t>
+          <t>19/11/2023 13:29</t>
         </is>
       </c>
       <c r="V84" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/kalamata-diagoras-fc/xxnsO5R7/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/ionikos-athens-kallithea/v1SypmlR/</t>
         </is>
       </c>
     </row>
@@ -8209,71 +8209,71 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>Apollon Pontou</t>
+          <t>Kalamata</t>
         </is>
       </c>
       <c r="G85" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>Aiolikos</t>
+          <t>Diagoras</t>
         </is>
       </c>
       <c r="I85" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J85" t="n">
-        <v>2.77</v>
+        <v>1.3</v>
       </c>
       <c r="K85" t="inlineStr">
         <is>
-          <t>19/11/2023 03:12</t>
+          <t>18/11/2023 02:12</t>
         </is>
       </c>
       <c r="L85" t="n">
-        <v>2.89</v>
+        <v>1.26</v>
       </c>
       <c r="M85" t="inlineStr">
         <is>
-          <t>19/11/2023 13:41</t>
+          <t>19/11/2023 13:49</t>
         </is>
       </c>
       <c r="N85" t="n">
-        <v>2.87</v>
+        <v>4.57</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
-          <t>19/11/2023 03:12</t>
+          <t>18/11/2023 02:12</t>
         </is>
       </c>
       <c r="P85" t="n">
-        <v>2.85</v>
+        <v>5.23</v>
       </c>
       <c r="Q85" t="inlineStr">
         <is>
-          <t>19/11/2023 13:24</t>
+          <t>19/11/2023 13:56</t>
         </is>
       </c>
       <c r="R85" t="n">
-        <v>2.65</v>
+        <v>8.08</v>
       </c>
       <c r="S85" t="inlineStr">
         <is>
-          <t>19/11/2023 03:12</t>
+          <t>18/11/2023 02:12</t>
         </is>
       </c>
       <c r="T85" t="n">
-        <v>2.67</v>
+        <v>12.07</v>
       </c>
       <c r="U85" t="inlineStr">
         <is>
-          <t>19/11/2023 13:41</t>
+          <t>19/11/2023 13:56</t>
         </is>
       </c>
       <c r="V85" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/apollon-pontou-aiolikos-fc/pIaVFeQP/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/kalamata-diagoras-fc/xxnsO5R7/</t>
         </is>
       </c>
     </row>
@@ -8301,22 +8301,22 @@
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>Giouchtas</t>
+          <t>Tilikratis L.</t>
         </is>
       </c>
       <c r="G86" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>PAE Chania</t>
+          <t>Panachaiki</t>
         </is>
       </c>
       <c r="I86" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J86" t="n">
-        <v>3.28</v>
+        <v>2.27</v>
       </c>
       <c r="K86" t="inlineStr">
         <is>
@@ -8324,15 +8324,15 @@
         </is>
       </c>
       <c r="L86" t="n">
-        <v>3.93</v>
+        <v>2.31</v>
       </c>
       <c r="M86" t="inlineStr">
         <is>
-          <t>19/11/2023 13:14</t>
+          <t>19/11/2023 13:54</t>
         </is>
       </c>
       <c r="N86" t="n">
-        <v>2.86</v>
+        <v>2.92</v>
       </c>
       <c r="O86" t="inlineStr">
         <is>
@@ -8340,15 +8340,15 @@
         </is>
       </c>
       <c r="P86" t="n">
-        <v>3.05</v>
+        <v>2.95</v>
       </c>
       <c r="Q86" t="inlineStr">
         <is>
-          <t>19/11/2023 12:51</t>
+          <t>19/11/2023 13:54</t>
         </is>
       </c>
       <c r="R86" t="n">
-        <v>2.17</v>
+        <v>3.02</v>
       </c>
       <c r="S86" t="inlineStr">
         <is>
@@ -8356,16 +8356,16 @@
         </is>
       </c>
       <c r="T86" t="n">
-        <v>2.04</v>
+        <v>3.35</v>
       </c>
       <c r="U86" t="inlineStr">
         <is>
-          <t>19/11/2023 13:14</t>
+          <t>19/11/2023 13:51</t>
         </is>
       </c>
       <c r="V86" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/giouchtas-pae-chania/4rzPnk48/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/tilikratis-lefkada-panachaiki/rZYSo9JE/</t>
         </is>
       </c>
     </row>
@@ -8393,71 +8393,71 @@
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>Kampaniakos</t>
+          <t>Apollon Pontou</t>
         </is>
       </c>
       <c r="G87" t="n">
+        <v>0</v>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>Aiolikos</t>
+        </is>
+      </c>
+      <c r="I87" t="n">
         <v>1</v>
       </c>
-      <c r="H87" t="inlineStr">
-        <is>
-          <t>Iraklis 1908</t>
-        </is>
-      </c>
-      <c r="I87" t="n">
-        <v>3</v>
-      </c>
       <c r="J87" t="n">
-        <v>3.87</v>
+        <v>2.77</v>
       </c>
       <c r="K87" t="inlineStr">
         <is>
-          <t>18/11/2023 02:12</t>
+          <t>19/11/2023 03:12</t>
         </is>
       </c>
       <c r="L87" t="n">
-        <v>4.12</v>
+        <v>2.89</v>
       </c>
       <c r="M87" t="inlineStr">
         <is>
-          <t>19/11/2023 12:04</t>
+          <t>19/11/2023 13:41</t>
         </is>
       </c>
       <c r="N87" t="n">
-        <v>3.15</v>
+        <v>2.87</v>
       </c>
       <c r="O87" t="inlineStr">
         <is>
-          <t>18/11/2023 02:12</t>
+          <t>19/11/2023 03:12</t>
         </is>
       </c>
       <c r="P87" t="n">
-        <v>3.11</v>
+        <v>2.85</v>
       </c>
       <c r="Q87" t="inlineStr">
         <is>
-          <t>19/11/2023 12:52</t>
+          <t>19/11/2023 13:24</t>
         </is>
       </c>
       <c r="R87" t="n">
-        <v>1.85</v>
+        <v>2.65</v>
       </c>
       <c r="S87" t="inlineStr">
         <is>
-          <t>18/11/2023 02:12</t>
+          <t>19/11/2023 03:12</t>
         </is>
       </c>
       <c r="T87" t="n">
-        <v>1.97</v>
+        <v>2.67</v>
       </c>
       <c r="U87" t="inlineStr">
         <is>
-          <t>19/11/2023 12:52</t>
+          <t>19/11/2023 13:41</t>
         </is>
       </c>
       <c r="V87" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/kampaniakos-iraklis-fc/6R0RGyBJ/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/apollon-pontou-aiolikos-fc/pIaVFeQP/</t>
         </is>
       </c>
     </row>
@@ -8485,22 +8485,22 @@
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>Ionikos</t>
+          <t>Kampaniakos</t>
         </is>
       </c>
       <c r="G88" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>Athens Kallithea</t>
+          <t>Iraklis 1908</t>
         </is>
       </c>
       <c r="I88" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J88" t="n">
-        <v>3.12</v>
+        <v>3.87</v>
       </c>
       <c r="K88" t="inlineStr">
         <is>
@@ -8508,15 +8508,15 @@
         </is>
       </c>
       <c r="L88" t="n">
-        <v>2.89</v>
+        <v>4.12</v>
       </c>
       <c r="M88" t="inlineStr">
         <is>
-          <t>19/11/2023 13:29</t>
+          <t>19/11/2023 12:04</t>
         </is>
       </c>
       <c r="N88" t="n">
-        <v>2.85</v>
+        <v>3.15</v>
       </c>
       <c r="O88" t="inlineStr">
         <is>
@@ -8524,15 +8524,15 @@
         </is>
       </c>
       <c r="P88" t="n">
-        <v>2.91</v>
+        <v>3.11</v>
       </c>
       <c r="Q88" t="inlineStr">
         <is>
-          <t>19/11/2023 13:29</t>
+          <t>19/11/2023 12:52</t>
         </is>
       </c>
       <c r="R88" t="n">
-        <v>2.26</v>
+        <v>1.85</v>
       </c>
       <c r="S88" t="inlineStr">
         <is>
@@ -8540,16 +8540,16 @@
         </is>
       </c>
       <c r="T88" t="n">
-        <v>2.62</v>
+        <v>1.97</v>
       </c>
       <c r="U88" t="inlineStr">
         <is>
-          <t>19/11/2023 13:29</t>
+          <t>19/11/2023 12:52</t>
         </is>
       </c>
       <c r="V88" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/ionikos-athens-kallithea/v1SypmlR/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/kampaniakos-iraklis-fc/6R0RGyBJ/</t>
         </is>
       </c>
     </row>
@@ -8761,22 +8761,22 @@
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>Athens Kallithea</t>
+          <t>Iraklis 1908</t>
         </is>
       </c>
       <c r="G91" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>Tilikratis L.</t>
+          <t>AEK Athens FC B</t>
         </is>
       </c>
       <c r="I91" t="n">
         <v>0</v>
       </c>
       <c r="J91" t="n">
-        <v>1.16</v>
+        <v>1.5</v>
       </c>
       <c r="K91" t="inlineStr">
         <is>
@@ -8784,15 +8784,15 @@
         </is>
       </c>
       <c r="L91" t="n">
-        <v>1.11</v>
+        <v>1.67</v>
       </c>
       <c r="M91" t="inlineStr">
         <is>
-          <t>25/11/2023 13:09</t>
+          <t>25/11/2023 13:45</t>
         </is>
       </c>
       <c r="N91" t="n">
-        <v>6.22</v>
+        <v>3.67</v>
       </c>
       <c r="O91" t="inlineStr">
         <is>
@@ -8800,15 +8800,15 @@
         </is>
       </c>
       <c r="P91" t="n">
-        <v>8.289999999999999</v>
+        <v>3.53</v>
       </c>
       <c r="Q91" t="inlineStr">
         <is>
-          <t>25/11/2023 13:10</t>
+          <t>25/11/2023 13:45</t>
         </is>
       </c>
       <c r="R91" t="n">
-        <v>12.53</v>
+        <v>5.66</v>
       </c>
       <c r="S91" t="inlineStr">
         <is>
@@ -8816,16 +8816,16 @@
         </is>
       </c>
       <c r="T91" t="n">
-        <v>23.73</v>
+        <v>5.3</v>
       </c>
       <c r="U91" t="inlineStr">
         <is>
-          <t>25/11/2023 13:10</t>
+          <t>25/11/2023 13:45</t>
         </is>
       </c>
       <c r="V91" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/athens-kallithea-tilikratis-lefkada/QL6KyPe7/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/iraklis-fc-aek/zmvA8DIa/</t>
         </is>
       </c>
     </row>
@@ -8945,22 +8945,22 @@
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>Iraklis 1908</t>
+          <t>Athens Kallithea</t>
         </is>
       </c>
       <c r="G93" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H93" t="inlineStr">
         <is>
-          <t>AEK Athens FC B</t>
+          <t>Tilikratis L.</t>
         </is>
       </c>
       <c r="I93" t="n">
         <v>0</v>
       </c>
       <c r="J93" t="n">
-        <v>1.5</v>
+        <v>1.16</v>
       </c>
       <c r="K93" t="inlineStr">
         <is>
@@ -8968,15 +8968,15 @@
         </is>
       </c>
       <c r="L93" t="n">
-        <v>1.67</v>
+        <v>1.11</v>
       </c>
       <c r="M93" t="inlineStr">
         <is>
-          <t>25/11/2023 13:45</t>
+          <t>25/11/2023 13:09</t>
         </is>
       </c>
       <c r="N93" t="n">
-        <v>3.67</v>
+        <v>6.22</v>
       </c>
       <c r="O93" t="inlineStr">
         <is>
@@ -8984,15 +8984,15 @@
         </is>
       </c>
       <c r="P93" t="n">
-        <v>3.53</v>
+        <v>8.289999999999999</v>
       </c>
       <c r="Q93" t="inlineStr">
         <is>
-          <t>25/11/2023 13:45</t>
+          <t>25/11/2023 13:10</t>
         </is>
       </c>
       <c r="R93" t="n">
-        <v>5.66</v>
+        <v>12.53</v>
       </c>
       <c r="S93" t="inlineStr">
         <is>
@@ -9000,16 +9000,16 @@
         </is>
       </c>
       <c r="T93" t="n">
-        <v>5.3</v>
+        <v>23.73</v>
       </c>
       <c r="U93" t="inlineStr">
         <is>
-          <t>25/11/2023 13:45</t>
+          <t>25/11/2023 13:10</t>
         </is>
       </c>
       <c r="V93" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/iraklis-fc-aek/zmvA8DIa/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/athens-kallithea-tilikratis-lefkada/QL6KyPe7/</t>
         </is>
       </c>
     </row>
@@ -9129,22 +9129,22 @@
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>Ilioupoli</t>
+          <t>Makedonikos</t>
         </is>
       </c>
       <c r="G95" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H95" t="inlineStr">
         <is>
-          <t>Giouchtas</t>
+          <t>Apollon Pontou</t>
         </is>
       </c>
       <c r="I95" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J95" t="n">
-        <v>1.97</v>
+        <v>1.53</v>
       </c>
       <c r="K95" t="inlineStr">
         <is>
@@ -9152,48 +9152,48 @@
         </is>
       </c>
       <c r="L95" t="n">
-        <v>2.19</v>
+        <v>1.54</v>
       </c>
       <c r="M95" t="inlineStr">
         <is>
+          <t>26/11/2023 13:44</t>
+        </is>
+      </c>
+      <c r="N95" t="n">
+        <v>3.51</v>
+      </c>
+      <c r="O95" t="inlineStr">
+        <is>
+          <t>25/11/2023 02:12</t>
+        </is>
+      </c>
+      <c r="P95" t="n">
+        <v>3.65</v>
+      </c>
+      <c r="Q95" t="inlineStr">
+        <is>
           <t>26/11/2023 13:59</t>
         </is>
       </c>
-      <c r="N95" t="n">
-        <v>3.02</v>
-      </c>
-      <c r="O95" t="inlineStr">
+      <c r="R95" t="n">
+        <v>5.58</v>
+      </c>
+      <c r="S95" t="inlineStr">
         <is>
           <t>25/11/2023 02:12</t>
         </is>
       </c>
-      <c r="P95" t="n">
-        <v>3.19</v>
-      </c>
-      <c r="Q95" t="inlineStr">
+      <c r="T95" t="n">
+        <v>6.81</v>
+      </c>
+      <c r="U95" t="inlineStr">
         <is>
           <t>26/11/2023 13:59</t>
         </is>
       </c>
-      <c r="R95" t="n">
-        <v>3.62</v>
-      </c>
-      <c r="S95" t="inlineStr">
-        <is>
-          <t>25/11/2023 02:12</t>
-        </is>
-      </c>
-      <c r="T95" t="n">
-        <v>3.32</v>
-      </c>
-      <c r="U95" t="inlineStr">
-        <is>
-          <t>26/11/2023 13:59</t>
-        </is>
-      </c>
       <c r="V95" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/ilioupoli-giouchtas/Wb7Gx5t1/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/makedonikos-neapolis-apollon-pontou/QyXM5B2I/</t>
         </is>
       </c>
     </row>
@@ -9221,22 +9221,22 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>PAE Chania</t>
+          <t>Ilioupoli</t>
         </is>
       </c>
       <c r="G96" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>PAE Egaleo</t>
+          <t>Giouchtas</t>
         </is>
       </c>
       <c r="I96" t="n">
         <v>0</v>
       </c>
       <c r="J96" t="n">
-        <v>1.55</v>
+        <v>1.97</v>
       </c>
       <c r="K96" t="inlineStr">
         <is>
@@ -9244,15 +9244,15 @@
         </is>
       </c>
       <c r="L96" t="n">
-        <v>1.2</v>
+        <v>2.19</v>
       </c>
       <c r="M96" t="inlineStr">
         <is>
-          <t>26/11/2023 13:55</t>
+          <t>26/11/2023 13:59</t>
         </is>
       </c>
       <c r="N96" t="n">
-        <v>3.48</v>
+        <v>3.02</v>
       </c>
       <c r="O96" t="inlineStr">
         <is>
@@ -9260,15 +9260,15 @@
         </is>
       </c>
       <c r="P96" t="n">
-        <v>6.56</v>
+        <v>3.19</v>
       </c>
       <c r="Q96" t="inlineStr">
         <is>
-          <t>26/11/2023 13:58</t>
+          <t>26/11/2023 13:59</t>
         </is>
       </c>
       <c r="R96" t="n">
-        <v>5.44</v>
+        <v>3.62</v>
       </c>
       <c r="S96" t="inlineStr">
         <is>
@@ -9276,16 +9276,16 @@
         </is>
       </c>
       <c r="T96" t="n">
-        <v>11.76</v>
+        <v>3.32</v>
       </c>
       <c r="U96" t="inlineStr">
         <is>
-          <t>26/11/2023 13:58</t>
+          <t>26/11/2023 13:59</t>
         </is>
       </c>
       <c r="V96" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/pae-chania-pae-egaleo/zXD7vRBl/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/ilioupoli-giouchtas/Wb7Gx5t1/</t>
         </is>
       </c>
     </row>
@@ -9405,7 +9405,7 @@
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>Karditsa</t>
+          <t>PAE Chania</t>
         </is>
       </c>
       <c r="G98" t="n">
@@ -9413,14 +9413,14 @@
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t>Niki Volos</t>
+          <t>PAE Egaleo</t>
         </is>
       </c>
       <c r="I98" t="n">
         <v>0</v>
       </c>
       <c r="J98" t="n">
-        <v>3.26</v>
+        <v>1.55</v>
       </c>
       <c r="K98" t="inlineStr">
         <is>
@@ -9428,15 +9428,15 @@
         </is>
       </c>
       <c r="L98" t="n">
-        <v>3.72</v>
+        <v>1.2</v>
       </c>
       <c r="M98" t="inlineStr">
         <is>
-          <t>26/11/2023 13:46</t>
+          <t>26/11/2023 13:55</t>
         </is>
       </c>
       <c r="N98" t="n">
-        <v>2.83</v>
+        <v>3.48</v>
       </c>
       <c r="O98" t="inlineStr">
         <is>
@@ -9444,15 +9444,15 @@
         </is>
       </c>
       <c r="P98" t="n">
-        <v>2.91</v>
+        <v>6.56</v>
       </c>
       <c r="Q98" t="inlineStr">
         <is>
-          <t>26/11/2023 13:46</t>
+          <t>26/11/2023 13:58</t>
         </is>
       </c>
       <c r="R98" t="n">
-        <v>2.2</v>
+        <v>5.44</v>
       </c>
       <c r="S98" t="inlineStr">
         <is>
@@ -9460,16 +9460,16 @@
         </is>
       </c>
       <c r="T98" t="n">
-        <v>2.18</v>
+        <v>11.76</v>
       </c>
       <c r="U98" t="inlineStr">
         <is>
-          <t>26/11/2023 13:46</t>
+          <t>26/11/2023 13:58</t>
         </is>
       </c>
       <c r="V98" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/karditsa-niki-volos/vuyR4VHO/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/pae-chania-pae-egaleo/zXD7vRBl/</t>
         </is>
       </c>
     </row>
@@ -9497,22 +9497,22 @@
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>Makedonikos</t>
+          <t>Karditsa</t>
         </is>
       </c>
       <c r="G99" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>Apollon Pontou</t>
+          <t>Niki Volos</t>
         </is>
       </c>
       <c r="I99" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J99" t="n">
-        <v>1.53</v>
+        <v>3.26</v>
       </c>
       <c r="K99" t="inlineStr">
         <is>
@@ -9520,15 +9520,15 @@
         </is>
       </c>
       <c r="L99" t="n">
-        <v>1.54</v>
+        <v>3.72</v>
       </c>
       <c r="M99" t="inlineStr">
         <is>
-          <t>26/11/2023 13:44</t>
+          <t>26/11/2023 13:46</t>
         </is>
       </c>
       <c r="N99" t="n">
-        <v>3.51</v>
+        <v>2.83</v>
       </c>
       <c r="O99" t="inlineStr">
         <is>
@@ -9536,15 +9536,15 @@
         </is>
       </c>
       <c r="P99" t="n">
-        <v>3.65</v>
+        <v>2.91</v>
       </c>
       <c r="Q99" t="inlineStr">
         <is>
-          <t>26/11/2023 13:59</t>
+          <t>26/11/2023 13:46</t>
         </is>
       </c>
       <c r="R99" t="n">
-        <v>5.58</v>
+        <v>2.2</v>
       </c>
       <c r="S99" t="inlineStr">
         <is>
@@ -9552,16 +9552,16 @@
         </is>
       </c>
       <c r="T99" t="n">
-        <v>6.81</v>
+        <v>2.18</v>
       </c>
       <c r="U99" t="inlineStr">
         <is>
-          <t>26/11/2023 13:59</t>
+          <t>26/11/2023 13:46</t>
         </is>
       </c>
       <c r="V99" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/makedonikos-neapolis-apollon-pontou/QyXM5B2I/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/karditsa-niki-volos/vuyR4VHO/</t>
         </is>
       </c>
     </row>
@@ -10325,22 +10325,22 @@
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>Apollon Pontou</t>
+          <t>PAOK B</t>
         </is>
       </c>
       <c r="G108" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H108" t="inlineStr">
         <is>
-          <t>Karditsa</t>
+          <t>Levadiakos</t>
         </is>
       </c>
       <c r="I108" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J108" t="n">
-        <v>3.51</v>
+        <v>4.7</v>
       </c>
       <c r="K108" t="inlineStr">
         <is>
@@ -10348,15 +10348,15 @@
         </is>
       </c>
       <c r="L108" t="n">
-        <v>3.95</v>
+        <v>6.1</v>
       </c>
       <c r="M108" t="inlineStr">
         <is>
-          <t>03/12/2023 13:33</t>
+          <t>03/12/2023 13:52</t>
         </is>
       </c>
       <c r="N108" t="n">
-        <v>2.83</v>
+        <v>3.28</v>
       </c>
       <c r="O108" t="inlineStr">
         <is>
@@ -10364,15 +10364,15 @@
         </is>
       </c>
       <c r="P108" t="n">
-        <v>2.85</v>
+        <v>3.7</v>
       </c>
       <c r="Q108" t="inlineStr">
         <is>
-          <t>03/12/2023 13:33</t>
+          <t>03/12/2023 13:52</t>
         </is>
       </c>
       <c r="R108" t="n">
-        <v>2.14</v>
+        <v>1.7</v>
       </c>
       <c r="S108" t="inlineStr">
         <is>
@@ -10380,16 +10380,16 @@
         </is>
       </c>
       <c r="T108" t="n">
-        <v>2.14</v>
+        <v>1.57</v>
       </c>
       <c r="U108" t="inlineStr">
         <is>
-          <t>03/12/2023 13:33</t>
+          <t>03/12/2023 13:52</t>
         </is>
       </c>
       <c r="V108" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/apollon-pontou-karditsa/MJUqLj25/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/paok-levadiakos/z3SXNhIn/</t>
         </is>
       </c>
     </row>
@@ -10417,22 +10417,22 @@
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>PAOK B</t>
+          <t>Apollon Pontou</t>
         </is>
       </c>
       <c r="G109" t="n">
+        <v>2</v>
+      </c>
+      <c r="H109" t="inlineStr">
+        <is>
+          <t>Karditsa</t>
+        </is>
+      </c>
+      <c r="I109" t="n">
         <v>1</v>
       </c>
-      <c r="H109" t="inlineStr">
-        <is>
-          <t>Levadiakos</t>
-        </is>
-      </c>
-      <c r="I109" t="n">
-        <v>3</v>
-      </c>
       <c r="J109" t="n">
-        <v>4.7</v>
+        <v>3.51</v>
       </c>
       <c r="K109" t="inlineStr">
         <is>
@@ -10440,15 +10440,15 @@
         </is>
       </c>
       <c r="L109" t="n">
-        <v>6.1</v>
+        <v>3.95</v>
       </c>
       <c r="M109" t="inlineStr">
         <is>
-          <t>03/12/2023 13:52</t>
+          <t>03/12/2023 13:33</t>
         </is>
       </c>
       <c r="N109" t="n">
-        <v>3.28</v>
+        <v>2.83</v>
       </c>
       <c r="O109" t="inlineStr">
         <is>
@@ -10456,15 +10456,15 @@
         </is>
       </c>
       <c r="P109" t="n">
-        <v>3.7</v>
+        <v>2.85</v>
       </c>
       <c r="Q109" t="inlineStr">
         <is>
-          <t>03/12/2023 13:52</t>
+          <t>03/12/2023 13:33</t>
         </is>
       </c>
       <c r="R109" t="n">
-        <v>1.7</v>
+        <v>2.14</v>
       </c>
       <c r="S109" t="inlineStr">
         <is>
@@ -10472,16 +10472,16 @@
         </is>
       </c>
       <c r="T109" t="n">
-        <v>1.57</v>
+        <v>2.14</v>
       </c>
       <c r="U109" t="inlineStr">
         <is>
-          <t>03/12/2023 13:52</t>
+          <t>03/12/2023 13:33</t>
         </is>
       </c>
       <c r="V109" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/paok-levadiakos/z3SXNhIn/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/apollon-pontou-karditsa/MJUqLj25/</t>
         </is>
       </c>
     </row>
@@ -10601,7 +10601,7 @@
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>Giouchtas</t>
+          <t>Ilioupoli</t>
         </is>
       </c>
       <c r="G111" t="n">
@@ -10609,63 +10609,63 @@
       </c>
       <c r="H111" t="inlineStr">
         <is>
-          <t>Ionikos</t>
+          <t>PAE Egaleo</t>
         </is>
       </c>
       <c r="I111" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J111" t="n">
-        <v>3.23</v>
+        <v>2.1</v>
       </c>
       <c r="K111" t="inlineStr">
         <is>
-          <t>02/12/2023 02:13</t>
+          <t>02/12/2023 02:42</t>
         </is>
       </c>
       <c r="L111" t="n">
-        <v>3.35</v>
+        <v>1.85</v>
       </c>
       <c r="M111" t="inlineStr">
         <is>
-          <t>03/12/2023 13:39</t>
+          <t>03/12/2023 13:55</t>
         </is>
       </c>
       <c r="N111" t="n">
-        <v>2.8</v>
+        <v>2.97</v>
       </c>
       <c r="O111" t="inlineStr">
         <is>
-          <t>02/12/2023 02:13</t>
+          <t>02/12/2023 02:42</t>
         </is>
       </c>
       <c r="P111" t="n">
-        <v>2.79</v>
+        <v>3.16</v>
       </c>
       <c r="Q111" t="inlineStr">
         <is>
-          <t>03/12/2023 13:39</t>
+          <t>03/12/2023 13:55</t>
         </is>
       </c>
       <c r="R111" t="n">
-        <v>2.28</v>
+        <v>3.39</v>
       </c>
       <c r="S111" t="inlineStr">
         <is>
-          <t>02/12/2023 02:13</t>
+          <t>02/12/2023 02:42</t>
         </is>
       </c>
       <c r="T111" t="n">
-        <v>2.42</v>
+        <v>4.65</v>
       </c>
       <c r="U111" t="inlineStr">
         <is>
-          <t>03/12/2023 13:39</t>
+          <t>03/12/2023 13:55</t>
         </is>
       </c>
       <c r="V111" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/giouchtas-ionikos/YFwVHu7U/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/ilioupoli-pae-egaleo/fPvRILiO/</t>
         </is>
       </c>
     </row>
@@ -10877,7 +10877,7 @@
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>Ilioupoli</t>
+          <t>Giouchtas</t>
         </is>
       </c>
       <c r="G114" t="n">
@@ -10885,63 +10885,63 @@
       </c>
       <c r="H114" t="inlineStr">
         <is>
-          <t>PAE Egaleo</t>
+          <t>Ionikos</t>
         </is>
       </c>
       <c r="I114" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J114" t="n">
-        <v>2.1</v>
+        <v>3.23</v>
       </c>
       <c r="K114" t="inlineStr">
         <is>
-          <t>02/12/2023 02:42</t>
+          <t>02/12/2023 02:13</t>
         </is>
       </c>
       <c r="L114" t="n">
-        <v>1.85</v>
+        <v>3.35</v>
       </c>
       <c r="M114" t="inlineStr">
         <is>
-          <t>03/12/2023 13:55</t>
+          <t>03/12/2023 13:39</t>
         </is>
       </c>
       <c r="N114" t="n">
-        <v>2.97</v>
+        <v>2.8</v>
       </c>
       <c r="O114" t="inlineStr">
         <is>
-          <t>02/12/2023 02:42</t>
+          <t>02/12/2023 02:13</t>
         </is>
       </c>
       <c r="P114" t="n">
-        <v>3.16</v>
+        <v>2.79</v>
       </c>
       <c r="Q114" t="inlineStr">
         <is>
-          <t>03/12/2023 13:55</t>
+          <t>03/12/2023 13:39</t>
         </is>
       </c>
       <c r="R114" t="n">
-        <v>3.39</v>
+        <v>2.28</v>
       </c>
       <c r="S114" t="inlineStr">
         <is>
-          <t>02/12/2023 02:42</t>
+          <t>02/12/2023 02:13</t>
         </is>
       </c>
       <c r="T114" t="n">
-        <v>4.65</v>
+        <v>2.42</v>
       </c>
       <c r="U114" t="inlineStr">
         <is>
-          <t>03/12/2023 13:55</t>
+          <t>03/12/2023 13:39</t>
         </is>
       </c>
       <c r="V114" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/ilioupoli-pae-egaleo/fPvRILiO/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/giouchtas-ionikos/YFwVHu7U/</t>
         </is>
       </c>
     </row>
@@ -11797,7 +11797,7 @@
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>Niki Volos</t>
+          <t>AEL Larissa</t>
         </is>
       </c>
       <c r="G124" t="n">
@@ -11805,14 +11805,14 @@
       </c>
       <c r="H124" t="inlineStr">
         <is>
-          <t>PAOK B</t>
+          <t>Apollon Pontou</t>
         </is>
       </c>
       <c r="I124" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J124" t="n">
-        <v>1.57</v>
+        <v>1.19</v>
       </c>
       <c r="K124" t="inlineStr">
         <is>
@@ -11820,15 +11820,15 @@
         </is>
       </c>
       <c r="L124" t="n">
-        <v>1.5</v>
+        <v>1.18</v>
       </c>
       <c r="M124" t="inlineStr">
         <is>
-          <t>11/12/2023 13:51</t>
+          <t>11/12/2023 13:57</t>
         </is>
       </c>
       <c r="N124" t="n">
-        <v>3.5</v>
+        <v>5.42</v>
       </c>
       <c r="O124" t="inlineStr">
         <is>
@@ -11836,15 +11836,15 @@
         </is>
       </c>
       <c r="P124" t="n">
-        <v>3.83</v>
+        <v>6.03</v>
       </c>
       <c r="Q124" t="inlineStr">
         <is>
-          <t>11/12/2023 13:58</t>
+          <t>11/12/2023 13:57</t>
         </is>
       </c>
       <c r="R124" t="n">
-        <v>5.09</v>
+        <v>11.94</v>
       </c>
       <c r="S124" t="inlineStr">
         <is>
@@ -11852,16 +11852,16 @@
         </is>
       </c>
       <c r="T124" t="n">
-        <v>7</v>
+        <v>16.47</v>
       </c>
       <c r="U124" t="inlineStr">
         <is>
-          <t>11/12/2023 13:58</t>
+          <t>11/12/2023 13:57</t>
         </is>
       </c>
       <c r="V124" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/niki-volos-paok/lYpQ0MGj/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/ael-larissa-apollon-pontou/lOsCOP8c/</t>
         </is>
       </c>
     </row>
@@ -11889,7 +11889,7 @@
       </c>
       <c r="F125" t="inlineStr">
         <is>
-          <t>AEL Larissa</t>
+          <t>Niki Volos</t>
         </is>
       </c>
       <c r="G125" t="n">
@@ -11897,14 +11897,14 @@
       </c>
       <c r="H125" t="inlineStr">
         <is>
-          <t>Apollon Pontou</t>
+          <t>PAOK B</t>
         </is>
       </c>
       <c r="I125" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J125" t="n">
-        <v>1.19</v>
+        <v>1.57</v>
       </c>
       <c r="K125" t="inlineStr">
         <is>
@@ -11912,15 +11912,15 @@
         </is>
       </c>
       <c r="L125" t="n">
-        <v>1.18</v>
+        <v>1.5</v>
       </c>
       <c r="M125" t="inlineStr">
         <is>
-          <t>11/12/2023 13:57</t>
+          <t>11/12/2023 13:51</t>
         </is>
       </c>
       <c r="N125" t="n">
-        <v>5.42</v>
+        <v>3.5</v>
       </c>
       <c r="O125" t="inlineStr">
         <is>
@@ -11928,15 +11928,15 @@
         </is>
       </c>
       <c r="P125" t="n">
-        <v>6.03</v>
+        <v>3.83</v>
       </c>
       <c r="Q125" t="inlineStr">
         <is>
-          <t>11/12/2023 13:57</t>
+          <t>11/12/2023 13:58</t>
         </is>
       </c>
       <c r="R125" t="n">
-        <v>11.94</v>
+        <v>5.09</v>
       </c>
       <c r="S125" t="inlineStr">
         <is>
@@ -11944,16 +11944,16 @@
         </is>
       </c>
       <c r="T125" t="n">
-        <v>16.47</v>
+        <v>7</v>
       </c>
       <c r="U125" t="inlineStr">
         <is>
-          <t>11/12/2023 13:57</t>
+          <t>11/12/2023 13:58</t>
         </is>
       </c>
       <c r="V125" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/ael-larissa-apollon-pontou/lOsCOP8c/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/niki-volos-paok/lYpQ0MGj/</t>
         </is>
       </c>
     </row>
@@ -11981,22 +11981,22 @@
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>Ionikos</t>
+          <t>AEK Athens FC B</t>
         </is>
       </c>
       <c r="G126" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H126" t="inlineStr">
         <is>
-          <t>PAE Egaleo</t>
+          <t>Kozani FC</t>
         </is>
       </c>
       <c r="I126" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J126" t="n">
-        <v>1.6</v>
+        <v>2.66</v>
       </c>
       <c r="K126" t="inlineStr">
         <is>
@@ -12004,15 +12004,15 @@
         </is>
       </c>
       <c r="L126" t="n">
-        <v>1.54</v>
+        <v>2.21</v>
       </c>
       <c r="M126" t="inlineStr">
         <is>
-          <t>13/12/2023 13:59</t>
+          <t>13/12/2023 13:54</t>
         </is>
       </c>
       <c r="N126" t="n">
-        <v>3.43</v>
+        <v>2.69</v>
       </c>
       <c r="O126" t="inlineStr">
         <is>
@@ -12020,15 +12020,15 @@
         </is>
       </c>
       <c r="P126" t="n">
-        <v>3.8</v>
+        <v>2.59</v>
       </c>
       <c r="Q126" t="inlineStr">
         <is>
-          <t>13/12/2023 13:59</t>
+          <t>13/12/2023 13:54</t>
         </is>
       </c>
       <c r="R126" t="n">
-        <v>5.27</v>
+        <v>2.79</v>
       </c>
       <c r="S126" t="inlineStr">
         <is>
@@ -12036,16 +12036,16 @@
         </is>
       </c>
       <c r="T126" t="n">
-        <v>5.17</v>
+        <v>4.29</v>
       </c>
       <c r="U126" t="inlineStr">
         <is>
-          <t>13/12/2023 13:59</t>
+          <t>13/12/2023 13:54</t>
         </is>
       </c>
       <c r="V126" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/ionikos-pae-egaleo/QNmnqPPE/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/aek-kozani-fc/U9HrhhYI/</t>
         </is>
       </c>
     </row>
@@ -12073,22 +12073,22 @@
       </c>
       <c r="F127" t="inlineStr">
         <is>
-          <t>AEK Athens FC B</t>
+          <t>Ionikos</t>
         </is>
       </c>
       <c r="G127" t="n">
+        <v>5</v>
+      </c>
+      <c r="H127" t="inlineStr">
+        <is>
+          <t>PAE Egaleo</t>
+        </is>
+      </c>
+      <c r="I127" t="n">
         <v>1</v>
       </c>
-      <c r="H127" t="inlineStr">
-        <is>
-          <t>Kozani FC</t>
-        </is>
-      </c>
-      <c r="I127" t="n">
-        <v>0</v>
-      </c>
       <c r="J127" t="n">
-        <v>2.66</v>
+        <v>1.6</v>
       </c>
       <c r="K127" t="inlineStr">
         <is>
@@ -12096,15 +12096,15 @@
         </is>
       </c>
       <c r="L127" t="n">
-        <v>2.21</v>
+        <v>1.54</v>
       </c>
       <c r="M127" t="inlineStr">
         <is>
-          <t>13/12/2023 13:54</t>
+          <t>13/12/2023 13:59</t>
         </is>
       </c>
       <c r="N127" t="n">
-        <v>2.69</v>
+        <v>3.43</v>
       </c>
       <c r="O127" t="inlineStr">
         <is>
@@ -12112,15 +12112,15 @@
         </is>
       </c>
       <c r="P127" t="n">
-        <v>2.59</v>
+        <v>3.8</v>
       </c>
       <c r="Q127" t="inlineStr">
         <is>
-          <t>13/12/2023 13:54</t>
+          <t>13/12/2023 13:59</t>
         </is>
       </c>
       <c r="R127" t="n">
-        <v>2.79</v>
+        <v>5.27</v>
       </c>
       <c r="S127" t="inlineStr">
         <is>
@@ -12128,16 +12128,16 @@
         </is>
       </c>
       <c r="T127" t="n">
-        <v>4.29</v>
+        <v>5.17</v>
       </c>
       <c r="U127" t="inlineStr">
         <is>
-          <t>13/12/2023 13:54</t>
+          <t>13/12/2023 13:59</t>
         </is>
       </c>
       <c r="V127" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/aek-kozani-fc/U9HrhhYI/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/ionikos-pae-egaleo/QNmnqPPE/</t>
         </is>
       </c>
     </row>
@@ -13177,22 +13177,22 @@
       </c>
       <c r="F139" t="inlineStr">
         <is>
-          <t>Kozani FC</t>
+          <t>Karditsa</t>
         </is>
       </c>
       <c r="G139" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H139" t="inlineStr">
         <is>
-          <t>Levadiakos</t>
+          <t>Iraklis 1908</t>
         </is>
       </c>
       <c r="I139" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J139" t="n">
-        <v>5.26</v>
+        <v>2.86</v>
       </c>
       <c r="K139" t="inlineStr">
         <is>
@@ -13200,15 +13200,15 @@
         </is>
       </c>
       <c r="L139" t="n">
-        <v>5.66</v>
+        <v>3.39</v>
       </c>
       <c r="M139" t="inlineStr">
         <is>
-          <t>03/01/2024 13:03</t>
+          <t>03/01/2024 13:59</t>
         </is>
       </c>
       <c r="N139" t="n">
-        <v>3.18</v>
+        <v>2.7</v>
       </c>
       <c r="O139" t="inlineStr">
         <is>
@@ -13216,15 +13216,15 @@
         </is>
       </c>
       <c r="P139" t="n">
-        <v>3.17</v>
+        <v>2.42</v>
       </c>
       <c r="Q139" t="inlineStr">
         <is>
-          <t>03/01/2024 12:54</t>
+          <t>03/01/2024 13:58</t>
         </is>
       </c>
       <c r="R139" t="n">
-        <v>1.66</v>
+        <v>2.6</v>
       </c>
       <c r="S139" t="inlineStr">
         <is>
@@ -13232,16 +13232,16 @@
         </is>
       </c>
       <c r="T139" t="n">
-        <v>1.73</v>
+        <v>2.75</v>
       </c>
       <c r="U139" t="inlineStr">
         <is>
-          <t>03/01/2024 13:03</t>
+          <t>03/01/2024 13:58</t>
         </is>
       </c>
       <c r="V139" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/kozani-fc-levadiakos/A1E7Da0d/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/karditsa-iraklis-fc/Gb1gy3h3/</t>
         </is>
       </c>
     </row>
@@ -13269,22 +13269,22 @@
       </c>
       <c r="F140" t="inlineStr">
         <is>
-          <t>Karditsa</t>
+          <t>Kozani FC</t>
         </is>
       </c>
       <c r="G140" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H140" t="inlineStr">
         <is>
-          <t>Iraklis 1908</t>
+          <t>Levadiakos</t>
         </is>
       </c>
       <c r="I140" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J140" t="n">
-        <v>2.86</v>
+        <v>5.26</v>
       </c>
       <c r="K140" t="inlineStr">
         <is>
@@ -13292,15 +13292,15 @@
         </is>
       </c>
       <c r="L140" t="n">
-        <v>3.39</v>
+        <v>5.66</v>
       </c>
       <c r="M140" t="inlineStr">
         <is>
-          <t>03/01/2024 13:59</t>
+          <t>03/01/2024 13:03</t>
         </is>
       </c>
       <c r="N140" t="n">
-        <v>2.7</v>
+        <v>3.18</v>
       </c>
       <c r="O140" t="inlineStr">
         <is>
@@ -13308,15 +13308,15 @@
         </is>
       </c>
       <c r="P140" t="n">
-        <v>2.42</v>
+        <v>3.17</v>
       </c>
       <c r="Q140" t="inlineStr">
         <is>
-          <t>03/01/2024 13:58</t>
+          <t>03/01/2024 12:54</t>
         </is>
       </c>
       <c r="R140" t="n">
-        <v>2.6</v>
+        <v>1.66</v>
       </c>
       <c r="S140" t="inlineStr">
         <is>
@@ -13324,16 +13324,16 @@
         </is>
       </c>
       <c r="T140" t="n">
-        <v>2.75</v>
+        <v>1.73</v>
       </c>
       <c r="U140" t="inlineStr">
         <is>
-          <t>03/01/2024 13:58</t>
+          <t>03/01/2024 13:03</t>
         </is>
       </c>
       <c r="V140" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/greece/super-league-2/karditsa-iraklis-fc/Gb1gy3h3/</t>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/kozani-fc-levadiakos/A1E7Da0d/</t>
         </is>
       </c>
     </row>
@@ -13426,6 +13426,190 @@
       <c r="V141" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/greece/super-league-2/makedonikos-neapolis-aiolikos-fc/x82kxqwc/</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="1" t="n">
+        <v>141</v>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>greece</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>super-league-2</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E142" s="2" t="n">
+        <v>45295.58333333334</v>
+      </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>Kampaniakos</t>
+        </is>
+      </c>
+      <c r="G142" t="n">
+        <v>2</v>
+      </c>
+      <c r="H142" t="inlineStr">
+        <is>
+          <t>PAOK B</t>
+        </is>
+      </c>
+      <c r="I142" t="n">
+        <v>0</v>
+      </c>
+      <c r="J142" t="n">
+        <v>2.81</v>
+      </c>
+      <c r="K142" t="inlineStr">
+        <is>
+          <t>03/01/2024 02:12</t>
+        </is>
+      </c>
+      <c r="L142" t="n">
+        <v>3.82</v>
+      </c>
+      <c r="M142" t="inlineStr">
+        <is>
+          <t>04/01/2024 13:56</t>
+        </is>
+      </c>
+      <c r="N142" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="O142" t="inlineStr">
+        <is>
+          <t>03/01/2024 02:12</t>
+        </is>
+      </c>
+      <c r="P142" t="n">
+        <v>3.07</v>
+      </c>
+      <c r="Q142" t="inlineStr">
+        <is>
+          <t>04/01/2024 13:56</t>
+        </is>
+      </c>
+      <c r="R142" t="n">
+        <v>2.47</v>
+      </c>
+      <c r="S142" t="inlineStr">
+        <is>
+          <t>03/01/2024 02:12</t>
+        </is>
+      </c>
+      <c r="T142" t="n">
+        <v>2.07</v>
+      </c>
+      <c r="U142" t="inlineStr">
+        <is>
+          <t>04/01/2024 13:56</t>
+        </is>
+      </c>
+      <c r="V142" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/kampaniakos-paok/CQf2ZtNF/</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="1" t="n">
+        <v>142</v>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>greece</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>super-league-2</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E143" s="2" t="n">
+        <v>45295.625</v>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>AEL Larissa</t>
+        </is>
+      </c>
+      <c r="G143" t="n">
+        <v>1</v>
+      </c>
+      <c r="H143" t="inlineStr">
+        <is>
+          <t>AEK Athens FC B</t>
+        </is>
+      </c>
+      <c r="I143" t="n">
+        <v>1</v>
+      </c>
+      <c r="J143" t="n">
+        <v>1.29</v>
+      </c>
+      <c r="K143" t="inlineStr">
+        <is>
+          <t>03/01/2024 03:12</t>
+        </is>
+      </c>
+      <c r="L143" t="n">
+        <v>1.59</v>
+      </c>
+      <c r="M143" t="inlineStr">
+        <is>
+          <t>04/01/2024 14:59</t>
+        </is>
+      </c>
+      <c r="N143" t="n">
+        <v>4.43</v>
+      </c>
+      <c r="O143" t="inlineStr">
+        <is>
+          <t>03/01/2024 03:12</t>
+        </is>
+      </c>
+      <c r="P143" t="n">
+        <v>3.47</v>
+      </c>
+      <c r="Q143" t="inlineStr">
+        <is>
+          <t>04/01/2024 14:59</t>
+        </is>
+      </c>
+      <c r="R143" t="n">
+        <v>9.68</v>
+      </c>
+      <c r="S143" t="inlineStr">
+        <is>
+          <t>03/01/2024 03:12</t>
+        </is>
+      </c>
+      <c r="T143" t="n">
+        <v>6.55</v>
+      </c>
+      <c r="U143" t="inlineStr">
+        <is>
+          <t>04/01/2024 14:59</t>
+        </is>
+      </c>
+      <c r="V143" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/greece/super-league-2/ael-larissa-aek/bNjbzN79/</t>
         </is>
       </c>
     </row>

</xml_diff>